<commit_message>
Add router_id parameter for ipv6 vsc support
</commit_message>
<xml_diff>
--- a/examples/excel/active_standby_vsds.xlsx
+++ b/examples/excel/active_standby_vsds.xlsx
@@ -2638,6 +2638,7 @@
     <author>ctrl_ip_vprn</author>
     <author>ctrl_ip_vprn_list</author>
     <author>system_ip</author>
+    <author>router_id</author>
     <author>vmname</author>
     <author>system_name</author>
     <author>xmpp_username</author>
@@ -2742,225 +2743,230 @@
     </comment>
     <comment authorId="11" ref="A18" shapeId="0">
       <text>
+        <t>Required IPv4 address when using an IPv6 system IP address [default: (system_ip)]</t>
+      </text>
+    </comment>
+    <comment authorId="12" ref="A19" shapeId="0">
+      <text>
         <t>Name of the virtual machine on the Hypervisor/vCenter Server. [default: (Hostname)]</t>
       </text>
     </comment>
-    <comment authorId="12" ref="A19" shapeId="0">
+    <comment authorId="13" ref="A20" shapeId="0">
       <text>
         <t>Name of the system if other than hostname [default: (Hostname)]</t>
       </text>
     </comment>
-    <comment authorId="13" ref="A20" shapeId="0">
+    <comment authorId="14" ref="A21" shapeId="0">
       <text>
         <t>Unique username used to identify this VSC in its XMPP connection with VSD [default: vsc1]</t>
       </text>
     </comment>
-    <comment authorId="14" ref="A22" shapeId="0">
+    <comment authorId="15" ref="A23" shapeId="0">
       <text>
         <t>Type of hypervisor environment where VMs will be instantiated. Use 'none' when skipping predeploy.</t>
       </text>
     </comment>
-    <comment authorId="15" ref="A23" shapeId="0">
+    <comment authorId="16" ref="A24" shapeId="0">
       <text>
         <t>Hostname or IP address of the hypervisor where VM  will be instantiated. In the case of deployment in a vCenter environment, this will be the FQDN of the vCenter Server</t>
       </text>
     </comment>
-    <comment authorId="16" ref="A25" shapeId="0">
+    <comment authorId="17" ref="A26" shapeId="0">
       <text>
         <t>Network Bridge used for the management interface of a component or the BOF interface on VSC. This will be a Distributed Virtual PortGroup (DVPG) when deploying on vCenter or a Linux network bridge when deploying on KVM. This field can be overridden by defining the management network bridge separately in the component configuration. Defaults to the global setting [default: (global Bridge interface)]</t>
       </text>
     </comment>
-    <comment authorId="17" ref="A26" shapeId="0">
+    <comment authorId="18" ref="A27" shapeId="0">
       <text>
         <t>Network Bridge used for the data path of a component or the Control interface on VSC. This will be a Distributed Virtual PortGroup (DVPG) when deploying on vCenter or a Linux network bridge when deploying on KVM. [default: (global Bridge interface)]</t>
       </text>
     </comment>
-    <comment authorId="18" ref="A27" shapeId="0">
+    <comment authorId="19" ref="A28" shapeId="0">
       <text>
         <t>FQDN of the VSD or VSD cluster for this VSC</t>
       </text>
     </comment>
-    <comment authorId="19" ref="A28" shapeId="0">
+    <comment authorId="20" ref="A29" shapeId="0">
       <text>
         <t>Private Management IP Address of VSC instances</t>
       </text>
     </comment>
-    <comment authorId="20" ref="A29" shapeId="0">
+    <comment authorId="21" ref="A30" shapeId="0">
       <text>
         <t>Private Control IP Address of VSC Instances</t>
       </text>
     </comment>
-    <comment authorId="21" ref="A30" shapeId="0">
+    <comment authorId="22" ref="A31" shapeId="0">
       <text>
         <t>Private Data Gateway IP Address of VSC Instances</t>
       </text>
     </comment>
-    <comment authorId="22" ref="A31" shapeId="0">
+    <comment authorId="23" ref="A32" shapeId="0">
       <text>
         <t>List of route reflector IP addresses if present (List items separated by comma.)</t>
       </text>
     </comment>
-    <comment authorId="23" ref="A33" shapeId="0">
+    <comment authorId="24" ref="A34" shapeId="0">
       <text>
         <t>Name of the vCenter Datacenter on which the VSC VM will be deployed. Defaults to the common vCenter Datacenter Name if not defined here. [default: (global vCenter Datacenter Name)]</t>
       </text>
     </comment>
-    <comment authorId="24" ref="A34" shapeId="0">
+    <comment authorId="25" ref="A35" shapeId="0">
       <text>
         <t>Name of the vCenter Cluster on which the VSC VM will be deployed. Defaults to the common vCenter Cluster Name if not defined here. [default: (global vCenter Cluster Name)]</t>
       </text>
     </comment>
-    <comment authorId="25" ref="A35" shapeId="0">
+    <comment authorId="26" ref="A36" shapeId="0">
       <text>
         <t>Requires ovftool 4.3. Reference to the host on the vCenter cluster on which to deploy Nuage components [default: (global vCenter Host Reference)]</t>
       </text>
     </comment>
-    <comment authorId="26" ref="A36" shapeId="0">
+    <comment authorId="27" ref="A37" shapeId="0">
       <text>
         <t>Name of the vCenter Datastore on which the VSC VM will be deployed. Defaults to the common vCenter Datastore Name if not defined here. [default: (global vCenter Datastore Name)]</t>
       </text>
     </comment>
-    <comment authorId="27" ref="A37" shapeId="0">
+    <comment authorId="28" ref="A38" shapeId="0">
       <text>
         <t>Optional path to a folder defined on vCenter where VM will be instantiated [default: (global vCenter VM folder)]</t>
       </text>
     </comment>
-    <comment authorId="28" ref="A38" shapeId="0">
+    <comment authorId="29" ref="A39" shapeId="0">
       <text>
         <t>Optional path to a hosts and clusters folder defined on vCenter where VM will be instantiated</t>
       </text>
     </comment>
-    <comment authorId="29" ref="A40" shapeId="0">
+    <comment authorId="30" ref="A41" shapeId="0">
       <text>
         <t>Name of image installed on OpenStack for VSC</t>
       </text>
     </comment>
-    <comment authorId="30" ref="A41" shapeId="0">
+    <comment authorId="31" ref="A42" shapeId="0">
       <text>
         <t>Name of instance flavor installed on OpenStack for VSC</t>
       </text>
     </comment>
-    <comment authorId="31" ref="A42" shapeId="0">
+    <comment authorId="32" ref="A43" shapeId="0">
       <text>
         <t>Name of availability zone on OpenStack for VSC</t>
       </text>
     </comment>
-    <comment authorId="32" ref="A43" shapeId="0">
+    <comment authorId="33" ref="A44" shapeId="0">
       <text>
         <t>Name of management network on OpenStack for VSC</t>
       </text>
     </comment>
-    <comment authorId="33" ref="A44" shapeId="0">
+    <comment authorId="34" ref="A45" shapeId="0">
       <text>
         <t>Name of management subnet on OpenStack for VSC</t>
       </text>
     </comment>
-    <comment authorId="34" ref="A45" shapeId="0">
+    <comment authorId="35" ref="A46" shapeId="0">
       <text>
         <t>Name for Mgmt interface</t>
       </text>
     </comment>
-    <comment authorId="35" ref="A46" shapeId="0">
+    <comment authorId="36" ref="A47" shapeId="0">
       <text>
         <t>Set of security groups to associate with Mgmt interface (List items separated by comma.)</t>
       </text>
     </comment>
-    <comment authorId="36" ref="A47" shapeId="0">
+    <comment authorId="37" ref="A48" shapeId="0">
       <text>
         <t>Name of control network on OpenStack for VSC</t>
       </text>
     </comment>
-    <comment authorId="37" ref="A48" shapeId="0">
+    <comment authorId="38" ref="A49" shapeId="0">
       <text>
         <t>Name of control subnet on OpenStack for VSC</t>
       </text>
     </comment>
-    <comment authorId="38" ref="A49" shapeId="0">
+    <comment authorId="39" ref="A50" shapeId="0">
       <text>
         <t>Name for Control interface</t>
       </text>
     </comment>
-    <comment authorId="39" ref="A50" shapeId="0">
+    <comment authorId="40" ref="A51" shapeId="0">
       <text>
         <t>Set of security groups to associate with Control interface (List items separated by comma.)</t>
       </text>
     </comment>
-    <comment authorId="40" ref="A51" shapeId="0">
+    <comment authorId="41" ref="A52" shapeId="0">
       <text>
         <t>Name for Mgmt interface</t>
       </text>
     </comment>
-    <comment authorId="41" ref="A52" shapeId="0">
+    <comment authorId="42" ref="A53" shapeId="0">
       <text>
         <t>Set of security groups to associate with Mgmt interface (List items separated by comma.)</t>
       </text>
     </comment>
-    <comment authorId="42" ref="A54" shapeId="0">
+    <comment authorId="43" ref="A55" shapeId="0">
       <text>
         <t>Used in postdeploy and health workflows as expected values if non-zero [default: 0]</t>
       </text>
     </comment>
-    <comment authorId="43" ref="A55" shapeId="0">
+    <comment authorId="44" ref="A56" shapeId="0">
       <text>
         <t>Used in postdeploy and health workflows as expected values if non-zero [default: 0]</t>
       </text>
     </comment>
-    <comment authorId="44" ref="A56" shapeId="0">
+    <comment authorId="45" ref="A57" shapeId="0">
       <text>
         <t>Used in postdeploy and health workflows as expected values if non-zero [default: 0]</t>
       </text>
     </comment>
-    <comment authorId="45" ref="A57" shapeId="0">
+    <comment authorId="46" ref="A58" shapeId="0">
       <text>
         <t>Used in postdeploy and health workflows as expected values if non-zero [default: 0]</t>
       </text>
     </comment>
-    <comment authorId="46" ref="A58" shapeId="0">
+    <comment authorId="47" ref="A59" shapeId="0">
       <text>
         <t>Used in postdeploy and health workflows as expected values if non-zero [default: 0]</t>
       </text>
     </comment>
-    <comment authorId="47" ref="A60" shapeId="0">
+    <comment authorId="48" ref="A61" shapeId="0">
       <text>
         <t>Ejabberd user id used to create the certificate</t>
       </text>
     </comment>
-    <comment authorId="48" ref="A61" shapeId="0">
+    <comment authorId="49" ref="A62" shapeId="0">
       <text>
         <t>Path to VSC certificate key pem file</t>
       </text>
     </comment>
-    <comment authorId="49" ref="A62" shapeId="0">
+    <comment authorId="50" ref="A63" shapeId="0">
       <text>
         <t>Path to VSC certificate pem file</t>
       </text>
     </comment>
-    <comment authorId="50" ref="A63" shapeId="0">
+    <comment authorId="51" ref="A64" shapeId="0">
       <text>
         <t>Path to CA certificate pem file</t>
       </text>
     </comment>
-    <comment authorId="51" ref="A64" shapeId="0">
+    <comment authorId="52" ref="A65" shapeId="0">
       <text>
         <t>XMPP domain used in custom certificates</t>
       </text>
     </comment>
-    <comment authorId="52" ref="A65" shapeId="0">
+    <comment authorId="53" ref="A66" shapeId="0">
       <text>
         <t>Name of the credentials set for the vsc</t>
       </text>
     </comment>
-    <comment authorId="53" ref="A67" shapeId="0">
+    <comment authorId="54" ref="A68" shapeId="0">
       <text>
         <t>Cpuset information for cpu pinning on KVM. For example, VSC requires 4 cores and sample values will be of the form [ 0, 1, 2, 3 ] (List items separated by comma.)</t>
       </text>
     </comment>
-    <comment authorId="54" ref="A68" shapeId="0">
+    <comment authorId="55" ref="A69" shapeId="0">
       <text>
         <t>Enables hardening configuration on VSC [default: True]</t>
       </text>
     </comment>
-    <comment authorId="55" ref="A69" shapeId="0">
+    <comment authorId="56" ref="A70" shapeId="0">
       <text>
         <t>Paths to files that can be optionally applied for additional VSC configuration (List items separated by comma.)</t>
       </text>
@@ -10669,7 +10675,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C69"/>
+  <dimension ref="A1:C70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10819,75 +10825,75 @@
     <row r="18">
       <c r="A18" s="6" t="inlineStr">
         <is>
-          <t>VM name</t>
+          <t>Router ID</t>
         </is>
       </c>
       <c r="B18" s="7" t="n"/>
       <c r="C18" s="7" t="n"/>
     </row>
     <row r="19">
-      <c r="A19" s="8" t="inlineStr">
+      <c r="A19" s="6" t="inlineStr">
+        <is>
+          <t>VM name</t>
+        </is>
+      </c>
+      <c r="B19" s="7" t="n"/>
+      <c r="C19" s="7" t="n"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="8" t="inlineStr">
         <is>
           <t>System Name</t>
         </is>
       </c>
-      <c r="B19" s="9" t="n"/>
-      <c r="C19" s="9" t="n"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="6" t="inlineStr">
+      <c r="B20" s="9" t="n"/>
+      <c r="C20" s="9" t="n"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="6" t="inlineStr">
         <is>
           <t>XMPP username</t>
         </is>
       </c>
-      <c r="B20" s="7" t="n"/>
-      <c r="C20" s="7" t="n"/>
-    </row>
-    <row r="21">
-      <c r="A21" s="3" t="inlineStr">
+      <c r="B21" s="7" t="n"/>
+      <c r="C21" s="7" t="n"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="3" t="inlineStr">
         <is>
           <t>Target Server</t>
         </is>
       </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="4" t="inlineStr">
-        <is>
-          <t>Target Server type</t>
-        </is>
-      </c>
-      <c r="B22" s="5" t="n"/>
-      <c r="C22" s="5" t="n"/>
     </row>
     <row r="23">
       <c r="A23" s="4" t="inlineStr">
         <is>
-          <t>Target Server IP or FQDN</t>
+          <t>Target Server type</t>
         </is>
       </c>
       <c r="B23" s="5" t="n"/>
       <c r="C23" s="5" t="n"/>
     </row>
     <row r="24">
-      <c r="A24" s="3" t="inlineStr">
+      <c r="A24" s="4" t="inlineStr">
+        <is>
+          <t>Target Server IP or FQDN</t>
+        </is>
+      </c>
+      <c r="B24" s="5" t="n"/>
+      <c r="C24" s="5" t="n"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="3" t="inlineStr">
         <is>
           <t>Bridges and Private IP</t>
         </is>
       </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="8" t="inlineStr">
-        <is>
-          <t>Management Network Bridge</t>
-        </is>
-      </c>
-      <c r="B25" s="9" t="n"/>
-      <c r="C25" s="9" t="n"/>
     </row>
     <row r="26">
       <c r="A26" s="8" t="inlineStr">
         <is>
-          <t>Data Network Bridge</t>
+          <t>Management Network Bridge</t>
         </is>
       </c>
       <c r="B26" s="9" t="n"/>
@@ -10896,7 +10902,7 @@
     <row r="27">
       <c r="A27" s="8" t="inlineStr">
         <is>
-          <t>VSD FQDN</t>
+          <t>Data Network Bridge</t>
         </is>
       </c>
       <c r="B27" s="9" t="n"/>
@@ -10905,7 +10911,7 @@
     <row r="28">
       <c r="A28" s="8" t="inlineStr">
         <is>
-          <t>Private Management IP</t>
+          <t>VSD FQDN</t>
         </is>
       </c>
       <c r="B28" s="9" t="n"/>
@@ -10914,7 +10920,7 @@
     <row r="29">
       <c r="A29" s="8" t="inlineStr">
         <is>
-          <t>Private Control IP Address</t>
+          <t>Private Management IP</t>
         </is>
       </c>
       <c r="B29" s="9" t="n"/>
@@ -10923,7 +10929,7 @@
     <row r="30">
       <c r="A30" s="8" t="inlineStr">
         <is>
-          <t>Private Data Gateway IP Address</t>
+          <t>Private Control IP Address</t>
         </is>
       </c>
       <c r="B30" s="9" t="n"/>
@@ -10932,32 +10938,32 @@
     <row r="31">
       <c r="A31" s="8" t="inlineStr">
         <is>
-          <t>List of route reflector IPs</t>
+          <t>Private Data Gateway IP Address</t>
         </is>
       </c>
       <c r="B31" s="9" t="n"/>
       <c r="C31" s="9" t="n"/>
     </row>
     <row r="32">
-      <c r="A32" s="3" t="inlineStr">
+      <c r="A32" s="8" t="inlineStr">
+        <is>
+          <t>List of route reflector IPs</t>
+        </is>
+      </c>
+      <c r="B32" s="9" t="n"/>
+      <c r="C32" s="9" t="n"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="3" t="inlineStr">
         <is>
           <t>vCenter Parameters</t>
         </is>
       </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="8" t="inlineStr">
-        <is>
-          <t>vCenter Datacenter Name</t>
-        </is>
-      </c>
-      <c r="B33" s="9" t="n"/>
-      <c r="C33" s="9" t="n"/>
     </row>
     <row r="34">
       <c r="A34" s="8" t="inlineStr">
         <is>
-          <t>vCenter Cluster Name</t>
+          <t>vCenter Datacenter Name</t>
         </is>
       </c>
       <c r="B34" s="9" t="n"/>
@@ -10966,7 +10972,7 @@
     <row r="35">
       <c r="A35" s="8" t="inlineStr">
         <is>
-          <t>vCenter Host Reference</t>
+          <t>vCenter Cluster Name</t>
         </is>
       </c>
       <c r="B35" s="9" t="n"/>
@@ -10975,50 +10981,50 @@
     <row r="36">
       <c r="A36" s="8" t="inlineStr">
         <is>
-          <t>vCenter Datastore Name</t>
+          <t>vCenter Host Reference</t>
         </is>
       </c>
       <c r="B36" s="9" t="n"/>
       <c r="C36" s="9" t="n"/>
     </row>
     <row r="37">
-      <c r="A37" s="6" t="inlineStr">
+      <c r="A37" s="8" t="inlineStr">
+        <is>
+          <t>vCenter Datastore Name</t>
+        </is>
+      </c>
+      <c r="B37" s="9" t="n"/>
+      <c r="C37" s="9" t="n"/>
+    </row>
+    <row r="38">
+      <c r="A38" s="6" t="inlineStr">
         <is>
           <t>vCenter VM Folder</t>
         </is>
       </c>
-      <c r="B37" s="7" t="n"/>
-      <c r="C37" s="7" t="n"/>
-    </row>
-    <row r="38">
-      <c r="A38" s="8" t="inlineStr">
+      <c r="B38" s="7" t="n"/>
+      <c r="C38" s="7" t="n"/>
+    </row>
+    <row r="39">
+      <c r="A39" s="8" t="inlineStr">
         <is>
           <t>vCenter Hosts and Clusters Folder</t>
         </is>
       </c>
-      <c r="B38" s="9" t="n"/>
-      <c r="C38" s="9" t="n"/>
-    </row>
-    <row r="39">
-      <c r="A39" s="3" t="inlineStr">
+      <c r="B39" s="9" t="n"/>
+      <c r="C39" s="9" t="n"/>
+    </row>
+    <row r="40">
+      <c r="A40" s="3" t="inlineStr">
         <is>
           <t>OpenStack Parameters</t>
         </is>
       </c>
-    </row>
-    <row r="40">
-      <c r="A40" s="6" t="inlineStr">
-        <is>
-          <t>OpenStack Image</t>
-        </is>
-      </c>
-      <c r="B40" s="7" t="n"/>
-      <c r="C40" s="7" t="n"/>
     </row>
     <row r="41">
       <c r="A41" s="6" t="inlineStr">
         <is>
-          <t>OpenStack Flavor</t>
+          <t>OpenStack Image</t>
         </is>
       </c>
       <c r="B41" s="7" t="n"/>
@@ -11027,7 +11033,7 @@
     <row r="42">
       <c r="A42" s="6" t="inlineStr">
         <is>
-          <t>OpenStack Availability Zone</t>
+          <t>OpenStack Flavor</t>
         </is>
       </c>
       <c r="B42" s="7" t="n"/>
@@ -11036,7 +11042,7 @@
     <row r="43">
       <c r="A43" s="6" t="inlineStr">
         <is>
-          <t>OpenStack Mgmt Network</t>
+          <t>OpenStack Availability Zone</t>
         </is>
       </c>
       <c r="B43" s="7" t="n"/>
@@ -11045,7 +11051,7 @@
     <row r="44">
       <c r="A44" s="6" t="inlineStr">
         <is>
-          <t>OpenStack Mgmt Subnet</t>
+          <t>OpenStack Mgmt Network</t>
         </is>
       </c>
       <c r="B44" s="7" t="n"/>
@@ -11054,7 +11060,7 @@
     <row r="45">
       <c r="A45" s="6" t="inlineStr">
         <is>
-          <t>OpenStack Mgmt Port Name</t>
+          <t>OpenStack Mgmt Subnet</t>
         </is>
       </c>
       <c r="B45" s="7" t="n"/>
@@ -11063,7 +11069,7 @@
     <row r="46">
       <c r="A46" s="6" t="inlineStr">
         <is>
-          <t>OpenStack Mgmt Port Security Groups</t>
+          <t>OpenStack Mgmt Port Name</t>
         </is>
       </c>
       <c r="B46" s="7" t="n"/>
@@ -11072,7 +11078,7 @@
     <row r="47">
       <c r="A47" s="6" t="inlineStr">
         <is>
-          <t>OpenStack Control Network</t>
+          <t>OpenStack Mgmt Port Security Groups</t>
         </is>
       </c>
       <c r="B47" s="7" t="n"/>
@@ -11081,7 +11087,7 @@
     <row r="48">
       <c r="A48" s="6" t="inlineStr">
         <is>
-          <t>OpenStack Control Subnet</t>
+          <t>OpenStack Control Network</t>
         </is>
       </c>
       <c r="B48" s="7" t="n"/>
@@ -11090,7 +11096,7 @@
     <row r="49">
       <c r="A49" s="6" t="inlineStr">
         <is>
-          <t>OpenStack Control Port Name</t>
+          <t>OpenStack Control Subnet</t>
         </is>
       </c>
       <c r="B49" s="7" t="n"/>
@@ -11099,7 +11105,7 @@
     <row r="50">
       <c r="A50" s="6" t="inlineStr">
         <is>
-          <t>OpenStack Control Port Security Groups</t>
+          <t>OpenStack Control Port Name</t>
         </is>
       </c>
       <c r="B50" s="7" t="n"/>
@@ -11108,7 +11114,7 @@
     <row r="51">
       <c r="A51" s="6" t="inlineStr">
         <is>
-          <t>OpenStack Port Name</t>
+          <t>OpenStack Control Port Security Groups</t>
         </is>
       </c>
       <c r="B51" s="7" t="n"/>
@@ -11117,32 +11123,32 @@
     <row r="52">
       <c r="A52" s="6" t="inlineStr">
         <is>
-          <t>OpenStack Port Security Groups</t>
+          <t>OpenStack Port Name</t>
         </is>
       </c>
       <c r="B52" s="7" t="n"/>
       <c r="C52" s="7" t="n"/>
     </row>
     <row r="53">
-      <c r="A53" s="3" t="inlineStr">
+      <c r="A53" s="6" t="inlineStr">
+        <is>
+          <t>OpenStack Port Security Groups</t>
+        </is>
+      </c>
+      <c r="B53" s="7" t="n"/>
+      <c r="C53" s="7" t="n"/>
+    </row>
+    <row r="54">
+      <c r="A54" s="3" t="inlineStr">
         <is>
           <t>Health Parameters</t>
         </is>
       </c>
-    </row>
-    <row r="54">
-      <c r="A54" s="8" t="inlineStr">
-        <is>
-          <t>Expected number of BGP neighbors</t>
-        </is>
-      </c>
-      <c r="B54" s="9" t="n"/>
-      <c r="C54" s="9" t="n"/>
     </row>
     <row r="55">
       <c r="A55" s="8" t="inlineStr">
         <is>
-          <t>Expected number of vswitches</t>
+          <t>Expected number of BGP neighbors</t>
         </is>
       </c>
       <c r="B55" s="9" t="n"/>
@@ -11151,7 +11157,7 @@
     <row r="56">
       <c r="A56" s="8" t="inlineStr">
         <is>
-          <t>Expected number of host vports</t>
+          <t>Expected number of vswitches</t>
         </is>
       </c>
       <c r="B56" s="9" t="n"/>
@@ -11160,7 +11166,7 @@
     <row r="57">
       <c r="A57" s="8" t="inlineStr">
         <is>
-          <t>Expected number of VM vports</t>
+          <t>Expected number of host vports</t>
         </is>
       </c>
       <c r="B57" s="9" t="n"/>
@@ -11169,32 +11175,32 @@
     <row r="58">
       <c r="A58" s="8" t="inlineStr">
         <is>
-          <t>Expected number of gateway ports</t>
+          <t>Expected number of VM vports</t>
         </is>
       </c>
       <c r="B58" s="9" t="n"/>
       <c r="C58" s="9" t="n"/>
     </row>
     <row r="59">
-      <c r="A59" s="3" t="inlineStr">
+      <c r="A59" s="8" t="inlineStr">
+        <is>
+          <t>Expected number of gateway ports</t>
+        </is>
+      </c>
+      <c r="B59" s="9" t="n"/>
+      <c r="C59" s="9" t="n"/>
+    </row>
+    <row r="60">
+      <c r="A60" s="3" t="inlineStr">
         <is>
           <t>Certificates and credentials</t>
         </is>
       </c>
-    </row>
-    <row r="60">
-      <c r="A60" s="8" t="inlineStr">
-        <is>
-          <t>Ejabberd user id</t>
-        </is>
-      </c>
-      <c r="B60" s="9" t="n"/>
-      <c r="C60" s="9" t="n"/>
     </row>
     <row r="61">
       <c r="A61" s="8" t="inlineStr">
         <is>
-          <t>Private key path</t>
+          <t>Ejabberd user id</t>
         </is>
       </c>
       <c r="B61" s="9" t="n"/>
@@ -11203,7 +11209,7 @@
     <row r="62">
       <c r="A62" s="8" t="inlineStr">
         <is>
-          <t>Certificate path</t>
+          <t>Private key path</t>
         </is>
       </c>
       <c r="B62" s="9" t="n"/>
@@ -11212,7 +11218,7 @@
     <row r="63">
       <c r="A63" s="8" t="inlineStr">
         <is>
-          <t>CA certificate path</t>
+          <t>Certificate path</t>
         </is>
       </c>
       <c r="B63" s="9" t="n"/>
@@ -11221,7 +11227,7 @@
     <row r="64">
       <c r="A64" s="8" t="inlineStr">
         <is>
-          <t>XMPP domain</t>
+          <t>CA certificate path</t>
         </is>
       </c>
       <c r="B64" s="9" t="n"/>
@@ -11230,32 +11236,32 @@
     <row r="65">
       <c r="A65" s="8" t="inlineStr">
         <is>
-          <t>Credentials set name</t>
+          <t>XMPP domain</t>
         </is>
       </c>
       <c r="B65" s="9" t="n"/>
       <c r="C65" s="9" t="n"/>
     </row>
     <row r="66">
-      <c r="A66" s="3" t="inlineStr">
+      <c r="A66" s="8" t="inlineStr">
+        <is>
+          <t>Credentials set name</t>
+        </is>
+      </c>
+      <c r="B66" s="9" t="n"/>
+      <c r="C66" s="9" t="n"/>
+    </row>
+    <row r="67">
+      <c r="A67" s="3" t="inlineStr">
         <is>
           <t>VSC Options</t>
         </is>
       </c>
-    </row>
-    <row r="67">
-      <c r="A67" s="8" t="inlineStr">
-        <is>
-          <t>KVM cpuset information</t>
-        </is>
-      </c>
-      <c r="B67" s="9" t="n"/>
-      <c r="C67" s="9" t="n"/>
     </row>
     <row r="68">
       <c r="A68" s="8" t="inlineStr">
         <is>
-          <t>Harden VSC</t>
+          <t>KVM cpuset information</t>
         </is>
       </c>
       <c r="B68" s="9" t="n"/>
@@ -11264,24 +11270,33 @@
     <row r="69">
       <c r="A69" s="8" t="inlineStr">
         <is>
-          <t>Paths to VSC Config Files</t>
+          <t>Harden VSC</t>
         </is>
       </c>
       <c r="B69" s="9" t="n"/>
       <c r="C69" s="9" t="n"/>
+    </row>
+    <row r="70">
+      <c r="A70" s="8" t="inlineStr">
+        <is>
+          <t>Paths to VSC Config Files</t>
+        </is>
+      </c>
+      <c r="B70" s="9" t="n"/>
+      <c r="C70" s="9" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="A10:C10"/>
     <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="A32:C32"/>
-    <mergeCell ref="A39:C39"/>
-    <mergeCell ref="A53:C53"/>
-    <mergeCell ref="A59:C59"/>
-    <mergeCell ref="A66:C66"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A33:C33"/>
+    <mergeCell ref="A40:C40"/>
+    <mergeCell ref="A54:C54"/>
+    <mergeCell ref="A60:C60"/>
+    <mergeCell ref="A67:C67"/>
   </mergeCells>
   <dataValidations count="20">
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B7" type="whole"/>
@@ -11290,14 +11305,12 @@
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="C12" type="whole"/>
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B13" type="whole"/>
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="C13" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="B22" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="B23" type="list">
       <formula1>"kvm,vcenter,openstack,nuagex,none"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="C22" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="C23" type="list">
       <formula1>"kvm,vcenter,openstack,nuagex,none"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B54" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="C54" type="whole"/>
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B55" type="whole"/>
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="C55" type="whole"/>
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B56" type="whole"/>
@@ -11306,10 +11319,12 @@
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="C57" type="whole"/>
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B58" type="whole"/>
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="C58" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="B68" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B59" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="C59" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="B69" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="C68" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="C69" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Remove custom vsd ipv6 script for vcenter
</commit_message>
<xml_diff>
--- a/examples/excel/active_standby_vsds.xlsx
+++ b/examples/excel/active_standby_vsds.xlsx
@@ -2387,7 +2387,6 @@
     <author>vcenter_datastore</author>
     <author>vcenter_vmfolder</author>
     <author>vcenter_host_clusters_folder</author>
-    <author>ipv6_script</author>
     <author>aws_region</author>
     <author>aws_ami_id</author>
     <author>aws_upgrade_ami_id</author>
@@ -2490,132 +2489,127 @@
         <t>Optional path to a hosts and clusters folder defined on vCenter where VM will be instantiated</t>
       </text>
     </comment>
-    <comment authorId="15" ref="A22" shapeId="0">
-      <text>
-        <t>Path to the script on the VSD to configure ipv6</t>
+    <comment authorId="15" ref="A23" shapeId="0">
+      <text>
+        <t>Only applicable for AWS deployments</t>
       </text>
     </comment>
     <comment authorId="16" ref="A24" shapeId="0">
       <text>
-        <t>Only applicable for AWS deployments</t>
+        <t>AMI ID for AWS instance</t>
       </text>
     </comment>
     <comment authorId="17" ref="A25" shapeId="0">
       <text>
-        <t>AMI ID for AWS instance</t>
+        <t>AMI VSD ID of the latest VSD release. Used only during an upgrade</t>
       </text>
     </comment>
     <comment authorId="18" ref="A26" shapeId="0">
       <text>
-        <t>AMI VSD ID of the latest VSD release. Used only during an upgrade</t>
+        <t>Instance Type to be used for a VSD instance</t>
       </text>
     </comment>
     <comment authorId="19" ref="A27" shapeId="0">
       <text>
-        <t>Instance Type to be used for a VSD instance</t>
+        <t>Name of the Keypair used to connect to AWS instances</t>
       </text>
     </comment>
     <comment authorId="20" ref="A28" shapeId="0">
       <text>
-        <t>Name of the Keypair used to connect to AWS instances</t>
-      </text>
-    </comment>
-    <comment authorId="21" ref="A29" shapeId="0">
-      <text>
         <t>ENI ID for VSD Instance on Management Subnet</t>
       </text>
     </comment>
+    <comment authorId="21" ref="A30" shapeId="0">
+      <text>
+        <t>Name of image installed on OpenStack for VSD</t>
+      </text>
+    </comment>
     <comment authorId="22" ref="A31" shapeId="0">
       <text>
-        <t>Name of image installed on OpenStack for VSD</t>
+        <t>Name of instance flavor installed on OpenStack for VSD</t>
       </text>
     </comment>
     <comment authorId="23" ref="A32" shapeId="0">
       <text>
-        <t>Name of instance flavor installed on OpenStack for VSD</t>
+        <t>Name of availability zone on OpenStack for VSD</t>
       </text>
     </comment>
     <comment authorId="24" ref="A33" shapeId="0">
       <text>
-        <t>Name of availability zone on OpenStack for VSD</t>
+        <t>Name of network on OpenStack for VSD</t>
       </text>
     </comment>
     <comment authorId="25" ref="A34" shapeId="0">
       <text>
-        <t>Name of network on OpenStack for VSD</t>
+        <t>Name of subnet on OpenStack for VSD</t>
       </text>
     </comment>
     <comment authorId="26" ref="A35" shapeId="0">
       <text>
-        <t>Name of subnet on OpenStack for VSD</t>
+        <t>Name for Mgmt interface</t>
       </text>
     </comment>
     <comment authorId="27" ref="A36" shapeId="0">
       <text>
-        <t>Name for Mgmt interface</t>
+        <t>Set of security groups to associate with Mgmt interface (List items separated by comma.)</t>
       </text>
     </comment>
     <comment authorId="28" ref="A37" shapeId="0">
       <text>
-        <t>Set of security groups to associate with Mgmt interface (List items separated by comma.)</t>
+        <t>Project name for OpenStack [default: ]</t>
       </text>
     </comment>
     <comment authorId="29" ref="A38" shapeId="0">
       <text>
-        <t>Project name for OpenStack [default: ]</t>
-      </text>
-    </comment>
-    <comment authorId="30" ref="A39" shapeId="0">
-      <text>
         <t>Keystone URL for OpenStack [default: ]</t>
       </text>
     </comment>
+    <comment authorId="30" ref="A40" shapeId="0">
+      <text>
+        <t>Cpuset information for cpu pinning on KVM. For example, VSD requires 6 cores and sample values will be of the form [ 0, 1, 2, 3, 4, 5 ] (List items separated by comma.)</t>
+      </text>
+    </comment>
     <comment authorId="31" ref="A41" shapeId="0">
       <text>
-        <t>Cpuset information for cpu pinning on KVM. For example, VSD requires 6 cores and sample values will be of the form [ 0, 1, 2, 3, 4, 5 ] (List items separated by comma.)</t>
+        <t>Lockout the user after reaching the number of failed login attempts</t>
       </text>
     </comment>
     <comment authorId="32" ref="A42" shapeId="0">
       <text>
-        <t>Lockout the user after reaching the number of failed login attempts</t>
+        <t>Lockout time after failed login attemps</t>
       </text>
     </comment>
     <comment authorId="33" ref="A43" shapeId="0">
       <text>
-        <t>Lockout time after failed login attemps</t>
+        <t>Enables advance API access logging</t>
       </text>
     </comment>
     <comment authorId="34" ref="A44" shapeId="0">
       <text>
-        <t>Enables advance API access logging</t>
-      </text>
-    </comment>
-    <comment authorId="35" ref="A45" shapeId="0">
-      <text>
         <t>Enables setup of a health monitoring agent [default: none]</t>
       </text>
     </comment>
+    <comment authorId="35" ref="A46" shapeId="0">
+      <text>
+        <t>TLS version to use</t>
+      </text>
+    </comment>
     <comment authorId="36" ref="A47" shapeId="0">
       <text>
-        <t>TLS version to use</t>
+        <t>Path to CA certificate pem file</t>
       </text>
     </comment>
     <comment authorId="37" ref="A48" shapeId="0">
       <text>
-        <t>Path to CA certificate pem file</t>
+        <t>Path to intermediate certificate pem file</t>
       </text>
     </comment>
     <comment authorId="38" ref="A49" shapeId="0">
       <text>
-        <t>Path to intermediate certificate pem file</t>
+        <t>Path to certificate pem file</t>
       </text>
     </comment>
     <comment authorId="39" ref="A50" shapeId="0">
-      <text>
-        <t>Path to certificate pem file</t>
-      </text>
-    </comment>
-    <comment authorId="40" ref="A51" shapeId="0">
       <text>
         <t>Name of the credentials set for the vsd</t>
       </text>
@@ -9811,7 +9805,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:G50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10191,29 +10185,29 @@
       <c r="G21" s="9" t="n"/>
     </row>
     <row r="22">
-      <c r="A22" s="8" t="inlineStr">
-        <is>
-          <t>VSD script to configure ipv6</t>
-        </is>
-      </c>
-      <c r="B22" s="9" t="n"/>
-      <c r="C22" s="9" t="n"/>
-      <c r="D22" s="9" t="n"/>
-      <c r="E22" s="9" t="n"/>
-      <c r="F22" s="9" t="n"/>
-      <c r="G22" s="9" t="n"/>
+      <c r="A22" s="3" t="inlineStr">
+        <is>
+          <t>AWS Parameters</t>
+        </is>
+      </c>
     </row>
     <row r="23">
-      <c r="A23" s="3" t="inlineStr">
-        <is>
-          <t>AWS Parameters</t>
-        </is>
-      </c>
+      <c r="A23" s="6" t="inlineStr">
+        <is>
+          <t>AWS Region</t>
+        </is>
+      </c>
+      <c r="B23" s="7" t="n"/>
+      <c r="C23" s="7" t="n"/>
+      <c r="D23" s="7" t="n"/>
+      <c r="E23" s="7" t="n"/>
+      <c r="F23" s="7" t="n"/>
+      <c r="G23" s="7" t="n"/>
     </row>
     <row r="24">
       <c r="A24" s="6" t="inlineStr">
         <is>
-          <t>AWS Region</t>
+          <t>AWS VSD AMI ID</t>
         </is>
       </c>
       <c r="B24" s="7" t="n"/>
@@ -10226,7 +10220,7 @@
     <row r="25">
       <c r="A25" s="6" t="inlineStr">
         <is>
-          <t>AWS VSD AMI ID</t>
+          <t>Upgrade AWS VSD AMI ID</t>
         </is>
       </c>
       <c r="B25" s="7" t="n"/>
@@ -10239,7 +10233,7 @@
     <row r="26">
       <c r="A26" s="6" t="inlineStr">
         <is>
-          <t>Upgrade AWS VSD AMI ID</t>
+          <t>AWS Instance Type</t>
         </is>
       </c>
       <c r="B26" s="7" t="n"/>
@@ -10252,7 +10246,7 @@
     <row r="27">
       <c r="A27" s="6" t="inlineStr">
         <is>
-          <t>AWS Instance Type</t>
+          <t>AWS Keypair Name</t>
         </is>
       </c>
       <c r="B27" s="7" t="n"/>
@@ -10265,7 +10259,7 @@
     <row r="28">
       <c r="A28" s="6" t="inlineStr">
         <is>
-          <t>AWS Keypair Name</t>
+          <t>AWS Management ENI ID</t>
         </is>
       </c>
       <c r="B28" s="7" t="n"/>
@@ -10276,29 +10270,29 @@
       <c r="G28" s="7" t="n"/>
     </row>
     <row r="29">
-      <c r="A29" s="6" t="inlineStr">
-        <is>
-          <t>AWS Management ENI ID</t>
-        </is>
-      </c>
-      <c r="B29" s="7" t="n"/>
-      <c r="C29" s="7" t="n"/>
-      <c r="D29" s="7" t="n"/>
-      <c r="E29" s="7" t="n"/>
-      <c r="F29" s="7" t="n"/>
-      <c r="G29" s="7" t="n"/>
+      <c r="A29" s="3" t="inlineStr">
+        <is>
+          <t>OpenStack Parameters</t>
+        </is>
+      </c>
     </row>
     <row r="30">
-      <c r="A30" s="3" t="inlineStr">
-        <is>
-          <t>OpenStack Parameters</t>
-        </is>
-      </c>
+      <c r="A30" s="6" t="inlineStr">
+        <is>
+          <t>OpenStack Image</t>
+        </is>
+      </c>
+      <c r="B30" s="7" t="n"/>
+      <c r="C30" s="7" t="n"/>
+      <c r="D30" s="7" t="n"/>
+      <c r="E30" s="7" t="n"/>
+      <c r="F30" s="7" t="n"/>
+      <c r="G30" s="7" t="n"/>
     </row>
     <row r="31">
       <c r="A31" s="6" t="inlineStr">
         <is>
-          <t>OpenStack Image</t>
+          <t>OpenStack Flavor</t>
         </is>
       </c>
       <c r="B31" s="7" t="n"/>
@@ -10311,7 +10305,7 @@
     <row r="32">
       <c r="A32" s="6" t="inlineStr">
         <is>
-          <t>OpenStack Flavor</t>
+          <t>OpenStack Availability Zone</t>
         </is>
       </c>
       <c r="B32" s="7" t="n"/>
@@ -10324,7 +10318,7 @@
     <row r="33">
       <c r="A33" s="6" t="inlineStr">
         <is>
-          <t>OpenStack Availability Zone</t>
+          <t>OpenStack Network</t>
         </is>
       </c>
       <c r="B33" s="7" t="n"/>
@@ -10337,7 +10331,7 @@
     <row r="34">
       <c r="A34" s="6" t="inlineStr">
         <is>
-          <t>OpenStack Network</t>
+          <t>OpenStack Subnet</t>
         </is>
       </c>
       <c r="B34" s="7" t="n"/>
@@ -10350,7 +10344,7 @@
     <row r="35">
       <c r="A35" s="6" t="inlineStr">
         <is>
-          <t>OpenStack Subnet</t>
+          <t>OpenStack Port Name</t>
         </is>
       </c>
       <c r="B35" s="7" t="n"/>
@@ -10363,7 +10357,7 @@
     <row r="36">
       <c r="A36" s="6" t="inlineStr">
         <is>
-          <t>OpenStack Port Name</t>
+          <t>OpenStack Port Security Groups</t>
         </is>
       </c>
       <c r="B36" s="7" t="n"/>
@@ -10376,7 +10370,7 @@
     <row r="37">
       <c r="A37" s="6" t="inlineStr">
         <is>
-          <t>OpenStack Port Security Groups</t>
+          <t>OpenStack Project Name</t>
         </is>
       </c>
       <c r="B37" s="7" t="n"/>
@@ -10389,7 +10383,7 @@
     <row r="38">
       <c r="A38" s="6" t="inlineStr">
         <is>
-          <t>OpenStack Project Name</t>
+          <t>OpenStack Keystone URL</t>
         </is>
       </c>
       <c r="B38" s="7" t="n"/>
@@ -10400,29 +10394,29 @@
       <c r="G38" s="7" t="n"/>
     </row>
     <row r="39">
-      <c r="A39" s="6" t="inlineStr">
-        <is>
-          <t>OpenStack Keystone URL</t>
-        </is>
-      </c>
-      <c r="B39" s="7" t="n"/>
-      <c r="C39" s="7" t="n"/>
-      <c r="D39" s="7" t="n"/>
-      <c r="E39" s="7" t="n"/>
-      <c r="F39" s="7" t="n"/>
-      <c r="G39" s="7" t="n"/>
+      <c r="A39" s="3" t="inlineStr">
+        <is>
+          <t>VSD Options</t>
+        </is>
+      </c>
     </row>
     <row r="40">
-      <c r="A40" s="3" t="inlineStr">
-        <is>
-          <t>VSD Options</t>
-        </is>
-      </c>
+      <c r="A40" s="8" t="inlineStr">
+        <is>
+          <t>KVM cpuset information</t>
+        </is>
+      </c>
+      <c r="B40" s="9" t="n"/>
+      <c r="C40" s="9" t="n"/>
+      <c r="D40" s="9" t="n"/>
+      <c r="E40" s="9" t="n"/>
+      <c r="F40" s="9" t="n"/>
+      <c r="G40" s="9" t="n"/>
     </row>
     <row r="41">
       <c r="A41" s="8" t="inlineStr">
         <is>
-          <t>KVM cpuset information</t>
+          <t>Failed login attempts</t>
         </is>
       </c>
       <c r="B41" s="9" t="n"/>
@@ -10435,7 +10429,7 @@
     <row r="42">
       <c r="A42" s="8" t="inlineStr">
         <is>
-          <t>Failed login attempts</t>
+          <t>Failed login lockout time</t>
         </is>
       </c>
       <c r="B42" s="9" t="n"/>
@@ -10448,7 +10442,7 @@
     <row r="43">
       <c r="A43" s="8" t="inlineStr">
         <is>
-          <t>Failed login lockout time</t>
+          <t>Advanced API Access Logging</t>
         </is>
       </c>
       <c r="B43" s="9" t="n"/>
@@ -10461,7 +10455,7 @@
     <row r="44">
       <c r="A44" s="8" t="inlineStr">
         <is>
-          <t>Advanced API Access Logging</t>
+          <t>Health monitoring agent</t>
         </is>
       </c>
       <c r="B44" s="9" t="n"/>
@@ -10472,29 +10466,29 @@
       <c r="G44" s="9" t="n"/>
     </row>
     <row r="45">
-      <c r="A45" s="8" t="inlineStr">
-        <is>
-          <t>Health monitoring agent</t>
-        </is>
-      </c>
-      <c r="B45" s="9" t="n"/>
-      <c r="C45" s="9" t="n"/>
-      <c r="D45" s="9" t="n"/>
-      <c r="E45" s="9" t="n"/>
-      <c r="F45" s="9" t="n"/>
-      <c r="G45" s="9" t="n"/>
+      <c r="A45" s="3" t="inlineStr">
+        <is>
+          <t>Security and Certificates</t>
+        </is>
+      </c>
     </row>
     <row r="46">
-      <c r="A46" s="3" t="inlineStr">
-        <is>
-          <t>Security and Certificates</t>
-        </is>
-      </c>
+      <c r="A46" s="8" t="inlineStr">
+        <is>
+          <t>TLS version</t>
+        </is>
+      </c>
+      <c r="B46" s="9" t="n"/>
+      <c r="C46" s="9" t="n"/>
+      <c r="D46" s="9" t="n"/>
+      <c r="E46" s="9" t="n"/>
+      <c r="F46" s="9" t="n"/>
+      <c r="G46" s="9" t="n"/>
     </row>
     <row r="47">
       <c r="A47" s="8" t="inlineStr">
         <is>
-          <t>TLS version</t>
+          <t>Path to CA certificate pem file</t>
         </is>
       </c>
       <c r="B47" s="9" t="n"/>
@@ -10507,7 +10501,7 @@
     <row r="48">
       <c r="A48" s="8" t="inlineStr">
         <is>
-          <t>Path to CA certificate pem file</t>
+          <t>Path to intermediate certificate pem file</t>
         </is>
       </c>
       <c r="B48" s="9" t="n"/>
@@ -10520,7 +10514,7 @@
     <row r="49">
       <c r="A49" s="8" t="inlineStr">
         <is>
-          <t>Path to intermediate certificate pem file</t>
+          <t>Path to certificate pem file</t>
         </is>
       </c>
       <c r="B49" s="9" t="n"/>
@@ -10533,7 +10527,7 @@
     <row r="50">
       <c r="A50" s="8" t="inlineStr">
         <is>
-          <t>Path to certificate pem file</t>
+          <t>Credentials set name</t>
         </is>
       </c>
       <c r="B50" s="9" t="n"/>
@@ -10543,28 +10537,15 @@
       <c r="F50" s="9" t="n"/>
       <c r="G50" s="9" t="n"/>
     </row>
-    <row r="51">
-      <c r="A51" s="8" t="inlineStr">
-        <is>
-          <t>Credentials set name</t>
-        </is>
-      </c>
-      <c r="B51" s="9" t="n"/>
-      <c r="C51" s="9" t="n"/>
-      <c r="D51" s="9" t="n"/>
-      <c r="E51" s="9" t="n"/>
-      <c r="F51" s="9" t="n"/>
-      <c r="G51" s="9" t="n"/>
-    </row>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="A4:G4"/>
     <mergeCell ref="A10:G10"/>
     <mergeCell ref="A15:G15"/>
-    <mergeCell ref="A23:G23"/>
-    <mergeCell ref="A30:G30"/>
-    <mergeCell ref="A40:G40"/>
-    <mergeCell ref="A46:G46"/>
+    <mergeCell ref="A22:G22"/>
+    <mergeCell ref="A29:G29"/>
+    <mergeCell ref="A39:G39"/>
+    <mergeCell ref="A45:G45"/>
   </mergeCells>
   <dataValidations count="42">
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B7" type="whole"/>
@@ -10591,70 +10572,70 @@
     <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="G13" type="list">
       <formula1>"kvm,vcenter,aws,openstack,nuagex,none"</formula1>
     </dataValidation>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B41" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="C41" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="D41" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="E41" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="F41" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="G41" type="whole"/>
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B42" type="whole"/>
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="C42" type="whole"/>
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="D42" type="whole"/>
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="E42" type="whole"/>
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="F42" type="whole"/>
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="G42" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B43" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="C43" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="D43" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="E43" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="F43" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="G43" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="B44" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="B43" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="C44" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="C43" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="D44" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="D43" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="E44" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="E43" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="F44" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="F43" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="G44" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="G43" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="B45" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="B44" type="list">
       <formula1>"none,zabbix"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="C45" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="C44" type="list">
       <formula1>"none,zabbix"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="D45" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="D44" type="list">
       <formula1>"none,zabbix"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="E45" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="E44" type="list">
       <formula1>"none,zabbix"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="F45" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="F44" type="list">
       <formula1>"none,zabbix"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="G45" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="G44" type="list">
       <formula1>"none,zabbix"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="B47" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="B46" type="list">
       <formula1>"1.0,1.2"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="C47" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="C46" type="list">
       <formula1>"1.0,1.2"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="D47" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="D46" type="list">
       <formula1>"1.0,1.2"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="E47" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="E46" type="list">
       <formula1>"1.0,1.2"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="F47" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="F46" type="list">
       <formula1>"1.0,1.2"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="G47" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="G46" type="list">
       <formula1>"1.0,1.2"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Update certificate procedure, refactor VSD version checking, verify api access logging happened
</commit_message>
<xml_diff>
--- a/examples/excel/active_standby_vsds.xlsx
+++ b/examples/excel/active_standby_vsds.xlsx
@@ -2591,7 +2591,7 @@
     </comment>
     <comment authorId="35" ref="A46" shapeId="0">
       <text>
-        <t>TLS version to use</t>
+        <t>Deprecated TLS version to use - always set to 1.2 starting in version 6.*</t>
       </text>
     </comment>
     <comment authorId="36" ref="A47" shapeId="0">
@@ -2632,6 +2632,7 @@
     <author>ctrl_ip_vprn</author>
     <author>ctrl_ip_vprn_list</author>
     <author>system_ip</author>
+    <author>router_id</author>
     <author>vmname</author>
     <author>system_name</author>
     <author>xmpp_username</author>
@@ -2736,225 +2737,230 @@
     </comment>
     <comment authorId="11" ref="A18" shapeId="0">
       <text>
+        <t>The router ID of this VSC in IPV4 address format. Required when system_ip is IPV6. [default: (System IP)]</t>
+      </text>
+    </comment>
+    <comment authorId="12" ref="A19" shapeId="0">
+      <text>
         <t>Name of the virtual machine on the Hypervisor/vCenter Server. [default: (Hostname)]</t>
       </text>
     </comment>
-    <comment authorId="12" ref="A19" shapeId="0">
+    <comment authorId="13" ref="A20" shapeId="0">
       <text>
         <t>Name of the system if other than hostname [default: (Hostname)]</t>
       </text>
     </comment>
-    <comment authorId="13" ref="A20" shapeId="0">
+    <comment authorId="14" ref="A21" shapeId="0">
       <text>
         <t>Unique username used to identify this VSC in its XMPP connection with VSD [default: vsc1]</t>
       </text>
     </comment>
-    <comment authorId="14" ref="A22" shapeId="0">
+    <comment authorId="15" ref="A23" shapeId="0">
       <text>
         <t>Type of hypervisor environment where VMs will be instantiated. Use 'none' when skipping predeploy.</t>
       </text>
     </comment>
-    <comment authorId="15" ref="A23" shapeId="0">
+    <comment authorId="16" ref="A24" shapeId="0">
       <text>
         <t>Hostname or IP address of the hypervisor where VM  will be instantiated. In the case of deployment in a vCenter environment, this will be the FQDN of the vCenter Server</t>
       </text>
     </comment>
-    <comment authorId="16" ref="A25" shapeId="0">
+    <comment authorId="17" ref="A26" shapeId="0">
       <text>
         <t>Network Bridge used for the management interface of a component or the BOF interface on VSC. This will be a Distributed Virtual PortGroup (DVPG) when deploying on vCenter or a Linux network bridge when deploying on KVM. This field can be overridden by defining the management network bridge separately in the component configuration. Defaults to the global setting [default: (global Bridge interface)]</t>
       </text>
     </comment>
-    <comment authorId="17" ref="A26" shapeId="0">
+    <comment authorId="18" ref="A27" shapeId="0">
       <text>
         <t>Network Bridge used for the data path of a component or the Control interface on VSC. This will be a Distributed Virtual PortGroup (DVPG) when deploying on vCenter or a Linux network bridge when deploying on KVM. [default: (global Bridge interface)]</t>
       </text>
     </comment>
-    <comment authorId="18" ref="A27" shapeId="0">
+    <comment authorId="19" ref="A28" shapeId="0">
       <text>
         <t>FQDN of the VSD or VSD cluster for this VSC</t>
       </text>
     </comment>
-    <comment authorId="19" ref="A28" shapeId="0">
+    <comment authorId="20" ref="A29" shapeId="0">
       <text>
         <t>Private Management IP Address of VSC instances</t>
       </text>
     </comment>
-    <comment authorId="20" ref="A29" shapeId="0">
+    <comment authorId="21" ref="A30" shapeId="0">
       <text>
         <t>Private Control IP Address of VSC Instances</t>
       </text>
     </comment>
-    <comment authorId="21" ref="A30" shapeId="0">
+    <comment authorId="22" ref="A31" shapeId="0">
       <text>
         <t>Private Data Gateway IP Address of VSC Instances</t>
       </text>
     </comment>
-    <comment authorId="22" ref="A31" shapeId="0">
+    <comment authorId="23" ref="A32" shapeId="0">
       <text>
         <t>List of route reflector IP addresses if present (List items separated by comma.)</t>
       </text>
     </comment>
-    <comment authorId="23" ref="A33" shapeId="0">
+    <comment authorId="24" ref="A34" shapeId="0">
       <text>
         <t>Name of the vCenter Datacenter on which the VSC VM will be deployed. Defaults to the common vCenter Datacenter Name if not defined here. [default: (global vCenter Datacenter Name)]</t>
       </text>
     </comment>
-    <comment authorId="24" ref="A34" shapeId="0">
+    <comment authorId="25" ref="A35" shapeId="0">
       <text>
         <t>Name of the vCenter Cluster on which the VSC VM will be deployed. Defaults to the common vCenter Cluster Name if not defined here. [default: (global vCenter Cluster Name)]</t>
       </text>
     </comment>
-    <comment authorId="25" ref="A35" shapeId="0">
+    <comment authorId="26" ref="A36" shapeId="0">
       <text>
         <t>Requires ovftool 4.3. Reference to the host on the vCenter cluster on which to deploy Nuage components [default: (global vCenter Host Reference)]</t>
       </text>
     </comment>
-    <comment authorId="26" ref="A36" shapeId="0">
+    <comment authorId="27" ref="A37" shapeId="0">
       <text>
         <t>Name of the vCenter Datastore on which the VSC VM will be deployed. Defaults to the common vCenter Datastore Name if not defined here. [default: (global vCenter Datastore Name)]</t>
       </text>
     </comment>
-    <comment authorId="27" ref="A37" shapeId="0">
+    <comment authorId="28" ref="A38" shapeId="0">
       <text>
         <t>Optional path to a folder defined on vCenter where VM will be instantiated [default: (global vCenter VM folder)]</t>
       </text>
     </comment>
-    <comment authorId="28" ref="A38" shapeId="0">
+    <comment authorId="29" ref="A39" shapeId="0">
       <text>
         <t>Optional path to a hosts and clusters folder defined on vCenter where VM will be instantiated</t>
       </text>
     </comment>
-    <comment authorId="29" ref="A40" shapeId="0">
+    <comment authorId="30" ref="A41" shapeId="0">
       <text>
         <t>Name of image installed on OpenStack for VSC</t>
       </text>
     </comment>
-    <comment authorId="30" ref="A41" shapeId="0">
+    <comment authorId="31" ref="A42" shapeId="0">
       <text>
         <t>Name of instance flavor installed on OpenStack for VSC</t>
       </text>
     </comment>
-    <comment authorId="31" ref="A42" shapeId="0">
+    <comment authorId="32" ref="A43" shapeId="0">
       <text>
         <t>Name of availability zone on OpenStack for VSC</t>
       </text>
     </comment>
-    <comment authorId="32" ref="A43" shapeId="0">
+    <comment authorId="33" ref="A44" shapeId="0">
       <text>
         <t>Name of management network on OpenStack for VSC</t>
       </text>
     </comment>
-    <comment authorId="33" ref="A44" shapeId="0">
+    <comment authorId="34" ref="A45" shapeId="0">
       <text>
         <t>Name of management subnet on OpenStack for VSC</t>
       </text>
     </comment>
-    <comment authorId="34" ref="A45" shapeId="0">
+    <comment authorId="35" ref="A46" shapeId="0">
       <text>
         <t>Name for Mgmt interface</t>
       </text>
     </comment>
-    <comment authorId="35" ref="A46" shapeId="0">
+    <comment authorId="36" ref="A47" shapeId="0">
       <text>
         <t>Set of security groups to associate with Mgmt interface (List items separated by comma.)</t>
       </text>
     </comment>
-    <comment authorId="36" ref="A47" shapeId="0">
+    <comment authorId="37" ref="A48" shapeId="0">
       <text>
         <t>Name of control network on OpenStack for VSC</t>
       </text>
     </comment>
-    <comment authorId="37" ref="A48" shapeId="0">
+    <comment authorId="38" ref="A49" shapeId="0">
       <text>
         <t>Name of control subnet on OpenStack for VSC</t>
       </text>
     </comment>
-    <comment authorId="38" ref="A49" shapeId="0">
+    <comment authorId="39" ref="A50" shapeId="0">
       <text>
         <t>Name for Control interface</t>
       </text>
     </comment>
-    <comment authorId="39" ref="A50" shapeId="0">
+    <comment authorId="40" ref="A51" shapeId="0">
       <text>
         <t>Set of security groups to associate with Control interface (List items separated by comma.)</t>
       </text>
     </comment>
-    <comment authorId="40" ref="A51" shapeId="0">
+    <comment authorId="41" ref="A52" shapeId="0">
       <text>
         <t>Name for Mgmt interface</t>
       </text>
     </comment>
-    <comment authorId="41" ref="A52" shapeId="0">
+    <comment authorId="42" ref="A53" shapeId="0">
       <text>
         <t>Set of security groups to associate with Mgmt interface (List items separated by comma.)</t>
       </text>
     </comment>
-    <comment authorId="42" ref="A54" shapeId="0">
+    <comment authorId="43" ref="A55" shapeId="0">
       <text>
         <t>Used in postdeploy and health workflows as expected values if non-zero [default: 0]</t>
       </text>
     </comment>
-    <comment authorId="43" ref="A55" shapeId="0">
+    <comment authorId="44" ref="A56" shapeId="0">
       <text>
         <t>Used in postdeploy and health workflows as expected values if non-zero [default: 0]</t>
       </text>
     </comment>
-    <comment authorId="44" ref="A56" shapeId="0">
+    <comment authorId="45" ref="A57" shapeId="0">
       <text>
         <t>Used in postdeploy and health workflows as expected values if non-zero [default: 0]</t>
       </text>
     </comment>
-    <comment authorId="45" ref="A57" shapeId="0">
+    <comment authorId="46" ref="A58" shapeId="0">
       <text>
         <t>Used in postdeploy and health workflows as expected values if non-zero [default: 0]</t>
       </text>
     </comment>
-    <comment authorId="46" ref="A58" shapeId="0">
+    <comment authorId="47" ref="A59" shapeId="0">
       <text>
         <t>Used in postdeploy and health workflows as expected values if non-zero [default: 0]</t>
       </text>
     </comment>
-    <comment authorId="47" ref="A60" shapeId="0">
+    <comment authorId="48" ref="A61" shapeId="0">
       <text>
         <t>Ejabberd user id used to create the certificate</t>
       </text>
     </comment>
-    <comment authorId="48" ref="A61" shapeId="0">
+    <comment authorId="49" ref="A62" shapeId="0">
       <text>
         <t>Path to VSC certificate key pem file</t>
       </text>
     </comment>
-    <comment authorId="49" ref="A62" shapeId="0">
+    <comment authorId="50" ref="A63" shapeId="0">
       <text>
         <t>Path to VSC certificate pem file</t>
       </text>
     </comment>
-    <comment authorId="50" ref="A63" shapeId="0">
+    <comment authorId="51" ref="A64" shapeId="0">
       <text>
         <t>Path to CA certificate pem file</t>
       </text>
     </comment>
-    <comment authorId="51" ref="A64" shapeId="0">
+    <comment authorId="52" ref="A65" shapeId="0">
       <text>
         <t>XMPP domain used in custom certificates</t>
       </text>
     </comment>
-    <comment authorId="52" ref="A65" shapeId="0">
+    <comment authorId="53" ref="A66" shapeId="0">
       <text>
         <t>Name of the credentials set for the vsc</t>
       </text>
     </comment>
-    <comment authorId="53" ref="A67" shapeId="0">
+    <comment authorId="54" ref="A68" shapeId="0">
       <text>
         <t>Cpuset information for cpu pinning on KVM. For example, VSC requires 4 cores and sample values will be of the form [ 0, 1, 2, 3 ] (List items separated by comma.)</t>
       </text>
     </comment>
-    <comment authorId="54" ref="A68" shapeId="0">
+    <comment authorId="55" ref="A69" shapeId="0">
       <text>
         <t>Enables hardening configuration on VSC [default: True]</t>
       </text>
     </comment>
-    <comment authorId="55" ref="A69" shapeId="0">
+    <comment authorId="56" ref="A70" shapeId="0">
       <text>
         <t>Paths to files that can be optionally applied for additional VSC configuration (List items separated by comma.)</t>
       </text>
@@ -10650,7 +10656,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C69"/>
+  <dimension ref="A1:C70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10800,75 +10806,75 @@
     <row r="18">
       <c r="A18" s="6" t="inlineStr">
         <is>
-          <t>VM name</t>
+          <t>Router ID</t>
         </is>
       </c>
       <c r="B18" s="7" t="n"/>
       <c r="C18" s="7" t="n"/>
     </row>
     <row r="19">
-      <c r="A19" s="8" t="inlineStr">
+      <c r="A19" s="6" t="inlineStr">
+        <is>
+          <t>VM name</t>
+        </is>
+      </c>
+      <c r="B19" s="7" t="n"/>
+      <c r="C19" s="7" t="n"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="8" t="inlineStr">
         <is>
           <t>System Name</t>
         </is>
       </c>
-      <c r="B19" s="9" t="n"/>
-      <c r="C19" s="9" t="n"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="6" t="inlineStr">
+      <c r="B20" s="9" t="n"/>
+      <c r="C20" s="9" t="n"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="6" t="inlineStr">
         <is>
           <t>XMPP username</t>
         </is>
       </c>
-      <c r="B20" s="7" t="n"/>
-      <c r="C20" s="7" t="n"/>
-    </row>
-    <row r="21">
-      <c r="A21" s="3" t="inlineStr">
+      <c r="B21" s="7" t="n"/>
+      <c r="C21" s="7" t="n"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="3" t="inlineStr">
         <is>
           <t>Target Server</t>
         </is>
       </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="4" t="inlineStr">
-        <is>
-          <t>Target Server type</t>
-        </is>
-      </c>
-      <c r="B22" s="5" t="n"/>
-      <c r="C22" s="5" t="n"/>
     </row>
     <row r="23">
       <c r="A23" s="4" t="inlineStr">
         <is>
-          <t>Target Server IP or FQDN</t>
+          <t>Target Server type</t>
         </is>
       </c>
       <c r="B23" s="5" t="n"/>
       <c r="C23" s="5" t="n"/>
     </row>
     <row r="24">
-      <c r="A24" s="3" t="inlineStr">
+      <c r="A24" s="4" t="inlineStr">
+        <is>
+          <t>Target Server IP or FQDN</t>
+        </is>
+      </c>
+      <c r="B24" s="5" t="n"/>
+      <c r="C24" s="5" t="n"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="3" t="inlineStr">
         <is>
           <t>Bridges and Private IP</t>
         </is>
       </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="8" t="inlineStr">
-        <is>
-          <t>Management Network Bridge</t>
-        </is>
-      </c>
-      <c r="B25" s="9" t="n"/>
-      <c r="C25" s="9" t="n"/>
     </row>
     <row r="26">
       <c r="A26" s="8" t="inlineStr">
         <is>
-          <t>Data Network Bridge</t>
+          <t>Management Network Bridge</t>
         </is>
       </c>
       <c r="B26" s="9" t="n"/>
@@ -10877,7 +10883,7 @@
     <row r="27">
       <c r="A27" s="8" t="inlineStr">
         <is>
-          <t>VSD FQDN</t>
+          <t>Data Network Bridge</t>
         </is>
       </c>
       <c r="B27" s="9" t="n"/>
@@ -10886,7 +10892,7 @@
     <row r="28">
       <c r="A28" s="8" t="inlineStr">
         <is>
-          <t>Private Management IP</t>
+          <t>VSD FQDN</t>
         </is>
       </c>
       <c r="B28" s="9" t="n"/>
@@ -10895,7 +10901,7 @@
     <row r="29">
       <c r="A29" s="8" t="inlineStr">
         <is>
-          <t>Private Control IP Address</t>
+          <t>Private Management IP</t>
         </is>
       </c>
       <c r="B29" s="9" t="n"/>
@@ -10904,7 +10910,7 @@
     <row r="30">
       <c r="A30" s="8" t="inlineStr">
         <is>
-          <t>Private Data Gateway IP Address</t>
+          <t>Private Control IP Address</t>
         </is>
       </c>
       <c r="B30" s="9" t="n"/>
@@ -10913,32 +10919,32 @@
     <row r="31">
       <c r="A31" s="8" t="inlineStr">
         <is>
-          <t>List of route reflector IPs</t>
+          <t>Private Data Gateway IP Address</t>
         </is>
       </c>
       <c r="B31" s="9" t="n"/>
       <c r="C31" s="9" t="n"/>
     </row>
     <row r="32">
-      <c r="A32" s="3" t="inlineStr">
+      <c r="A32" s="8" t="inlineStr">
+        <is>
+          <t>List of route reflector IPs</t>
+        </is>
+      </c>
+      <c r="B32" s="9" t="n"/>
+      <c r="C32" s="9" t="n"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="3" t="inlineStr">
         <is>
           <t>vCenter Parameters</t>
         </is>
       </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="8" t="inlineStr">
-        <is>
-          <t>vCenter Datacenter Name</t>
-        </is>
-      </c>
-      <c r="B33" s="9" t="n"/>
-      <c r="C33" s="9" t="n"/>
     </row>
     <row r="34">
       <c r="A34" s="8" t="inlineStr">
         <is>
-          <t>vCenter Cluster Name</t>
+          <t>vCenter Datacenter Name</t>
         </is>
       </c>
       <c r="B34" s="9" t="n"/>
@@ -10947,7 +10953,7 @@
     <row r="35">
       <c r="A35" s="8" t="inlineStr">
         <is>
-          <t>vCenter Host Reference</t>
+          <t>vCenter Cluster Name</t>
         </is>
       </c>
       <c r="B35" s="9" t="n"/>
@@ -10956,50 +10962,50 @@
     <row r="36">
       <c r="A36" s="8" t="inlineStr">
         <is>
-          <t>vCenter Datastore Name</t>
+          <t>vCenter Host Reference</t>
         </is>
       </c>
       <c r="B36" s="9" t="n"/>
       <c r="C36" s="9" t="n"/>
     </row>
     <row r="37">
-      <c r="A37" s="6" t="inlineStr">
+      <c r="A37" s="8" t="inlineStr">
+        <is>
+          <t>vCenter Datastore Name</t>
+        </is>
+      </c>
+      <c r="B37" s="9" t="n"/>
+      <c r="C37" s="9" t="n"/>
+    </row>
+    <row r="38">
+      <c r="A38" s="6" t="inlineStr">
         <is>
           <t>vCenter VM Folder</t>
         </is>
       </c>
-      <c r="B37" s="7" t="n"/>
-      <c r="C37" s="7" t="n"/>
-    </row>
-    <row r="38">
-      <c r="A38" s="8" t="inlineStr">
+      <c r="B38" s="7" t="n"/>
+      <c r="C38" s="7" t="n"/>
+    </row>
+    <row r="39">
+      <c r="A39" s="8" t="inlineStr">
         <is>
           <t>vCenter Hosts and Clusters Folder</t>
         </is>
       </c>
-      <c r="B38" s="9" t="n"/>
-      <c r="C38" s="9" t="n"/>
-    </row>
-    <row r="39">
-      <c r="A39" s="3" t="inlineStr">
+      <c r="B39" s="9" t="n"/>
+      <c r="C39" s="9" t="n"/>
+    </row>
+    <row r="40">
+      <c r="A40" s="3" t="inlineStr">
         <is>
           <t>OpenStack Parameters</t>
         </is>
       </c>
-    </row>
-    <row r="40">
-      <c r="A40" s="6" t="inlineStr">
-        <is>
-          <t>OpenStack Image</t>
-        </is>
-      </c>
-      <c r="B40" s="7" t="n"/>
-      <c r="C40" s="7" t="n"/>
     </row>
     <row r="41">
       <c r="A41" s="6" t="inlineStr">
         <is>
-          <t>OpenStack Flavor</t>
+          <t>OpenStack Image</t>
         </is>
       </c>
       <c r="B41" s="7" t="n"/>
@@ -11008,7 +11014,7 @@
     <row r="42">
       <c r="A42" s="6" t="inlineStr">
         <is>
-          <t>OpenStack Availability Zone</t>
+          <t>OpenStack Flavor</t>
         </is>
       </c>
       <c r="B42" s="7" t="n"/>
@@ -11017,7 +11023,7 @@
     <row r="43">
       <c r="A43" s="6" t="inlineStr">
         <is>
-          <t>OpenStack Mgmt Network</t>
+          <t>OpenStack Availability Zone</t>
         </is>
       </c>
       <c r="B43" s="7" t="n"/>
@@ -11026,7 +11032,7 @@
     <row r="44">
       <c r="A44" s="6" t="inlineStr">
         <is>
-          <t>OpenStack Mgmt Subnet</t>
+          <t>OpenStack Mgmt Network</t>
         </is>
       </c>
       <c r="B44" s="7" t="n"/>
@@ -11035,7 +11041,7 @@
     <row r="45">
       <c r="A45" s="6" t="inlineStr">
         <is>
-          <t>OpenStack Mgmt Port Name</t>
+          <t>OpenStack Mgmt Subnet</t>
         </is>
       </c>
       <c r="B45" s="7" t="n"/>
@@ -11044,7 +11050,7 @@
     <row r="46">
       <c r="A46" s="6" t="inlineStr">
         <is>
-          <t>OpenStack Mgmt Port Security Groups</t>
+          <t>OpenStack Mgmt Port Name</t>
         </is>
       </c>
       <c r="B46" s="7" t="n"/>
@@ -11053,7 +11059,7 @@
     <row r="47">
       <c r="A47" s="6" t="inlineStr">
         <is>
-          <t>OpenStack Control Network</t>
+          <t>OpenStack Mgmt Port Security Groups</t>
         </is>
       </c>
       <c r="B47" s="7" t="n"/>
@@ -11062,7 +11068,7 @@
     <row r="48">
       <c r="A48" s="6" t="inlineStr">
         <is>
-          <t>OpenStack Control Subnet</t>
+          <t>OpenStack Control Network</t>
         </is>
       </c>
       <c r="B48" s="7" t="n"/>
@@ -11071,7 +11077,7 @@
     <row r="49">
       <c r="A49" s="6" t="inlineStr">
         <is>
-          <t>OpenStack Control Port Name</t>
+          <t>OpenStack Control Subnet</t>
         </is>
       </c>
       <c r="B49" s="7" t="n"/>
@@ -11080,7 +11086,7 @@
     <row r="50">
       <c r="A50" s="6" t="inlineStr">
         <is>
-          <t>OpenStack Control Port Security Groups</t>
+          <t>OpenStack Control Port Name</t>
         </is>
       </c>
       <c r="B50" s="7" t="n"/>
@@ -11089,7 +11095,7 @@
     <row r="51">
       <c r="A51" s="6" t="inlineStr">
         <is>
-          <t>OpenStack Port Name</t>
+          <t>OpenStack Control Port Security Groups</t>
         </is>
       </c>
       <c r="B51" s="7" t="n"/>
@@ -11098,32 +11104,32 @@
     <row r="52">
       <c r="A52" s="6" t="inlineStr">
         <is>
-          <t>OpenStack Port Security Groups</t>
+          <t>OpenStack Port Name</t>
         </is>
       </c>
       <c r="B52" s="7" t="n"/>
       <c r="C52" s="7" t="n"/>
     </row>
     <row r="53">
-      <c r="A53" s="3" t="inlineStr">
+      <c r="A53" s="6" t="inlineStr">
+        <is>
+          <t>OpenStack Port Security Groups</t>
+        </is>
+      </c>
+      <c r="B53" s="7" t="n"/>
+      <c r="C53" s="7" t="n"/>
+    </row>
+    <row r="54">
+      <c r="A54" s="3" t="inlineStr">
         <is>
           <t>Health Parameters</t>
         </is>
       </c>
-    </row>
-    <row r="54">
-      <c r="A54" s="8" t="inlineStr">
-        <is>
-          <t>Expected number of BGP neighbors</t>
-        </is>
-      </c>
-      <c r="B54" s="9" t="n"/>
-      <c r="C54" s="9" t="n"/>
     </row>
     <row r="55">
       <c r="A55" s="8" t="inlineStr">
         <is>
-          <t>Expected number of vswitches</t>
+          <t>Expected number of BGP neighbors</t>
         </is>
       </c>
       <c r="B55" s="9" t="n"/>
@@ -11132,7 +11138,7 @@
     <row r="56">
       <c r="A56" s="8" t="inlineStr">
         <is>
-          <t>Expected number of host vports</t>
+          <t>Expected number of vswitches</t>
         </is>
       </c>
       <c r="B56" s="9" t="n"/>
@@ -11141,7 +11147,7 @@
     <row r="57">
       <c r="A57" s="8" t="inlineStr">
         <is>
-          <t>Expected number of VM vports</t>
+          <t>Expected number of host vports</t>
         </is>
       </c>
       <c r="B57" s="9" t="n"/>
@@ -11150,32 +11156,32 @@
     <row r="58">
       <c r="A58" s="8" t="inlineStr">
         <is>
-          <t>Expected number of gateway ports</t>
+          <t>Expected number of VM vports</t>
         </is>
       </c>
       <c r="B58" s="9" t="n"/>
       <c r="C58" s="9" t="n"/>
     </row>
     <row r="59">
-      <c r="A59" s="3" t="inlineStr">
+      <c r="A59" s="8" t="inlineStr">
+        <is>
+          <t>Expected number of gateway ports</t>
+        </is>
+      </c>
+      <c r="B59" s="9" t="n"/>
+      <c r="C59" s="9" t="n"/>
+    </row>
+    <row r="60">
+      <c r="A60" s="3" t="inlineStr">
         <is>
           <t>Certificates and credentials</t>
         </is>
       </c>
-    </row>
-    <row r="60">
-      <c r="A60" s="8" t="inlineStr">
-        <is>
-          <t>Ejabberd user id</t>
-        </is>
-      </c>
-      <c r="B60" s="9" t="n"/>
-      <c r="C60" s="9" t="n"/>
     </row>
     <row r="61">
       <c r="A61" s="8" t="inlineStr">
         <is>
-          <t>Private key path</t>
+          <t>Ejabberd user id</t>
         </is>
       </c>
       <c r="B61" s="9" t="n"/>
@@ -11184,7 +11190,7 @@
     <row r="62">
       <c r="A62" s="8" t="inlineStr">
         <is>
-          <t>Certificate path</t>
+          <t>Private key path</t>
         </is>
       </c>
       <c r="B62" s="9" t="n"/>
@@ -11193,7 +11199,7 @@
     <row r="63">
       <c r="A63" s="8" t="inlineStr">
         <is>
-          <t>CA certificate path</t>
+          <t>Certificate path</t>
         </is>
       </c>
       <c r="B63" s="9" t="n"/>
@@ -11202,7 +11208,7 @@
     <row r="64">
       <c r="A64" s="8" t="inlineStr">
         <is>
-          <t>XMPP domain</t>
+          <t>CA certificate path</t>
         </is>
       </c>
       <c r="B64" s="9" t="n"/>
@@ -11211,32 +11217,32 @@
     <row r="65">
       <c r="A65" s="8" t="inlineStr">
         <is>
-          <t>Credentials set name</t>
+          <t>XMPP domain</t>
         </is>
       </c>
       <c r="B65" s="9" t="n"/>
       <c r="C65" s="9" t="n"/>
     </row>
     <row r="66">
-      <c r="A66" s="3" t="inlineStr">
+      <c r="A66" s="8" t="inlineStr">
+        <is>
+          <t>Credentials set name</t>
+        </is>
+      </c>
+      <c r="B66" s="9" t="n"/>
+      <c r="C66" s="9" t="n"/>
+    </row>
+    <row r="67">
+      <c r="A67" s="3" t="inlineStr">
         <is>
           <t>VSC Options</t>
         </is>
       </c>
-    </row>
-    <row r="67">
-      <c r="A67" s="8" t="inlineStr">
-        <is>
-          <t>KVM cpuset information</t>
-        </is>
-      </c>
-      <c r="B67" s="9" t="n"/>
-      <c r="C67" s="9" t="n"/>
     </row>
     <row r="68">
       <c r="A68" s="8" t="inlineStr">
         <is>
-          <t>Harden VSC</t>
+          <t>KVM cpuset information</t>
         </is>
       </c>
       <c r="B68" s="9" t="n"/>
@@ -11245,24 +11251,33 @@
     <row r="69">
       <c r="A69" s="8" t="inlineStr">
         <is>
-          <t>Paths to VSC Config Files</t>
+          <t>Harden VSC</t>
         </is>
       </c>
       <c r="B69" s="9" t="n"/>
       <c r="C69" s="9" t="n"/>
+    </row>
+    <row r="70">
+      <c r="A70" s="8" t="inlineStr">
+        <is>
+          <t>Paths to VSC Config Files</t>
+        </is>
+      </c>
+      <c r="B70" s="9" t="n"/>
+      <c r="C70" s="9" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="A10:C10"/>
     <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="A32:C32"/>
-    <mergeCell ref="A39:C39"/>
-    <mergeCell ref="A53:C53"/>
-    <mergeCell ref="A59:C59"/>
-    <mergeCell ref="A66:C66"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A33:C33"/>
+    <mergeCell ref="A40:C40"/>
+    <mergeCell ref="A54:C54"/>
+    <mergeCell ref="A60:C60"/>
+    <mergeCell ref="A67:C67"/>
   </mergeCells>
   <dataValidations count="20">
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B7" type="whole"/>
@@ -11271,14 +11286,12 @@
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="C12" type="whole"/>
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B13" type="whole"/>
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="C13" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="B22" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="B23" type="list">
       <formula1>"kvm,vcenter,openstack,nuagex,none"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="C22" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="C23" type="list">
       <formula1>"kvm,vcenter,openstack,nuagex,none"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B54" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="C54" type="whole"/>
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B55" type="whole"/>
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="C55" type="whole"/>
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B56" type="whole"/>
@@ -11287,10 +11300,12 @@
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="C57" type="whole"/>
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B58" type="whole"/>
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="C58" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="B68" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B59" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="C59" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="B69" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="C68" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="C69" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
added <including the file name> to enhance several descriptions in common.json
</commit_message>
<xml_diff>
--- a/examples/excel/active_standby_vsds.xlsx
+++ b/examples/excel/active_standby_vsds.xlsx
@@ -1408,12 +1408,12 @@
     </comment>
     <comment authorId="49" ref="A65" shapeId="0">
       <text>
-        <t>Path to the standard license file for the VSD [default: ]</t>
+        <t>Path to the standard license file for the VSD including the file name [default: ]</t>
       </text>
     </comment>
     <comment authorId="50" ref="A66" shapeId="0">
       <text>
-        <t>Path to the cluster license file for the VSD [default: ]</t>
+        <t>Path to the cluster license file for the VSD including the file name [default: ]</t>
       </text>
     </comment>
     <comment authorId="51" ref="A67" shapeId="0">
@@ -1423,17 +1423,17 @@
     </comment>
     <comment authorId="52" ref="A68" shapeId="0">
       <text>
-        <t>Path to the Ejabberd license file for the VSD [default: ]</t>
+        <t>Path to the Ejabberd license file for the VSD including the file name [default: ]</t>
       </text>
     </comment>
     <comment authorId="53" ref="A69" shapeId="0">
       <text>
-        <t>Path to the license file for the SD-WAN Portal [default: ]</t>
+        <t>Path to the license file for the SD-WAN Portal including the file name [default: ]</t>
       </text>
     </comment>
     <comment authorId="54" ref="A70" shapeId="0">
       <text>
-        <t>Path to the license file for the NUH [default: ]</t>
+        <t>Path to the license file for the NUH including the file name [default: ]</t>
       </text>
     </comment>
     <comment authorId="55" ref="A72" shapeId="0">
@@ -7206,7 +7206,7 @@
     <row r="69">
       <c r="A69" s="8" t="inlineStr">
         <is>
-          <t>SD-WAN Portal License Filename</t>
+          <t>SD-WAN Portal License File</t>
         </is>
       </c>
       <c r="B69" s="9" t="n"/>

</xml_diff>

<commit_message>
Adding portal fallocate size
</commit_message>
<xml_diff>
--- a/examples/excel/active_standby_vsds.xlsx
+++ b/examples/excel/active_standby_vsds.xlsx
@@ -1121,6 +1121,7 @@
     <author>vsd_fallocate_size_gb</author>
     <author>vsc_fallocate_size_gb</author>
     <author>vstat_allocate_size_gb</author>
+    <author>portal_allocate_size_gb</author>
     <author>vcin_allocate_size_gb</author>
     <author>nsgv_allocate_size_gb</author>
     <author>vsd_ram</author>
@@ -1478,190 +1479,195 @@
     </comment>
     <comment authorId="63" ref="A81" shapeId="0">
       <text>
+        <t>Amount of Portal disk space to pre-allocate, in GB. Note: Values smaller than the default are for lab and PoC only. Production deployments should not modify this value. [default: 285]</t>
+      </text>
+    </comment>
+    <comment authorId="64" ref="A82" shapeId="0">
+      <text>
         <t>Amount of VCIN disk space to pre-allocate, in GB. Note: Values smaller than the default are for lab and PoC only. Production deployments should not modify this value. [default: 285]</t>
       </text>
     </comment>
-    <comment authorId="64" ref="A82" shapeId="0">
+    <comment authorId="65" ref="A83" shapeId="0">
       <text>
         <t>Amount of NSGV disk space to pre-allocate, in GB. Note: Values smaller than the default are for lab and PoC only. Production deployments should not modify this value. [default: 4]</t>
       </text>
     </comment>
-    <comment authorId="65" ref="A84" shapeId="0">
+    <comment authorId="66" ref="A85" shapeId="0">
       <text>
         <t>Amount of VSD RAM to allocate, in GB. Valid only for KVM deployments. Note: Values smaller than the default are for lab and PoC only. Production deployments must use a value greater than or equal to the default. [default: 24]</t>
       </text>
     </comment>
-    <comment authorId="66" ref="A85" shapeId="0">
+    <comment authorId="67" ref="A86" shapeId="0">
       <text>
         <t>Amount of VSC RAM to allocate, in GB. Valid only for KVM deployments. Note: Values smaller than the default are for lab and PoC only. Production deployments must use a value greater than or equal to the default. [default: 4]</t>
       </text>
     </comment>
-    <comment authorId="67" ref="A86" shapeId="0">
+    <comment authorId="68" ref="A87" shapeId="0">
       <text>
         <t>Amount of VSTAT RAM to allocate, in GB. Valid only for KVM deployments. Note: Values smaller than the default are for lab and PoC only. Production deployments must use a value greater than or equal to the default. [default: 16]</t>
       </text>
     </comment>
-    <comment authorId="68" ref="A87" shapeId="0">
+    <comment authorId="69" ref="A88" shapeId="0">
       <text>
         <t>Amount of VCIN RAM to allocate, in GB. Valid only for KVM deployments. Note: Values smaller than the default are for lab and PoC only. Production deployments must use a value greater than or equal to the default. [default: 24]</t>
       </text>
     </comment>
-    <comment authorId="69" ref="A88" shapeId="0">
+    <comment authorId="70" ref="A89" shapeId="0">
       <text>
         <t>Amount of NUH RAM to allocate, in GB. Valid only for KVM deployments. Note: Values smaller than the default are for lab and PoC only. Production deployments must use a value greater than or equal to the default. [default: 8]</t>
       </text>
     </comment>
-    <comment authorId="70" ref="A89" shapeId="0">
+    <comment authorId="71" ref="A90" shapeId="0">
       <text>
         <t>Amount of Webfilter RAM to allocate, in GB. Valid only for KVM deployments. Note: Values smaller than the default are for lab and PoC only. Production deployments must use a value greater than or equal to the default. [default: 8]</t>
       </text>
     </comment>
-    <comment authorId="71" ref="A90" shapeId="0">
+    <comment authorId="72" ref="A91" shapeId="0">
       <text>
         <t>Amount of Portal RAM to allocate, in GB. Valid only for KVM deployments. Note: Values smaller than the default are for lab and PoC only. Production deployments must use a value greater than or equal to the default. [default: 24]</t>
       </text>
     </comment>
-    <comment authorId="72" ref="A92" shapeId="0">
+    <comment authorId="73" ref="A93" shapeId="0">
       <text>
         <t>Number of CPU's for VSD. Valid only for KVM deployments [default: 6]</t>
       </text>
     </comment>
-    <comment authorId="73" ref="A93" shapeId="0">
+    <comment authorId="74" ref="A94" shapeId="0">
       <text>
         <t>Number of CPU's for VSC. Valid only for KVM deployments [default: 6]</t>
       </text>
     </comment>
-    <comment authorId="74" ref="A94" shapeId="0">
+    <comment authorId="75" ref="A95" shapeId="0">
       <text>
         <t>Number of CPU's for VSTAT. Valid only for KVM deployments [default: 6]</t>
       </text>
     </comment>
-    <comment authorId="75" ref="A95" shapeId="0">
+    <comment authorId="76" ref="A96" shapeId="0">
       <text>
         <t>Number of CPU's for VNSUTIL. Valid only for KVM deployments [default: 2]</t>
       </text>
     </comment>
-    <comment authorId="76" ref="A96" shapeId="0">
+    <comment authorId="77" ref="A97" shapeId="0">
       <text>
         <t>Number of CPU's for NUH. Valid only for KVM deployments [default: 2]</t>
       </text>
     </comment>
-    <comment authorId="77" ref="A97" shapeId="0">
+    <comment authorId="78" ref="A98" shapeId="0">
       <text>
         <t>Number of CPU's for VCIN. Valid only for KVM deployments [default: 6]</t>
       </text>
     </comment>
-    <comment authorId="78" ref="A98" shapeId="0">
+    <comment authorId="79" ref="A99" shapeId="0">
       <text>
         <t>Number of CPU's for Portal vm. Valid only for KVM deployments [default: 6]</t>
       </text>
     </comment>
-    <comment authorId="79" ref="A99" shapeId="0">
+    <comment authorId="80" ref="A100" shapeId="0">
       <text>
         <t>Number of CPU's for Webfilter vm. Valid only for KVM deployments [default: 2]</t>
       </text>
     </comment>
-    <comment authorId="80" ref="A101" shapeId="0">
+    <comment authorId="81" ref="A102" shapeId="0">
       <text>
         <t>VSD Architect URL. Required for tasks during Upgrade, Health Checks etc [default: https://(vsd_fqdn):8443]</t>
       </text>
     </comment>
-    <comment authorId="81" ref="A102" shapeId="0">
+    <comment authorId="82" ref="A103" shapeId="0">
       <text>
         <t>Enterprise name used for authentication with VSD Architect. Required for tasks during Upgrade, Health Checks etc [default: csp]</t>
       </text>
     </comment>
-    <comment authorId="82" ref="A103" shapeId="0">
+    <comment authorId="83" ref="A104" shapeId="0">
       <text>
         <t>VCIN URL used for API interaction. Required for tasks like VRS-E upgrade (through VCIN) [default: https://(vcin_ip_address):8443]</t>
       </text>
     </comment>
-    <comment authorId="83" ref="A104" shapeId="0">
+    <comment authorId="84" ref="A105" shapeId="0">
       <text>
         <t>Enterprise name used for authentication with VCIN. Required for tasks like VRS-E upgrade (through VCIN) [default: csp]</t>
       </text>
     </comment>
-    <comment authorId="84" ref="A106" shapeId="0">
+    <comment authorId="85" ref="A107" shapeId="0">
       <text>
         <t>List of hooks files (List items separated by comma.)</t>
       </text>
     </comment>
-    <comment authorId="85" ref="A107" shapeId="0">
+    <comment authorId="86" ref="A108" shapeId="0">
       <text>
         <t>Skip tasks and playbooks (List items separated by comma.)</t>
       </text>
     </comment>
-    <comment authorId="86" ref="A109" shapeId="0">
+    <comment authorId="87" ref="A110" shapeId="0">
       <text>
         <t>Address of SMTP server to be used if emailing health results</t>
       </text>
     </comment>
-    <comment authorId="87" ref="A110" shapeId="0">
+    <comment authorId="88" ref="A111" shapeId="0">
       <text>
         <t>Port to be used on the SMTP Server [default: 25]</t>
       </text>
     </comment>
-    <comment authorId="88" ref="A111" shapeId="0">
+    <comment authorId="89" ref="A112" shapeId="0">
       <text>
         <t>Email address from which health report will be sent</t>
       </text>
     </comment>
-    <comment authorId="89" ref="A112" shapeId="0">
+    <comment authorId="90" ref="A113" shapeId="0">
       <text>
         <t>List of destination email addresses (List items separated by comma.)</t>
       </text>
     </comment>
-    <comment authorId="90" ref="A114" shapeId="0">
+    <comment authorId="91" ref="A115" shapeId="0">
       <text>
         <t>Address of the mail server to be used to receive monit alerts via email</t>
       </text>
     </comment>
-    <comment authorId="91" ref="A115" shapeId="0">
+    <comment authorId="92" ref="A116" shapeId="0">
       <text>
         <t>Port on mail server to be used for monit alerts [default: 25]</t>
       </text>
     </comment>
-    <comment authorId="92" ref="A116" shapeId="0">
+    <comment authorId="93" ref="A117" shapeId="0">
       <text>
         <t>Encryption to be used when sending monit alerts via email</t>
       </text>
     </comment>
-    <comment authorId="93" ref="A117" shapeId="0">
+    <comment authorId="94" ref="A118" shapeId="0">
       <text>
         <t>Enables use of monit eventqueue to store alerts if email alerts fail to send [default: True]</t>
       </text>
     </comment>
-    <comment authorId="94" ref="A118" shapeId="0">
+    <comment authorId="95" ref="A119" shapeId="0">
       <text>
         <t>Email address from which monit alerts will be sent</t>
       </text>
     </comment>
-    <comment authorId="95" ref="A119" shapeId="0">
+    <comment authorId="96" ref="A120" shapeId="0">
       <text>
         <t>Email address to reply to monit alert emails</t>
       </text>
     </comment>
-    <comment authorId="96" ref="A120" shapeId="0">
+    <comment authorId="97" ref="A121" shapeId="0">
       <text>
         <t>Email subject for alert emails. Overrides monit default alert subject</t>
       </text>
     </comment>
-    <comment authorId="97" ref="A121" shapeId="0">
+    <comment authorId="98" ref="A122" shapeId="0">
       <text>
         <t>Email message for alert emails. Overrides monit default alert message</t>
       </text>
     </comment>
-    <comment authorId="98" ref="A122" shapeId="0">
+    <comment authorId="99" ref="A123" shapeId="0">
       <text>
         <t>Destination email address for monit alerts</t>
       </text>
     </comment>
-    <comment authorId="99" ref="A123" shapeId="0">
+    <comment authorId="100" ref="A124" shapeId="0">
       <text>
         <t>Specific events for which alerts should be sent. One string can be used to hold multiple events, separated by commas</t>
       </text>
     </comment>
-    <comment authorId="100" ref="A124" shapeId="0">
+    <comment authorId="101" ref="A125" shapeId="0">
       <text>
         <t>Events for which alerts should not be sent. One string can be used to hold multiple events, separated by commas</t>
       </text>
@@ -6641,7 +6647,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B124"/>
+  <dimension ref="A1:B125"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7300,7 +7306,7 @@
     <row r="81">
       <c r="A81" s="8" t="inlineStr">
         <is>
-          <t>VCIN Disk Size</t>
+          <t>Portal Disk Size</t>
         </is>
       </c>
       <c r="B81" s="9" t="n"/>
@@ -7308,30 +7314,30 @@
     <row r="82">
       <c r="A82" s="8" t="inlineStr">
         <is>
+          <t>VCIN Disk Size</t>
+        </is>
+      </c>
+      <c r="B82" s="9" t="n"/>
+    </row>
+    <row r="83">
+      <c r="A83" s="8" t="inlineStr">
+        <is>
           <t>NSGV Disk Size</t>
         </is>
       </c>
-      <c r="B82" s="9" t="n"/>
-    </row>
-    <row r="83">
-      <c r="A83" s="3" t="inlineStr">
+      <c r="B83" s="9" t="n"/>
+    </row>
+    <row r="84">
+      <c r="A84" s="3" t="inlineStr">
         <is>
           <t>KVM RAM</t>
         </is>
       </c>
-    </row>
-    <row r="84">
-      <c r="A84" s="8" t="inlineStr">
-        <is>
-          <t>KVM VSD RAM</t>
-        </is>
-      </c>
-      <c r="B84" s="9" t="n"/>
     </row>
     <row r="85">
       <c r="A85" s="8" t="inlineStr">
         <is>
-          <t>KVM VSC RAM</t>
+          <t>KVM VSD RAM</t>
         </is>
       </c>
       <c r="B85" s="9" t="n"/>
@@ -7339,7 +7345,7 @@
     <row r="86">
       <c r="A86" s="8" t="inlineStr">
         <is>
-          <t>KVM VSTAT RAM</t>
+          <t>KVM VSC RAM</t>
         </is>
       </c>
       <c r="B86" s="9" t="n"/>
@@ -7347,7 +7353,7 @@
     <row r="87">
       <c r="A87" s="8" t="inlineStr">
         <is>
-          <t>KVM VCIN RAM</t>
+          <t>KVM VSTAT RAM</t>
         </is>
       </c>
       <c r="B87" s="9" t="n"/>
@@ -7355,7 +7361,7 @@
     <row r="88">
       <c r="A88" s="8" t="inlineStr">
         <is>
-          <t>KVM NUH RAM</t>
+          <t>KVM VCIN RAM</t>
         </is>
       </c>
       <c r="B88" s="9" t="n"/>
@@ -7363,7 +7369,7 @@
     <row r="89">
       <c r="A89" s="8" t="inlineStr">
         <is>
-          <t>KVM Webfilter RAM</t>
+          <t>KVM NUH RAM</t>
         </is>
       </c>
       <c r="B89" s="9" t="n"/>
@@ -7371,30 +7377,30 @@
     <row r="90">
       <c r="A90" s="8" t="inlineStr">
         <is>
+          <t>KVM Webfilter RAM</t>
+        </is>
+      </c>
+      <c r="B90" s="9" t="n"/>
+    </row>
+    <row r="91">
+      <c r="A91" s="8" t="inlineStr">
+        <is>
           <t>KVM Portal RAM</t>
         </is>
       </c>
-      <c r="B90" s="9" t="n"/>
-    </row>
-    <row r="91">
-      <c r="A91" s="3" t="inlineStr">
+      <c r="B91" s="9" t="n"/>
+    </row>
+    <row r="92">
+      <c r="A92" s="3" t="inlineStr">
         <is>
           <t>KVM CPU</t>
         </is>
       </c>
-    </row>
-    <row r="92">
-      <c r="A92" s="8" t="inlineStr">
-        <is>
-          <t>KVM VSD CPU cores</t>
-        </is>
-      </c>
-      <c r="B92" s="9" t="n"/>
     </row>
     <row r="93">
       <c r="A93" s="8" t="inlineStr">
         <is>
-          <t>VSC CPU cores</t>
+          <t>KVM VSD CPU cores</t>
         </is>
       </c>
       <c r="B93" s="9" t="n"/>
@@ -7402,7 +7408,7 @@
     <row r="94">
       <c r="A94" s="8" t="inlineStr">
         <is>
-          <t>KVM VSTAT CPU cores</t>
+          <t>VSC CPU cores</t>
         </is>
       </c>
       <c r="B94" s="9" t="n"/>
@@ -7410,7 +7416,7 @@
     <row r="95">
       <c r="A95" s="8" t="inlineStr">
         <is>
-          <t>KVM VNSUTIL CPU cores</t>
+          <t>KVM VSTAT CPU cores</t>
         </is>
       </c>
       <c r="B95" s="9" t="n"/>
@@ -7418,7 +7424,7 @@
     <row r="96">
       <c r="A96" s="8" t="inlineStr">
         <is>
-          <t>KVM NUH CPU cores</t>
+          <t>KVM VNSUTIL CPU cores</t>
         </is>
       </c>
       <c r="B96" s="9" t="n"/>
@@ -7426,7 +7432,7 @@
     <row r="97">
       <c r="A97" s="8" t="inlineStr">
         <is>
-          <t>KVM VCIN CPU cores</t>
+          <t>KVM NUH CPU cores</t>
         </is>
       </c>
       <c r="B97" s="9" t="n"/>
@@ -7434,7 +7440,7 @@
     <row r="98">
       <c r="A98" s="8" t="inlineStr">
         <is>
-          <t>KVM Portal VM CPU cores</t>
+          <t>KVM VCIN CPU cores</t>
         </is>
       </c>
       <c r="B98" s="9" t="n"/>
@@ -7442,30 +7448,30 @@
     <row r="99">
       <c r="A99" s="8" t="inlineStr">
         <is>
+          <t>KVM Portal VM CPU cores</t>
+        </is>
+      </c>
+      <c r="B99" s="9" t="n"/>
+    </row>
+    <row r="100">
+      <c r="A100" s="8" t="inlineStr">
+        <is>
           <t>KVM Webfilter VM CPU cores</t>
         </is>
       </c>
-      <c r="B99" s="9" t="n"/>
-    </row>
-    <row r="100">
-      <c r="A100" s="3" t="inlineStr">
+      <c r="B100" s="9" t="n"/>
+    </row>
+    <row r="101">
+      <c r="A101" s="3" t="inlineStr">
         <is>
           <t>Authentication</t>
         </is>
       </c>
-    </row>
-    <row r="101">
-      <c r="A101" s="8" t="inlineStr">
-        <is>
-          <t>VSD Architect URL</t>
-        </is>
-      </c>
-      <c r="B101" s="9" t="n"/>
     </row>
     <row r="102">
       <c r="A102" s="8" t="inlineStr">
         <is>
-          <t>VSD Enterprise</t>
+          <t>VSD Architect URL</t>
         </is>
       </c>
       <c r="B102" s="9" t="n"/>
@@ -7473,7 +7479,7 @@
     <row r="103">
       <c r="A103" s="8" t="inlineStr">
         <is>
-          <t>VCIN URL</t>
+          <t>VSD Enterprise</t>
         </is>
       </c>
       <c r="B103" s="9" t="n"/>
@@ -7481,53 +7487,53 @@
     <row r="104">
       <c r="A104" s="8" t="inlineStr">
         <is>
+          <t>VCIN URL</t>
+        </is>
+      </c>
+      <c r="B104" s="9" t="n"/>
+    </row>
+    <row r="105">
+      <c r="A105" s="8" t="inlineStr">
+        <is>
           <t>VCIN Enterprise</t>
         </is>
       </c>
-      <c r="B104" s="9" t="n"/>
-    </row>
-    <row r="105">
-      <c r="A105" s="3" t="inlineStr">
+      <c r="B105" s="9" t="n"/>
+    </row>
+    <row r="106">
+      <c r="A106" s="3" t="inlineStr">
         <is>
           <t>Hooks</t>
         </is>
       </c>
-    </row>
-    <row r="106">
-      <c r="A106" s="8" t="inlineStr">
-        <is>
-          <t>hooks</t>
-        </is>
-      </c>
-      <c r="B106" s="9" t="n"/>
     </row>
     <row r="107">
       <c r="A107" s="8" t="inlineStr">
         <is>
+          <t>hooks</t>
+        </is>
+      </c>
+      <c r="B107" s="9" t="n"/>
+    </row>
+    <row r="108">
+      <c r="A108" s="8" t="inlineStr">
+        <is>
           <t>skip actions</t>
         </is>
       </c>
-      <c r="B107" s="9" t="n"/>
-    </row>
-    <row r="108">
-      <c r="A108" s="3" t="inlineStr">
+      <c r="B108" s="9" t="n"/>
+    </row>
+    <row r="109">
+      <c r="A109" s="3" t="inlineStr">
         <is>
           <t>Component Health Report Email Options</t>
         </is>
       </c>
-    </row>
-    <row r="109">
-      <c r="A109" s="8" t="inlineStr">
-        <is>
-          <t>Health Report SMTP Server</t>
-        </is>
-      </c>
-      <c r="B109" s="9" t="n"/>
     </row>
     <row r="110">
       <c r="A110" s="8" t="inlineStr">
         <is>
-          <t>Health Report SMTP Server Port</t>
+          <t>Health Report SMTP Server</t>
         </is>
       </c>
       <c r="B110" s="9" t="n"/>
@@ -7535,7 +7541,7 @@
     <row r="111">
       <c r="A111" s="8" t="inlineStr">
         <is>
-          <t>Health Report Email From Address</t>
+          <t>Health Report SMTP Server Port</t>
         </is>
       </c>
       <c r="B111" s="9" t="n"/>
@@ -7543,30 +7549,30 @@
     <row r="112">
       <c r="A112" s="8" t="inlineStr">
         <is>
+          <t>Health Report Email From Address</t>
+        </is>
+      </c>
+      <c r="B112" s="9" t="n"/>
+    </row>
+    <row r="113">
+      <c r="A113" s="8" t="inlineStr">
+        <is>
           <t>Health Report Destination Email Address(es)</t>
         </is>
       </c>
-      <c r="B112" s="9" t="n"/>
-    </row>
-    <row r="113">
-      <c r="A113" s="3" t="inlineStr">
+      <c r="B113" s="9" t="n"/>
+    </row>
+    <row r="114">
+      <c r="A114" s="3" t="inlineStr">
         <is>
           <t>VSD Monit Email Alerts Configuration</t>
         </is>
       </c>
-    </row>
-    <row r="114">
-      <c r="A114" s="8" t="inlineStr">
-        <is>
-          <t>VSD Monit Mail Server</t>
-        </is>
-      </c>
-      <c r="B114" s="9" t="n"/>
     </row>
     <row r="115">
       <c r="A115" s="8" t="inlineStr">
         <is>
-          <t>VSD Monit Mail Server Port</t>
+          <t>VSD Monit Mail Server</t>
         </is>
       </c>
       <c r="B115" s="9" t="n"/>
@@ -7574,7 +7580,7 @@
     <row r="116">
       <c r="A116" s="8" t="inlineStr">
         <is>
-          <t>VSD Monit Mail Server Encryption Type</t>
+          <t>VSD Monit Mail Server Port</t>
         </is>
       </c>
       <c r="B116" s="9" t="n"/>
@@ -7582,7 +7588,7 @@
     <row r="117">
       <c r="A117" s="8" t="inlineStr">
         <is>
-          <t>Use VSD Monit Eventqueue</t>
+          <t>VSD Monit Mail Server Encryption Type</t>
         </is>
       </c>
       <c r="B117" s="9" t="n"/>
@@ -7590,7 +7596,7 @@
     <row r="118">
       <c r="A118" s="8" t="inlineStr">
         <is>
-          <t>VSD Monit From Email Address</t>
+          <t>Use VSD Monit Eventqueue</t>
         </is>
       </c>
       <c r="B118" s="9" t="n"/>
@@ -7598,7 +7604,7 @@
     <row r="119">
       <c r="A119" s="8" t="inlineStr">
         <is>
-          <t>VSD Monit Reply-To Email Address</t>
+          <t>VSD Monit From Email Address</t>
         </is>
       </c>
       <c r="B119" s="9" t="n"/>
@@ -7606,7 +7612,7 @@
     <row r="120">
       <c r="A120" s="8" t="inlineStr">
         <is>
-          <t>VSD Monit Email Alert Subject</t>
+          <t>VSD Monit Reply-To Email Address</t>
         </is>
       </c>
       <c r="B120" s="9" t="n"/>
@@ -7614,7 +7620,7 @@
     <row r="121">
       <c r="A121" s="8" t="inlineStr">
         <is>
-          <t>VSD Monit Email Alert Message</t>
+          <t>VSD Monit Email Alert Subject</t>
         </is>
       </c>
       <c r="B121" s="9" t="n"/>
@@ -7622,7 +7628,7 @@
     <row r="122">
       <c r="A122" s="8" t="inlineStr">
         <is>
-          <t>VSD Monit Destination Email Address</t>
+          <t>VSD Monit Email Alert Message</t>
         </is>
       </c>
       <c r="B122" s="9" t="n"/>
@@ -7630,7 +7636,7 @@
     <row r="123">
       <c r="A123" s="8" t="inlineStr">
         <is>
-          <t>VSD Monit Only Alert On</t>
+          <t>VSD Monit Destination Email Address</t>
         </is>
       </c>
       <c r="B123" s="9" t="n"/>
@@ -7638,10 +7644,18 @@
     <row r="124">
       <c r="A124" s="8" t="inlineStr">
         <is>
+          <t>VSD Monit Only Alert On</t>
+        </is>
+      </c>
+      <c r="B124" s="9" t="n"/>
+    </row>
+    <row r="125">
+      <c r="A125" s="8" t="inlineStr">
+        <is>
           <t>VSD Monit Do Not Alert On</t>
         </is>
       </c>
-      <c r="B124" s="9" t="n"/>
+      <c r="B125" s="9" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="20">
@@ -7659,14 +7673,14 @@
     <mergeCell ref="A64:B64"/>
     <mergeCell ref="A71:B71"/>
     <mergeCell ref="A77:B77"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="A91:B91"/>
-    <mergeCell ref="A100:B100"/>
-    <mergeCell ref="A105:B105"/>
-    <mergeCell ref="A108:B108"/>
-    <mergeCell ref="A113:B113"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="A101:B101"/>
+    <mergeCell ref="A106:B106"/>
+    <mergeCell ref="A109:B109"/>
+    <mergeCell ref="A114:B114"/>
   </mergeCells>
-  <dataValidations count="39">
+  <dataValidations count="40">
     <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="B24" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
@@ -7712,14 +7726,14 @@
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B80" type="whole"/>
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B81" type="whole"/>
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B82" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B84" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B83" type="whole"/>
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B85" type="whole"/>
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B86" type="whole"/>
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B87" type="whole"/>
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B88" type="whole"/>
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B89" type="whole"/>
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B90" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B92" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B91" type="whole"/>
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B93" type="whole"/>
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B94" type="whole"/>
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B95" type="whole"/>
@@ -7727,9 +7741,10 @@
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B97" type="whole"/>
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B98" type="whole"/>
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B99" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B110" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B115" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="B117" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B100" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B111" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B116" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="B118" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Template changes to automate NSGv bootstrap
</commit_message>
<xml_diff>
--- a/examples/excel/active_standby_vsds.xlsx
+++ b/examples/excel/active_standby_vsds.xlsx
@@ -342,6 +342,7 @@
     <author>provision_vpc_nsg_wan_subnet_cidr</author>
     <author>provision_vpc_nsg_lan_subnet_cidr</author>
     <author>provision_vpc_private_subnet_cidr</author>
+    <author>proxy_external_ip</author>
     <author>nsg_organization</author>
     <author>nsg_name</author>
     <author>match_type</author>
@@ -505,107 +506,112 @@
         <t>Private Subnet CIDR for provisioning a VPC for the NSGv on AWS [default: ]</t>
       </text>
     </comment>
-    <comment authorId="28" ref="A39" shapeId="0">
+    <comment authorId="28" ref="A38" shapeId="0">
+      <text>
+        <t>IP address of the VNSUtil VM or the NUH used as a proxy for the NSGv on AWS [default: ]</t>
+      </text>
+    </comment>
+    <comment authorId="29" ref="A40" shapeId="0">
       <text>
         <t>Organization on the VSD to associate with the NSG being bootstrapped, overrides global setting. [default: ]</t>
       </text>
     </comment>
-    <comment authorId="29" ref="A40" shapeId="0">
+    <comment authorId="30" ref="A41" shapeId="0">
       <text>
         <t>Name of the NSG on the VSD [default: ]</t>
       </text>
     </comment>
-    <comment authorId="30" ref="A41" shapeId="0">
+    <comment authorId="31" ref="A42" shapeId="0">
       <text>
         <t>Field type to match against for NSGv activation. [default: none]</t>
       </text>
     </comment>
-    <comment authorId="31" ref="A42" shapeId="0">
+    <comment authorId="32" ref="A43" shapeId="0">
       <text>
         <t>Value to match against for NSGv activation. [default: ]</t>
       </text>
     </comment>
-    <comment authorId="32" ref="A43" shapeId="0">
+    <comment authorId="33" ref="A44" shapeId="0">
       <text>
         <t>Enables SSH on NSGv when set. [default: False]</t>
       </text>
     </comment>
-    <comment authorId="33" ref="A45" shapeId="0">
+    <comment authorId="34" ref="A46" shapeId="0">
       <text>
         <t>Name of the NSG infra profile template on the VSD [default: ]</t>
       </text>
     </comment>
-    <comment authorId="34" ref="A46" shapeId="0">
+    <comment authorId="35" ref="A47" shapeId="0">
       <text>
         <t>Name of the NSG infra profile on the VSD [default: ]</t>
       </text>
     </comment>
-    <comment authorId="35" ref="A47" shapeId="0">
+    <comment authorId="36" ref="A48" shapeId="0">
       <text>
         <t>Name of the NSG infra profile proxy DNS on the VSD [default: ]</t>
       </text>
     </comment>
-    <comment authorId="36" ref="A48" shapeId="0">
+    <comment authorId="37" ref="A49" shapeId="0">
       <text>
         <t>Allows NSGs using this profile to override SSH access. [default: False]</t>
       </text>
     </comment>
-    <comment authorId="37" ref="A50" shapeId="0">
+    <comment authorId="38" ref="A51" shapeId="0">
       <text>
         <t>Name of the VSC infra profile for the NSG on the VSD [default: ]</t>
       </text>
     </comment>
-    <comment authorId="38" ref="A51" shapeId="0">
+    <comment authorId="39" ref="A52" shapeId="0">
       <text>
         <t>Host name or IP address of the VSC infra profile first controller for the NSG [default: ]</t>
       </text>
     </comment>
-    <comment authorId="39" ref="A52" shapeId="0">
+    <comment authorId="40" ref="A53" shapeId="0">
       <text>
         <t>Host name or IP address of the VSC infra profile second controller for the NSG [default: ]</t>
       </text>
     </comment>
-    <comment authorId="40" ref="A53" shapeId="0">
+    <comment authorId="41" ref="A54" shapeId="0">
       <text>
         <t>Name of the network port for the NSG [default: ]</t>
       </text>
     </comment>
-    <comment authorId="41" ref="A55" shapeId="0">
+    <comment authorId="42" ref="A56" shapeId="0">
       <text>
         <t>Physical name of the network port for the NSG [default: port1]</t>
       </text>
     </comment>
-    <comment authorId="42" ref="A56" shapeId="0">
+    <comment authorId="43" ref="A57" shapeId="0">
       <text>
         <t>Name of the access port for the NSG. Deprecated in favor of access_ports [default: ]</t>
       </text>
     </comment>
-    <comment authorId="43" ref="A57" shapeId="0">
+    <comment authorId="44" ref="A58" shapeId="0">
       <text>
         <t>Physical name of the access port for the NSG. Deprecated in favor of access_ports [default: port2]</t>
       </text>
     </comment>
-    <comment authorId="44" ref="A58" shapeId="0">
+    <comment authorId="45" ref="A59" shapeId="0">
       <text>
         <t>VLAN range of the access port for the NSG. Deprecated in favor of access_ports [default: ]</t>
       </text>
     </comment>
-    <comment authorId="45" ref="A59" shapeId="0">
+    <comment authorId="46" ref="A60" shapeId="0">
       <text>
         <t>VLAN number of the NSG access port for the NSG. Deprecated in favor of access_ports [default: 0]</t>
       </text>
     </comment>
-    <comment authorId="46" ref="A60" shapeId="0">
+    <comment authorId="47" ref="A61" shapeId="0">
       <text>
         <t>Name of access ports list. (List items separated by comma.)</t>
       </text>
     </comment>
-    <comment authorId="47" ref="A62" shapeId="0">
+    <comment authorId="48" ref="A63" shapeId="0">
       <text>
         <t>The port for telnet to HV host to access NSGv serial or console terminal [default: 2300]</t>
       </text>
     </comment>
-    <comment authorId="48" ref="A63" shapeId="0">
+    <comment authorId="49" ref="A64" shapeId="0">
       <text>
         <t>Name of the credentials set for the vsd</t>
       </text>
@@ -4326,7 +4332,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G63"/>
+  <dimension ref="A1:G64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4764,29 +4770,29 @@
       <c r="G37" s="9" t="n"/>
     </row>
     <row r="38">
-      <c r="A38" s="3" t="inlineStr">
+      <c r="A38" s="8" t="inlineStr">
+        <is>
+          <t>Proxy IP Address</t>
+        </is>
+      </c>
+      <c r="B38" s="9" t="n"/>
+      <c r="C38" s="9" t="n"/>
+      <c r="D38" s="9" t="n"/>
+      <c r="E38" s="9" t="n"/>
+      <c r="F38" s="9" t="n"/>
+      <c r="G38" s="9" t="n"/>
+    </row>
+    <row r="39">
+      <c r="A39" s="3" t="inlineStr">
         <is>
           <t>NSGv Zero-Factor Bootstrap</t>
         </is>
       </c>
-    </row>
-    <row r="39">
-      <c r="A39" s="8" t="inlineStr">
-        <is>
-          <t>NSG Organization</t>
-        </is>
-      </c>
-      <c r="B39" s="9" t="n"/>
-      <c r="C39" s="9" t="n"/>
-      <c r="D39" s="9" t="n"/>
-      <c r="E39" s="9" t="n"/>
-      <c r="F39" s="9" t="n"/>
-      <c r="G39" s="9" t="n"/>
     </row>
     <row r="40">
       <c r="A40" s="8" t="inlineStr">
         <is>
-          <t>NSG Name</t>
+          <t>NSG Organization</t>
         </is>
       </c>
       <c r="B40" s="9" t="n"/>
@@ -4797,22 +4803,22 @@
       <c r="G40" s="9" t="n"/>
     </row>
     <row r="41">
-      <c r="A41" s="6" t="inlineStr">
-        <is>
-          <t>Activation Matching Type</t>
-        </is>
-      </c>
-      <c r="B41" s="7" t="n"/>
-      <c r="C41" s="7" t="n"/>
-      <c r="D41" s="7" t="n"/>
-      <c r="E41" s="7" t="n"/>
-      <c r="F41" s="7" t="n"/>
-      <c r="G41" s="7" t="n"/>
+      <c r="A41" s="8" t="inlineStr">
+        <is>
+          <t>NSG Name</t>
+        </is>
+      </c>
+      <c r="B41" s="9" t="n"/>
+      <c r="C41" s="9" t="n"/>
+      <c r="D41" s="9" t="n"/>
+      <c r="E41" s="9" t="n"/>
+      <c r="F41" s="9" t="n"/>
+      <c r="G41" s="9" t="n"/>
     </row>
     <row r="42">
       <c r="A42" s="6" t="inlineStr">
         <is>
-          <t>Activation Matching Value</t>
+          <t>Activation Matching Type</t>
         </is>
       </c>
       <c r="B42" s="7" t="n"/>
@@ -4823,42 +4829,42 @@
       <c r="G42" s="7" t="n"/>
     </row>
     <row r="43">
-      <c r="A43" s="8" t="inlineStr">
+      <c r="A43" s="6" t="inlineStr">
+        <is>
+          <t>Activation Matching Value</t>
+        </is>
+      </c>
+      <c r="B43" s="7" t="n"/>
+      <c r="C43" s="7" t="n"/>
+      <c r="D43" s="7" t="n"/>
+      <c r="E43" s="7" t="n"/>
+      <c r="F43" s="7" t="n"/>
+      <c r="G43" s="7" t="n"/>
+    </row>
+    <row r="44">
+      <c r="A44" s="8" t="inlineStr">
         <is>
           <t>Enable SSH on NSGv</t>
         </is>
       </c>
-      <c r="B43" s="9" t="n"/>
-      <c r="C43" s="9" t="n"/>
-      <c r="D43" s="9" t="n"/>
-      <c r="E43" s="9" t="n"/>
-      <c r="F43" s="9" t="n"/>
-      <c r="G43" s="9" t="n"/>
-    </row>
-    <row r="44">
-      <c r="A44" s="3" t="inlineStr">
+      <c r="B44" s="9" t="n"/>
+      <c r="C44" s="9" t="n"/>
+      <c r="D44" s="9" t="n"/>
+      <c r="E44" s="9" t="n"/>
+      <c r="F44" s="9" t="n"/>
+      <c r="G44" s="9" t="n"/>
+    </row>
+    <row r="45">
+      <c r="A45" s="3" t="inlineStr">
         <is>
           <t>NSG Advanced Options</t>
         </is>
       </c>
-    </row>
-    <row r="45">
-      <c r="A45" s="8" t="inlineStr">
-        <is>
-          <t>NSG Infra Profile Template Name</t>
-        </is>
-      </c>
-      <c r="B45" s="9" t="n"/>
-      <c r="C45" s="9" t="n"/>
-      <c r="D45" s="9" t="n"/>
-      <c r="E45" s="9" t="n"/>
-      <c r="F45" s="9" t="n"/>
-      <c r="G45" s="9" t="n"/>
     </row>
     <row r="46">
       <c r="A46" s="8" t="inlineStr">
         <is>
-          <t>NSG Infra Profile Name</t>
+          <t>NSG Infra Profile Template Name</t>
         </is>
       </c>
       <c r="B46" s="9" t="n"/>
@@ -4871,7 +4877,7 @@
     <row r="47">
       <c r="A47" s="8" t="inlineStr">
         <is>
-          <t>NSG Infra Profile Proxy DNS Name</t>
+          <t>NSG Infra Profile Name</t>
         </is>
       </c>
       <c r="B47" s="9" t="n"/>
@@ -4884,7 +4890,7 @@
     <row r="48">
       <c r="A48" s="8" t="inlineStr">
         <is>
-          <t>Allow SSH Access Override</t>
+          <t>NSG Infra Profile Proxy DNS Name</t>
         </is>
       </c>
       <c r="B48" s="9" t="n"/>
@@ -4895,29 +4901,29 @@
       <c r="G48" s="9" t="n"/>
     </row>
     <row r="49">
-      <c r="A49" s="3" t="inlineStr">
+      <c r="A49" s="8" t="inlineStr">
+        <is>
+          <t>Allow SSH Access Override</t>
+        </is>
+      </c>
+      <c r="B49" s="9" t="n"/>
+      <c r="C49" s="9" t="n"/>
+      <c r="D49" s="9" t="n"/>
+      <c r="E49" s="9" t="n"/>
+      <c r="F49" s="9" t="n"/>
+      <c r="G49" s="9" t="n"/>
+    </row>
+    <row r="50">
+      <c r="A50" s="3" t="inlineStr">
         <is>
           <t>VSC Info</t>
         </is>
       </c>
-    </row>
-    <row r="50">
-      <c r="A50" s="8" t="inlineStr">
-        <is>
-          <t>VSC Infra Profile Name</t>
-        </is>
-      </c>
-      <c r="B50" s="9" t="n"/>
-      <c r="C50" s="9" t="n"/>
-      <c r="D50" s="9" t="n"/>
-      <c r="E50" s="9" t="n"/>
-      <c r="F50" s="9" t="n"/>
-      <c r="G50" s="9" t="n"/>
     </row>
     <row r="51">
       <c r="A51" s="8" t="inlineStr">
         <is>
-          <t>VSC Infra Profile First Controller</t>
+          <t>VSC Infra Profile Name</t>
         </is>
       </c>
       <c r="B51" s="9" t="n"/>
@@ -4930,7 +4936,7 @@
     <row r="52">
       <c r="A52" s="8" t="inlineStr">
         <is>
-          <t>VSC Infra Profile Second Controller</t>
+          <t>VSC Infra Profile First Controller</t>
         </is>
       </c>
       <c r="B52" s="9" t="n"/>
@@ -4943,7 +4949,7 @@
     <row r="53">
       <c r="A53" s="8" t="inlineStr">
         <is>
-          <t>NSG Network Port Name</t>
+          <t>VSC Infra Profile Second Controller</t>
         </is>
       </c>
       <c r="B53" s="9" t="n"/>
@@ -4954,29 +4960,29 @@
       <c r="G53" s="9" t="n"/>
     </row>
     <row r="54">
-      <c r="A54" s="3" t="inlineStr">
+      <c r="A54" s="8" t="inlineStr">
+        <is>
+          <t>NSG Network Port Name</t>
+        </is>
+      </c>
+      <c r="B54" s="9" t="n"/>
+      <c r="C54" s="9" t="n"/>
+      <c r="D54" s="9" t="n"/>
+      <c r="E54" s="9" t="n"/>
+      <c r="F54" s="9" t="n"/>
+      <c r="G54" s="9" t="n"/>
+    </row>
+    <row r="55">
+      <c r="A55" s="3" t="inlineStr">
         <is>
           <t>Network and Access Ports</t>
         </is>
       </c>
-    </row>
-    <row r="55">
-      <c r="A55" s="8" t="inlineStr">
-        <is>
-          <t>NSG Network Port Physical Name</t>
-        </is>
-      </c>
-      <c r="B55" s="9" t="n"/>
-      <c r="C55" s="9" t="n"/>
-      <c r="D55" s="9" t="n"/>
-      <c r="E55" s="9" t="n"/>
-      <c r="F55" s="9" t="n"/>
-      <c r="G55" s="9" t="n"/>
     </row>
     <row r="56">
       <c r="A56" s="8" t="inlineStr">
         <is>
-          <t>NSG Access Port Name</t>
+          <t>NSG Network Port Physical Name</t>
         </is>
       </c>
       <c r="B56" s="9" t="n"/>
@@ -4989,7 +4995,7 @@
     <row r="57">
       <c r="A57" s="8" t="inlineStr">
         <is>
-          <t>NSG Access Port Physical Name</t>
+          <t>NSG Access Port Name</t>
         </is>
       </c>
       <c r="B57" s="9" t="n"/>
@@ -5002,7 +5008,7 @@
     <row r="58">
       <c r="A58" s="8" t="inlineStr">
         <is>
-          <t>NSG Access Port VLAN Range</t>
+          <t>NSG Access Port Physical Name</t>
         </is>
       </c>
       <c r="B58" s="9" t="n"/>
@@ -5015,7 +5021,7 @@
     <row r="59">
       <c r="A59" s="8" t="inlineStr">
         <is>
-          <t>NSG Access Port VLAN Number</t>
+          <t>NSG Access Port VLAN Range</t>
         </is>
       </c>
       <c r="B59" s="9" t="n"/>
@@ -5026,42 +5032,42 @@
       <c r="G59" s="9" t="n"/>
     </row>
     <row r="60">
-      <c r="A60" s="6" t="inlineStr">
+      <c r="A60" s="8" t="inlineStr">
+        <is>
+          <t>NSG Access Port VLAN Number</t>
+        </is>
+      </c>
+      <c r="B60" s="9" t="n"/>
+      <c r="C60" s="9" t="n"/>
+      <c r="D60" s="9" t="n"/>
+      <c r="E60" s="9" t="n"/>
+      <c r="F60" s="9" t="n"/>
+      <c r="G60" s="9" t="n"/>
+    </row>
+    <row r="61">
+      <c r="A61" s="6" t="inlineStr">
         <is>
           <t>NSGv Access ports list name</t>
         </is>
       </c>
-      <c r="B60" s="7" t="n"/>
-      <c r="C60" s="7" t="n"/>
-      <c r="D60" s="7" t="n"/>
-      <c r="E60" s="7" t="n"/>
-      <c r="F60" s="7" t="n"/>
-      <c r="G60" s="7" t="n"/>
-    </row>
-    <row r="61">
-      <c r="A61" s="3" t="inlineStr">
+      <c r="B61" s="7" t="n"/>
+      <c r="C61" s="7" t="n"/>
+      <c r="D61" s="7" t="n"/>
+      <c r="E61" s="7" t="n"/>
+      <c r="F61" s="7" t="n"/>
+      <c r="G61" s="7" t="n"/>
+    </row>
+    <row r="62">
+      <c r="A62" s="3" t="inlineStr">
         <is>
           <t>Telnet and Credentials</t>
         </is>
       </c>
-    </row>
-    <row r="62">
-      <c r="A62" s="8" t="inlineStr">
-        <is>
-          <t>Telnet port for console</t>
-        </is>
-      </c>
-      <c r="B62" s="9" t="n"/>
-      <c r="C62" s="9" t="n"/>
-      <c r="D62" s="9" t="n"/>
-      <c r="E62" s="9" t="n"/>
-      <c r="F62" s="9" t="n"/>
-      <c r="G62" s="9" t="n"/>
     </row>
     <row r="63">
       <c r="A63" s="8" t="inlineStr">
         <is>
-          <t>Credentials set name</t>
+          <t>Telnet port for console</t>
         </is>
       </c>
       <c r="B63" s="9" t="n"/>
@@ -5070,6 +5076,19 @@
       <c r="E63" s="9" t="n"/>
       <c r="F63" s="9" t="n"/>
       <c r="G63" s="9" t="n"/>
+    </row>
+    <row r="64">
+      <c r="A64" s="8" t="inlineStr">
+        <is>
+          <t>Credentials set name</t>
+        </is>
+      </c>
+      <c r="B64" s="9" t="n"/>
+      <c r="C64" s="9" t="n"/>
+      <c r="D64" s="9" t="n"/>
+      <c r="E64" s="9" t="n"/>
+      <c r="F64" s="9" t="n"/>
+      <c r="G64" s="9" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -5079,11 +5098,11 @@
     <mergeCell ref="A18:G18"/>
     <mergeCell ref="A24:G24"/>
     <mergeCell ref="A33:G33"/>
-    <mergeCell ref="A38:G38"/>
-    <mergeCell ref="A44:G44"/>
-    <mergeCell ref="A49:G49"/>
-    <mergeCell ref="A54:G54"/>
-    <mergeCell ref="A61:G61"/>
+    <mergeCell ref="A39:G39"/>
+    <mergeCell ref="A45:G45"/>
+    <mergeCell ref="A50:G50"/>
+    <mergeCell ref="A55:G55"/>
+    <mergeCell ref="A62:G62"/>
   </mergeCells>
   <dataValidations count="42">
     <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="B6" type="list">
@@ -5122,72 +5141,72 @@
     <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="G9" type="list">
       <formula1>"none,zfb_metro,zfb_external,activation_link"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="B41" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="B42" type="list">
       <formula1>"none,hostname,ip_address,mac_address,nsgateway_id,serial_number,uuid"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="C41" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="C42" type="list">
       <formula1>"none,hostname,ip_address,mac_address,nsgateway_id,serial_number,uuid"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="D41" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="D42" type="list">
       <formula1>"none,hostname,ip_address,mac_address,nsgateway_id,serial_number,uuid"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="E41" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="E42" type="list">
       <formula1>"none,hostname,ip_address,mac_address,nsgateway_id,serial_number,uuid"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="F41" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="F42" type="list">
       <formula1>"none,hostname,ip_address,mac_address,nsgateway_id,serial_number,uuid"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="G41" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="G42" type="list">
       <formula1>"none,hostname,ip_address,mac_address,nsgateway_id,serial_number,uuid"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="B43" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="B44" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="C43" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="C44" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="D43" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="D44" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="E43" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="E44" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="F43" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="F44" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="G43" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="G44" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="B48" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="B49" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="C48" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="C49" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="D48" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="D49" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="E48" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="E49" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="F48" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="F49" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="G48" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="G49" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B59" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="C59" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="D59" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="E59" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="F59" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="G59" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B62" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="C62" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="D62" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="E62" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="F62" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="G62" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B60" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="C60" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="D60" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="E60" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="F60" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="G60" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B63" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="C63" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="D63" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="E63" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="F63" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="G63" type="whole"/>
   </dataValidations>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <legacyDrawing r:id="anysvml"/>

</xml_diff>

<commit_message>
Adding variable cpu cores to nsgv
</commit_message>
<xml_diff>
--- a/examples/excel/active_standby_vsds.xlsx
+++ b/examples/excel/active_standby_vsds.xlsx
@@ -317,6 +317,7 @@
     <author>vmname</author>
     <author>target_server_type</author>
     <author>target_server</author>
+    <author>cpu_cores</author>
     <author>bootstrap_method</author>
     <author>iso_path</author>
     <author>iso_file</author>
@@ -380,232 +381,237 @@
         <t>Hostname or IP address of the hypervisor or vCenter server where the NSGv will be instantiated</t>
       </text>
     </comment>
-    <comment authorId="3" ref="A9" shapeId="0">
+    <comment authorId="3" ref="A8" shapeId="0">
+      <text>
+        <t>Number of CPU cores to defined for the VM</t>
+      </text>
+    </comment>
+    <comment authorId="4" ref="A10" shapeId="0">
       <text>
         <t>Bootstrap method for the NSGv. The default is 'none' which means no bootstrap will be performed. 'zfb_metro' creates a boostrap ISO file based on the contents of the file nsgv_bootstrap.yml. 'zfb_external' is used when a 3rd-party ISO file is to be used. [default: none]</t>
       </text>
     </comment>
-    <comment authorId="4" ref="A10" shapeId="0">
+    <comment authorId="5" ref="A11" shapeId="0">
       <text>
         <t>Local path to the 3rd-party ISO file to use for bootstrap. Only required when bootstrap_method id set to 'zfb_external'</t>
       </text>
     </comment>
-    <comment authorId="5" ref="A11" shapeId="0">
+    <comment authorId="6" ref="A12" shapeId="0">
       <text>
         <t>Name of the 3rd-party ISO file to use for bootstrap. Only required when bootstrap_method id set to 'zfb_external'</t>
       </text>
     </comment>
-    <comment authorId="6" ref="A12" shapeId="0">
+    <comment authorId="7" ref="A13" shapeId="0">
       <text>
         <t xml:space="preserve"> [default: ]</t>
       </text>
     </comment>
-    <comment authorId="7" ref="A13" shapeId="0">
+    <comment authorId="8" ref="A14" shapeId="0">
       <text>
         <t>MAC address the proxy will use to recognize the NSGV at boot/DHCP time. Only required when bootstrap_method is set to 'zfb_metro'</t>
       </text>
     </comment>
-    <comment authorId="8" ref="A15" shapeId="0">
+    <comment authorId="9" ref="A16" shapeId="0">
       <text>
         <t>Network Bridge used for the management path of this component. This will be a Distributed Virtual PortGroup (DVPG) when deploying on vCenter or a Linux network bridge. [default: (global Bridge interface)]</t>
       </text>
     </comment>
-    <comment authorId="9" ref="A16" shapeId="0">
+    <comment authorId="10" ref="A17" shapeId="0">
       <text>
         <t>Network Bridge used for the data path of this component. This will be a Distributed Virtual PortGroup (DVPG) when deploying on vCenter or a Linux network bridge. [default: (global Bridge interface)]</t>
       </text>
     </comment>
-    <comment authorId="10" ref="A17" shapeId="0">
+    <comment authorId="11" ref="A18" shapeId="0">
       <text>
         <t>Network bridge used for the access network when installing an NSGv. This will be a Distributed Virtual PortGroup (DVPG) when deploying on vCenter or a Linux network bridge [default: (global Bridge interface)]</t>
       </text>
     </comment>
-    <comment authorId="11" ref="A19" shapeId="0">
+    <comment authorId="12" ref="A20" shapeId="0">
       <text>
         <t>Name of the vCenter Datacenter on which the NSG VM will be deployed. Defaults to the common vCenter Datacenter Name if not defined here. [default: (global vCenter Datacenter Name)]</t>
       </text>
     </comment>
-    <comment authorId="12" ref="A20" shapeId="0">
+    <comment authorId="13" ref="A21" shapeId="0">
       <text>
         <t>Name of the vCenter Cluster on which the NSG VM will be deployed. Defaults to the common vCenter Cluster Name if not defined here. [default: (global vCenter Cluster Name)]</t>
       </text>
     </comment>
-    <comment authorId="13" ref="A21" shapeId="0">
+    <comment authorId="14" ref="A22" shapeId="0">
       <text>
         <t>Requires ovftool 4.3. Reference to the host on the vCenter cluster on which to deploy Nuage components [default: (global vCenter Host Reference)]</t>
       </text>
     </comment>
-    <comment authorId="14" ref="A22" shapeId="0">
+    <comment authorId="15" ref="A23" shapeId="0">
       <text>
         <t>Name of the vCenter Datastore on which the NSG VM will be deployed. Defaults to the common vCenter Datastore Name if not defined here. [default: (global vCenter Datastore Name)]</t>
       </text>
     </comment>
-    <comment authorId="15" ref="A23" shapeId="0">
+    <comment authorId="16" ref="A24" shapeId="0">
       <text>
         <t>Optional path to a hosts and clusters folder defined on vCenter where VM will be instantiated</t>
       </text>
     </comment>
-    <comment authorId="16" ref="A25" shapeId="0">
+    <comment authorId="17" ref="A26" shapeId="0">
       <text>
         <t>AWS Region</t>
       </text>
     </comment>
-    <comment authorId="17" ref="A26" shapeId="0">
+    <comment authorId="18" ref="A27" shapeId="0">
       <text>
         <t>AMI ID for AWS instance</t>
       </text>
     </comment>
-    <comment authorId="18" ref="A27" shapeId="0">
+    <comment authorId="19" ref="A28" shapeId="0">
       <text>
         <t>AMI ID of the upgraded image</t>
       </text>
     </comment>
-    <comment authorId="19" ref="A28" shapeId="0">
+    <comment authorId="20" ref="A29" shapeId="0">
       <text>
         <t>Instance Type of the AWS Instance</t>
       </text>
     </comment>
-    <comment authorId="20" ref="A29" shapeId="0">
+    <comment authorId="21" ref="A30" shapeId="0">
       <text>
         <t>Name of the Keypair used to connect to VPC</t>
       </text>
     </comment>
-    <comment authorId="21" ref="A30" shapeId="0">
+    <comment authorId="22" ref="A31" shapeId="0">
       <text>
         <t>ENI for Access Subnetwork</t>
       </text>
     </comment>
-    <comment authorId="22" ref="A31" shapeId="0">
+    <comment authorId="23" ref="A32" shapeId="0">
       <text>
         <t>ENI for Access Subnetwork</t>
       </text>
     </comment>
-    <comment authorId="23" ref="A32" shapeId="0">
+    <comment authorId="24" ref="A33" shapeId="0">
       <text>
         <t>AWS WAN EIP AllocID</t>
       </text>
     </comment>
-    <comment authorId="24" ref="A34" shapeId="0">
+    <comment authorId="25" ref="A35" shapeId="0">
       <text>
         <t>CIDR for provisioning a VPC for the NSGv on AWS [default: ]</t>
       </text>
     </comment>
-    <comment authorId="25" ref="A35" shapeId="0">
+    <comment authorId="26" ref="A36" shapeId="0">
       <text>
         <t>WAN Subnet CIDR for provisioning a VPC for the NSGv on AWS [default: ]</t>
       </text>
     </comment>
-    <comment authorId="26" ref="A36" shapeId="0">
+    <comment authorId="27" ref="A37" shapeId="0">
       <text>
         <t>LAN Subnet CIDR for provisioning a VPC for the NSGv on AWS [default: ]</t>
       </text>
     </comment>
-    <comment authorId="27" ref="A37" shapeId="0">
+    <comment authorId="28" ref="A38" shapeId="0">
       <text>
         <t>Private Subnet CIDR for provisioning a VPC for the NSGv on AWS [default: ]</t>
       </text>
     </comment>
-    <comment authorId="28" ref="A39" shapeId="0">
+    <comment authorId="29" ref="A40" shapeId="0">
       <text>
         <t>Organization on the VSD to associate with the NSG being bootstrapped, overrides global setting. [default: ]</t>
       </text>
     </comment>
-    <comment authorId="29" ref="A40" shapeId="0">
+    <comment authorId="30" ref="A41" shapeId="0">
       <text>
         <t>Name of the NSG on the VSD [default: ]</t>
       </text>
     </comment>
-    <comment authorId="30" ref="A41" shapeId="0">
+    <comment authorId="31" ref="A42" shapeId="0">
       <text>
         <t>Field type to match against for NSGv activation. [default: none]</t>
       </text>
     </comment>
-    <comment authorId="31" ref="A42" shapeId="0">
+    <comment authorId="32" ref="A43" shapeId="0">
       <text>
         <t>Value to match against for NSGv activation. [default: ]</t>
       </text>
     </comment>
-    <comment authorId="32" ref="A43" shapeId="0">
+    <comment authorId="33" ref="A44" shapeId="0">
       <text>
         <t>Enables SSH on NSGv when set. [default: False]</t>
       </text>
     </comment>
-    <comment authorId="33" ref="A45" shapeId="0">
+    <comment authorId="34" ref="A46" shapeId="0">
       <text>
         <t>Name of the NSG infra profile template on the VSD [default: ]</t>
       </text>
     </comment>
-    <comment authorId="34" ref="A46" shapeId="0">
+    <comment authorId="35" ref="A47" shapeId="0">
       <text>
         <t>Name of the NSG infra profile on the VSD [default: ]</t>
       </text>
     </comment>
-    <comment authorId="35" ref="A47" shapeId="0">
+    <comment authorId="36" ref="A48" shapeId="0">
       <text>
         <t>Name of the NSG infra profile proxy DNS on the VSD [default: ]</t>
       </text>
     </comment>
-    <comment authorId="36" ref="A48" shapeId="0">
+    <comment authorId="37" ref="A49" shapeId="0">
       <text>
         <t>Allows NSGs using this profile to override SSH access. [default: False]</t>
       </text>
     </comment>
-    <comment authorId="37" ref="A50" shapeId="0">
+    <comment authorId="38" ref="A51" shapeId="0">
       <text>
         <t>Name of the VSC infra profile for the NSG on the VSD [default: ]</t>
       </text>
     </comment>
-    <comment authorId="38" ref="A51" shapeId="0">
+    <comment authorId="39" ref="A52" shapeId="0">
       <text>
         <t>Host name or IP address of the VSC infra profile first controller for the NSG [default: ]</t>
       </text>
     </comment>
-    <comment authorId="39" ref="A52" shapeId="0">
+    <comment authorId="40" ref="A53" shapeId="0">
       <text>
         <t>Host name or IP address of the VSC infra profile second controller for the NSG [default: ]</t>
       </text>
     </comment>
-    <comment authorId="40" ref="A53" shapeId="0">
+    <comment authorId="41" ref="A54" shapeId="0">
       <text>
         <t>Name of the network port for the NSG [default: ]</t>
       </text>
     </comment>
-    <comment authorId="41" ref="A55" shapeId="0">
+    <comment authorId="42" ref="A56" shapeId="0">
       <text>
         <t>Physical name of the network port for the NSG [default: port1]</t>
       </text>
     </comment>
-    <comment authorId="42" ref="A56" shapeId="0">
+    <comment authorId="43" ref="A57" shapeId="0">
       <text>
         <t>Name of the access port for the NSG. Deprecated in favor of access_ports [default: ]</t>
       </text>
     </comment>
-    <comment authorId="43" ref="A57" shapeId="0">
+    <comment authorId="44" ref="A58" shapeId="0">
       <text>
         <t>Physical name of the access port for the NSG. Deprecated in favor of access_ports [default: port2]</t>
       </text>
     </comment>
-    <comment authorId="44" ref="A58" shapeId="0">
+    <comment authorId="45" ref="A59" shapeId="0">
       <text>
         <t>VLAN range of the access port for the NSG. Deprecated in favor of access_ports [default: ]</t>
       </text>
     </comment>
-    <comment authorId="45" ref="A59" shapeId="0">
+    <comment authorId="46" ref="A60" shapeId="0">
       <text>
         <t>VLAN number of the NSG access port for the NSG. Deprecated in favor of access_ports [default: 0]</t>
       </text>
     </comment>
-    <comment authorId="46" ref="A60" shapeId="0">
+    <comment authorId="47" ref="A61" shapeId="0">
       <text>
         <t>Name of access ports list. (List items separated by comma.)</t>
       </text>
     </comment>
-    <comment authorId="47" ref="A62" shapeId="0">
+    <comment authorId="48" ref="A63" shapeId="0">
       <text>
         <t>The port for telnet to HV host to access NSGv serial or console terminal [default: 2300]</t>
       </text>
     </comment>
-    <comment authorId="48" ref="A63" shapeId="0">
+    <comment authorId="49" ref="A64" shapeId="0">
       <text>
         <t>Name of the credentials set for the vsd</t>
       </text>
@@ -4332,7 +4338,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G63"/>
+  <dimension ref="A1:G64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4410,29 +4416,29 @@
       <c r="G7" s="5" t="n"/>
     </row>
     <row r="8">
-      <c r="A8" s="3" t="inlineStr">
+      <c r="A8" s="6" t="inlineStr">
+        <is>
+          <t>Number of CPU cores</t>
+        </is>
+      </c>
+      <c r="B8" s="7" t="n"/>
+      <c r="C8" s="7" t="n"/>
+      <c r="D8" s="7" t="n"/>
+      <c r="E8" s="7" t="n"/>
+      <c r="F8" s="7" t="n"/>
+      <c r="G8" s="7" t="n"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="3" t="inlineStr">
         <is>
           <t>Bootstrap Parameters</t>
         </is>
       </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="6" t="inlineStr">
-        <is>
-          <t>Bootstrap Method</t>
-        </is>
-      </c>
-      <c r="B9" s="7" t="n"/>
-      <c r="C9" s="7" t="n"/>
-      <c r="D9" s="7" t="n"/>
-      <c r="E9" s="7" t="n"/>
-      <c r="F9" s="7" t="n"/>
-      <c r="G9" s="7" t="n"/>
     </row>
     <row r="10">
       <c r="A10" s="6" t="inlineStr">
         <is>
-          <t>External Bootstrap ISO File Directory</t>
+          <t>Bootstrap Method</t>
         </is>
       </c>
       <c r="B10" s="7" t="n"/>
@@ -4445,7 +4451,7 @@
     <row r="11">
       <c r="A11" s="6" t="inlineStr">
         <is>
-          <t>External Bootstrap ISO File Name</t>
+          <t>External Bootstrap ISO File Directory</t>
         </is>
       </c>
       <c r="B11" s="7" t="n"/>
@@ -4458,7 +4464,7 @@
     <row r="12">
       <c r="A12" s="6" t="inlineStr">
         <is>
-          <t>IP Address to assign to NSGv by VNSUtil</t>
+          <t>External Bootstrap ISO File Name</t>
         </is>
       </c>
       <c r="B12" s="7" t="n"/>
@@ -4471,7 +4477,7 @@
     <row r="13">
       <c r="A13" s="6" t="inlineStr">
         <is>
-          <t>NSGV MAC Address</t>
+          <t>IP Address to assign to NSGv by VNSUtil</t>
         </is>
       </c>
       <c r="B13" s="7" t="n"/>
@@ -4482,29 +4488,29 @@
       <c r="G13" s="7" t="n"/>
     </row>
     <row r="14">
-      <c r="A14" s="3" t="inlineStr">
+      <c r="A14" s="6" t="inlineStr">
+        <is>
+          <t>NSGV MAC Address</t>
+        </is>
+      </c>
+      <c r="B14" s="7" t="n"/>
+      <c r="C14" s="7" t="n"/>
+      <c r="D14" s="7" t="n"/>
+      <c r="E14" s="7" t="n"/>
+      <c r="F14" s="7" t="n"/>
+      <c r="G14" s="7" t="n"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="3" t="inlineStr">
         <is>
           <t>Bridge info</t>
         </is>
       </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="8" t="inlineStr">
-        <is>
-          <t>Management Network Bridge</t>
-        </is>
-      </c>
-      <c r="B15" s="9" t="n"/>
-      <c r="C15" s="9" t="n"/>
-      <c r="D15" s="9" t="n"/>
-      <c r="E15" s="9" t="n"/>
-      <c r="F15" s="9" t="n"/>
-      <c r="G15" s="9" t="n"/>
     </row>
     <row r="16">
       <c r="A16" s="8" t="inlineStr">
         <is>
-          <t>Data Network Bridge</t>
+          <t>Management Network Bridge</t>
         </is>
       </c>
       <c r="B16" s="9" t="n"/>
@@ -4515,42 +4521,42 @@
       <c r="G16" s="9" t="n"/>
     </row>
     <row r="17">
-      <c r="A17" s="6" t="inlineStr">
+      <c r="A17" s="8" t="inlineStr">
+        <is>
+          <t>Data Network Bridge</t>
+        </is>
+      </c>
+      <c r="B17" s="9" t="n"/>
+      <c r="C17" s="9" t="n"/>
+      <c r="D17" s="9" t="n"/>
+      <c r="E17" s="9" t="n"/>
+      <c r="F17" s="9" t="n"/>
+      <c r="G17" s="9" t="n"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="6" t="inlineStr">
         <is>
           <t>NSGv Access Bridge</t>
         </is>
       </c>
-      <c r="B17" s="7" t="n"/>
-      <c r="C17" s="7" t="n"/>
-      <c r="D17" s="7" t="n"/>
-      <c r="E17" s="7" t="n"/>
-      <c r="F17" s="7" t="n"/>
-      <c r="G17" s="7" t="n"/>
-    </row>
-    <row r="18">
-      <c r="A18" s="3" t="inlineStr">
+      <c r="B18" s="7" t="n"/>
+      <c r="C18" s="7" t="n"/>
+      <c r="D18" s="7" t="n"/>
+      <c r="E18" s="7" t="n"/>
+      <c r="F18" s="7" t="n"/>
+      <c r="G18" s="7" t="n"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="3" t="inlineStr">
         <is>
           <t>vCenter Parameters</t>
         </is>
       </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="8" t="inlineStr">
-        <is>
-          <t>vCenter Datacenter Name</t>
-        </is>
-      </c>
-      <c r="B19" s="9" t="n"/>
-      <c r="C19" s="9" t="n"/>
-      <c r="D19" s="9" t="n"/>
-      <c r="E19" s="9" t="n"/>
-      <c r="F19" s="9" t="n"/>
-      <c r="G19" s="9" t="n"/>
     </row>
     <row r="20">
       <c r="A20" s="8" t="inlineStr">
         <is>
-          <t>vCenter Cluster Name</t>
+          <t>vCenter Datacenter Name</t>
         </is>
       </c>
       <c r="B20" s="9" t="n"/>
@@ -4563,7 +4569,7 @@
     <row r="21">
       <c r="A21" s="8" t="inlineStr">
         <is>
-          <t>vCenter Host Reference</t>
+          <t>vCenter Cluster Name</t>
         </is>
       </c>
       <c r="B21" s="9" t="n"/>
@@ -4576,7 +4582,7 @@
     <row r="22">
       <c r="A22" s="8" t="inlineStr">
         <is>
-          <t>vCenter Datastore Name</t>
+          <t>vCenter Host Reference</t>
         </is>
       </c>
       <c r="B22" s="9" t="n"/>
@@ -4589,7 +4595,7 @@
     <row r="23">
       <c r="A23" s="8" t="inlineStr">
         <is>
-          <t>vCenter Hosts and Clusters Folder</t>
+          <t>vCenter Datastore Name</t>
         </is>
       </c>
       <c r="B23" s="9" t="n"/>
@@ -4600,29 +4606,29 @@
       <c r="G23" s="9" t="n"/>
     </row>
     <row r="24">
-      <c r="A24" s="3" t="inlineStr">
+      <c r="A24" s="8" t="inlineStr">
+        <is>
+          <t>vCenter Hosts and Clusters Folder</t>
+        </is>
+      </c>
+      <c r="B24" s="9" t="n"/>
+      <c r="C24" s="9" t="n"/>
+      <c r="D24" s="9" t="n"/>
+      <c r="E24" s="9" t="n"/>
+      <c r="F24" s="9" t="n"/>
+      <c r="G24" s="9" t="n"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="3" t="inlineStr">
         <is>
           <t>AWS Parameters</t>
         </is>
       </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="6" t="inlineStr">
-        <is>
-          <t>AWS Region</t>
-        </is>
-      </c>
-      <c r="B25" s="7" t="n"/>
-      <c r="C25" s="7" t="n"/>
-      <c r="D25" s="7" t="n"/>
-      <c r="E25" s="7" t="n"/>
-      <c r="F25" s="7" t="n"/>
-      <c r="G25" s="7" t="n"/>
     </row>
     <row r="26">
       <c r="A26" s="6" t="inlineStr">
         <is>
-          <t>AWS AMI ID</t>
+          <t>AWS Region</t>
         </is>
       </c>
       <c r="B26" s="7" t="n"/>
@@ -4635,7 +4641,7 @@
     <row r="27">
       <c r="A27" s="6" t="inlineStr">
         <is>
-          <t>AWS AMI ID for Upgrading Instance</t>
+          <t>AWS AMI ID</t>
         </is>
       </c>
       <c r="B27" s="7" t="n"/>
@@ -4648,7 +4654,7 @@
     <row r="28">
       <c r="A28" s="6" t="inlineStr">
         <is>
-          <t>AWS Instance Type</t>
+          <t>AWS AMI ID for Upgrading Instance</t>
         </is>
       </c>
       <c r="B28" s="7" t="n"/>
@@ -4661,7 +4667,7 @@
     <row r="29">
       <c r="A29" s="6" t="inlineStr">
         <is>
-          <t>AWS Keypair Name</t>
+          <t>AWS Instance Type</t>
         </is>
       </c>
       <c r="B29" s="7" t="n"/>
@@ -4674,7 +4680,7 @@
     <row r="30">
       <c r="A30" s="6" t="inlineStr">
         <is>
-          <t>AWS Access ENI</t>
+          <t>AWS Keypair Name</t>
         </is>
       </c>
       <c r="B30" s="7" t="n"/>
@@ -4687,7 +4693,7 @@
     <row r="31">
       <c r="A31" s="6" t="inlineStr">
         <is>
-          <t>AWS Data ENI</t>
+          <t>AWS Access ENI</t>
         </is>
       </c>
       <c r="B31" s="7" t="n"/>
@@ -4700,7 +4706,7 @@
     <row r="32">
       <c r="A32" s="6" t="inlineStr">
         <is>
-          <t>AWS WAN EIP AllocID</t>
+          <t>AWS Data ENI</t>
         </is>
       </c>
       <c r="B32" s="7" t="n"/>
@@ -4711,29 +4717,29 @@
       <c r="G32" s="7" t="n"/>
     </row>
     <row r="33">
-      <c r="A33" s="3" t="inlineStr">
+      <c r="A33" s="6" t="inlineStr">
+        <is>
+          <t>AWS WAN EIP AllocID</t>
+        </is>
+      </c>
+      <c r="B33" s="7" t="n"/>
+      <c r="C33" s="7" t="n"/>
+      <c r="D33" s="7" t="n"/>
+      <c r="E33" s="7" t="n"/>
+      <c r="F33" s="7" t="n"/>
+      <c r="G33" s="7" t="n"/>
+    </row>
+    <row r="34">
+      <c r="A34" s="3" t="inlineStr">
         <is>
           <t>AWS VPC Parameters</t>
         </is>
       </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="8" t="inlineStr">
-        <is>
-          <t>AWS Provision VPC CIDR</t>
-        </is>
-      </c>
-      <c r="B34" s="9" t="n"/>
-      <c r="C34" s="9" t="n"/>
-      <c r="D34" s="9" t="n"/>
-      <c r="E34" s="9" t="n"/>
-      <c r="F34" s="9" t="n"/>
-      <c r="G34" s="9" t="n"/>
     </row>
     <row r="35">
       <c r="A35" s="8" t="inlineStr">
         <is>
-          <t>AWS Provision VPC NSG WAN Subnet CIDR</t>
+          <t>AWS Provision VPC CIDR</t>
         </is>
       </c>
       <c r="B35" s="9" t="n"/>
@@ -4746,7 +4752,7 @@
     <row r="36">
       <c r="A36" s="8" t="inlineStr">
         <is>
-          <t>AWS Provision VPC NSG LAN Subnet CIDR</t>
+          <t>AWS Provision VPC NSG WAN Subnet CIDR</t>
         </is>
       </c>
       <c r="B36" s="9" t="n"/>
@@ -4759,7 +4765,7 @@
     <row r="37">
       <c r="A37" s="8" t="inlineStr">
         <is>
-          <t>AWS Provision VPC Private Subnet CIDR</t>
+          <t>AWS Provision VPC NSG LAN Subnet CIDR</t>
         </is>
       </c>
       <c r="B37" s="9" t="n"/>
@@ -4770,29 +4776,29 @@
       <c r="G37" s="9" t="n"/>
     </row>
     <row r="38">
-      <c r="A38" s="3" t="inlineStr">
+      <c r="A38" s="8" t="inlineStr">
+        <is>
+          <t>AWS Provision VPC Private Subnet CIDR</t>
+        </is>
+      </c>
+      <c r="B38" s="9" t="n"/>
+      <c r="C38" s="9" t="n"/>
+      <c r="D38" s="9" t="n"/>
+      <c r="E38" s="9" t="n"/>
+      <c r="F38" s="9" t="n"/>
+      <c r="G38" s="9" t="n"/>
+    </row>
+    <row r="39">
+      <c r="A39" s="3" t="inlineStr">
         <is>
           <t>NSGv Zero-Factor Bootstrap</t>
         </is>
       </c>
-    </row>
-    <row r="39">
-      <c r="A39" s="8" t="inlineStr">
-        <is>
-          <t>NSG Organization</t>
-        </is>
-      </c>
-      <c r="B39" s="9" t="n"/>
-      <c r="C39" s="9" t="n"/>
-      <c r="D39" s="9" t="n"/>
-      <c r="E39" s="9" t="n"/>
-      <c r="F39" s="9" t="n"/>
-      <c r="G39" s="9" t="n"/>
     </row>
     <row r="40">
       <c r="A40" s="8" t="inlineStr">
         <is>
-          <t>NSG Name</t>
+          <t>NSG Organization</t>
         </is>
       </c>
       <c r="B40" s="9" t="n"/>
@@ -4803,22 +4809,22 @@
       <c r="G40" s="9" t="n"/>
     </row>
     <row r="41">
-      <c r="A41" s="6" t="inlineStr">
-        <is>
-          <t>Activation Matching Type</t>
-        </is>
-      </c>
-      <c r="B41" s="7" t="n"/>
-      <c r="C41" s="7" t="n"/>
-      <c r="D41" s="7" t="n"/>
-      <c r="E41" s="7" t="n"/>
-      <c r="F41" s="7" t="n"/>
-      <c r="G41" s="7" t="n"/>
+      <c r="A41" s="8" t="inlineStr">
+        <is>
+          <t>NSG Name</t>
+        </is>
+      </c>
+      <c r="B41" s="9" t="n"/>
+      <c r="C41" s="9" t="n"/>
+      <c r="D41" s="9" t="n"/>
+      <c r="E41" s="9" t="n"/>
+      <c r="F41" s="9" t="n"/>
+      <c r="G41" s="9" t="n"/>
     </row>
     <row r="42">
       <c r="A42" s="6" t="inlineStr">
         <is>
-          <t>Activation Matching Value</t>
+          <t>Activation Matching Type</t>
         </is>
       </c>
       <c r="B42" s="7" t="n"/>
@@ -4829,42 +4835,42 @@
       <c r="G42" s="7" t="n"/>
     </row>
     <row r="43">
-      <c r="A43" s="8" t="inlineStr">
+      <c r="A43" s="6" t="inlineStr">
+        <is>
+          <t>Activation Matching Value</t>
+        </is>
+      </c>
+      <c r="B43" s="7" t="n"/>
+      <c r="C43" s="7" t="n"/>
+      <c r="D43" s="7" t="n"/>
+      <c r="E43" s="7" t="n"/>
+      <c r="F43" s="7" t="n"/>
+      <c r="G43" s="7" t="n"/>
+    </row>
+    <row r="44">
+      <c r="A44" s="8" t="inlineStr">
         <is>
           <t>Enable SSH on NSGv</t>
         </is>
       </c>
-      <c r="B43" s="9" t="n"/>
-      <c r="C43" s="9" t="n"/>
-      <c r="D43" s="9" t="n"/>
-      <c r="E43" s="9" t="n"/>
-      <c r="F43" s="9" t="n"/>
-      <c r="G43" s="9" t="n"/>
-    </row>
-    <row r="44">
-      <c r="A44" s="3" t="inlineStr">
+      <c r="B44" s="9" t="n"/>
+      <c r="C44" s="9" t="n"/>
+      <c r="D44" s="9" t="n"/>
+      <c r="E44" s="9" t="n"/>
+      <c r="F44" s="9" t="n"/>
+      <c r="G44" s="9" t="n"/>
+    </row>
+    <row r="45">
+      <c r="A45" s="3" t="inlineStr">
         <is>
           <t>NSG Advanced Options</t>
         </is>
       </c>
-    </row>
-    <row r="45">
-      <c r="A45" s="8" t="inlineStr">
-        <is>
-          <t>NSG Infra Profile Template Name</t>
-        </is>
-      </c>
-      <c r="B45" s="9" t="n"/>
-      <c r="C45" s="9" t="n"/>
-      <c r="D45" s="9" t="n"/>
-      <c r="E45" s="9" t="n"/>
-      <c r="F45" s="9" t="n"/>
-      <c r="G45" s="9" t="n"/>
     </row>
     <row r="46">
       <c r="A46" s="8" t="inlineStr">
         <is>
-          <t>NSG Infra Profile Name</t>
+          <t>NSG Infra Profile Template Name</t>
         </is>
       </c>
       <c r="B46" s="9" t="n"/>
@@ -4877,7 +4883,7 @@
     <row r="47">
       <c r="A47" s="8" t="inlineStr">
         <is>
-          <t>NSG Infra Profile Proxy DNS Name</t>
+          <t>NSG Infra Profile Name</t>
         </is>
       </c>
       <c r="B47" s="9" t="n"/>
@@ -4890,7 +4896,7 @@
     <row r="48">
       <c r="A48" s="8" t="inlineStr">
         <is>
-          <t>Allow SSH Access Override</t>
+          <t>NSG Infra Profile Proxy DNS Name</t>
         </is>
       </c>
       <c r="B48" s="9" t="n"/>
@@ -4901,29 +4907,29 @@
       <c r="G48" s="9" t="n"/>
     </row>
     <row r="49">
-      <c r="A49" s="3" t="inlineStr">
+      <c r="A49" s="8" t="inlineStr">
+        <is>
+          <t>Allow SSH Access Override</t>
+        </is>
+      </c>
+      <c r="B49" s="9" t="n"/>
+      <c r="C49" s="9" t="n"/>
+      <c r="D49" s="9" t="n"/>
+      <c r="E49" s="9" t="n"/>
+      <c r="F49" s="9" t="n"/>
+      <c r="G49" s="9" t="n"/>
+    </row>
+    <row r="50">
+      <c r="A50" s="3" t="inlineStr">
         <is>
           <t>VSC Info</t>
         </is>
       </c>
-    </row>
-    <row r="50">
-      <c r="A50" s="8" t="inlineStr">
-        <is>
-          <t>VSC Infra Profile Name</t>
-        </is>
-      </c>
-      <c r="B50" s="9" t="n"/>
-      <c r="C50" s="9" t="n"/>
-      <c r="D50" s="9" t="n"/>
-      <c r="E50" s="9" t="n"/>
-      <c r="F50" s="9" t="n"/>
-      <c r="G50" s="9" t="n"/>
     </row>
     <row r="51">
       <c r="A51" s="8" t="inlineStr">
         <is>
-          <t>VSC Infra Profile First Controller</t>
+          <t>VSC Infra Profile Name</t>
         </is>
       </c>
       <c r="B51" s="9" t="n"/>
@@ -4936,7 +4942,7 @@
     <row r="52">
       <c r="A52" s="8" t="inlineStr">
         <is>
-          <t>VSC Infra Profile Second Controller</t>
+          <t>VSC Infra Profile First Controller</t>
         </is>
       </c>
       <c r="B52" s="9" t="n"/>
@@ -4949,7 +4955,7 @@
     <row r="53">
       <c r="A53" s="8" t="inlineStr">
         <is>
-          <t>NSG Network Port Name</t>
+          <t>VSC Infra Profile Second Controller</t>
         </is>
       </c>
       <c r="B53" s="9" t="n"/>
@@ -4960,29 +4966,29 @@
       <c r="G53" s="9" t="n"/>
     </row>
     <row r="54">
-      <c r="A54" s="3" t="inlineStr">
+      <c r="A54" s="8" t="inlineStr">
+        <is>
+          <t>NSG Network Port Name</t>
+        </is>
+      </c>
+      <c r="B54" s="9" t="n"/>
+      <c r="C54" s="9" t="n"/>
+      <c r="D54" s="9" t="n"/>
+      <c r="E54" s="9" t="n"/>
+      <c r="F54" s="9" t="n"/>
+      <c r="G54" s="9" t="n"/>
+    </row>
+    <row r="55">
+      <c r="A55" s="3" t="inlineStr">
         <is>
           <t>Network and Access Ports</t>
         </is>
       </c>
-    </row>
-    <row r="55">
-      <c r="A55" s="8" t="inlineStr">
-        <is>
-          <t>NSG Network Port Physical Name</t>
-        </is>
-      </c>
-      <c r="B55" s="9" t="n"/>
-      <c r="C55" s="9" t="n"/>
-      <c r="D55" s="9" t="n"/>
-      <c r="E55" s="9" t="n"/>
-      <c r="F55" s="9" t="n"/>
-      <c r="G55" s="9" t="n"/>
     </row>
     <row r="56">
       <c r="A56" s="8" t="inlineStr">
         <is>
-          <t>NSG Access Port Name</t>
+          <t>NSG Network Port Physical Name</t>
         </is>
       </c>
       <c r="B56" s="9" t="n"/>
@@ -4995,7 +5001,7 @@
     <row r="57">
       <c r="A57" s="8" t="inlineStr">
         <is>
-          <t>NSG Access Port Physical Name</t>
+          <t>NSG Access Port Name</t>
         </is>
       </c>
       <c r="B57" s="9" t="n"/>
@@ -5008,7 +5014,7 @@
     <row r="58">
       <c r="A58" s="8" t="inlineStr">
         <is>
-          <t>NSG Access Port VLAN Range</t>
+          <t>NSG Access Port Physical Name</t>
         </is>
       </c>
       <c r="B58" s="9" t="n"/>
@@ -5021,7 +5027,7 @@
     <row r="59">
       <c r="A59" s="8" t="inlineStr">
         <is>
-          <t>NSG Access Port VLAN Number</t>
+          <t>NSG Access Port VLAN Range</t>
         </is>
       </c>
       <c r="B59" s="9" t="n"/>
@@ -5032,42 +5038,42 @@
       <c r="G59" s="9" t="n"/>
     </row>
     <row r="60">
-      <c r="A60" s="6" t="inlineStr">
+      <c r="A60" s="8" t="inlineStr">
+        <is>
+          <t>NSG Access Port VLAN Number</t>
+        </is>
+      </c>
+      <c r="B60" s="9" t="n"/>
+      <c r="C60" s="9" t="n"/>
+      <c r="D60" s="9" t="n"/>
+      <c r="E60" s="9" t="n"/>
+      <c r="F60" s="9" t="n"/>
+      <c r="G60" s="9" t="n"/>
+    </row>
+    <row r="61">
+      <c r="A61" s="6" t="inlineStr">
         <is>
           <t>NSGv Access ports list name</t>
         </is>
       </c>
-      <c r="B60" s="7" t="n"/>
-      <c r="C60" s="7" t="n"/>
-      <c r="D60" s="7" t="n"/>
-      <c r="E60" s="7" t="n"/>
-      <c r="F60" s="7" t="n"/>
-      <c r="G60" s="7" t="n"/>
-    </row>
-    <row r="61">
-      <c r="A61" s="3" t="inlineStr">
+      <c r="B61" s="7" t="n"/>
+      <c r="C61" s="7" t="n"/>
+      <c r="D61" s="7" t="n"/>
+      <c r="E61" s="7" t="n"/>
+      <c r="F61" s="7" t="n"/>
+      <c r="G61" s="7" t="n"/>
+    </row>
+    <row r="62">
+      <c r="A62" s="3" t="inlineStr">
         <is>
           <t>Telnet and Credentials</t>
         </is>
       </c>
-    </row>
-    <row r="62">
-      <c r="A62" s="8" t="inlineStr">
-        <is>
-          <t>Telnet port for console</t>
-        </is>
-      </c>
-      <c r="B62" s="9" t="n"/>
-      <c r="C62" s="9" t="n"/>
-      <c r="D62" s="9" t="n"/>
-      <c r="E62" s="9" t="n"/>
-      <c r="F62" s="9" t="n"/>
-      <c r="G62" s="9" t="n"/>
     </row>
     <row r="63">
       <c r="A63" s="8" t="inlineStr">
         <is>
-          <t>Credentials set name</t>
+          <t>Telnet port for console</t>
         </is>
       </c>
       <c r="B63" s="9" t="n"/>
@@ -5077,19 +5083,32 @@
       <c r="F63" s="9" t="n"/>
       <c r="G63" s="9" t="n"/>
     </row>
+    <row r="64">
+      <c r="A64" s="8" t="inlineStr">
+        <is>
+          <t>Credentials set name</t>
+        </is>
+      </c>
+      <c r="B64" s="9" t="n"/>
+      <c r="C64" s="9" t="n"/>
+      <c r="D64" s="9" t="n"/>
+      <c r="E64" s="9" t="n"/>
+      <c r="F64" s="9" t="n"/>
+      <c r="G64" s="9" t="n"/>
+    </row>
   </sheetData>
   <mergeCells count="11">
     <mergeCell ref="A4:G4"/>
-    <mergeCell ref="A8:G8"/>
-    <mergeCell ref="A14:G14"/>
-    <mergeCell ref="A18:G18"/>
-    <mergeCell ref="A24:G24"/>
-    <mergeCell ref="A33:G33"/>
-    <mergeCell ref="A38:G38"/>
-    <mergeCell ref="A44:G44"/>
-    <mergeCell ref="A49:G49"/>
-    <mergeCell ref="A54:G54"/>
-    <mergeCell ref="A61:G61"/>
+    <mergeCell ref="A9:G9"/>
+    <mergeCell ref="A15:G15"/>
+    <mergeCell ref="A19:G19"/>
+    <mergeCell ref="A25:G25"/>
+    <mergeCell ref="A34:G34"/>
+    <mergeCell ref="A39:G39"/>
+    <mergeCell ref="A45:G45"/>
+    <mergeCell ref="A50:G50"/>
+    <mergeCell ref="A55:G55"/>
+    <mergeCell ref="A62:G62"/>
   </mergeCells>
   <dataValidations count="42">
     <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="B6" type="list">
@@ -5110,90 +5129,90 @@
     <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="G6" type="list">
       <formula1>"kvm,vcenter,aws"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="B9" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="B10" type="list">
       <formula1>"none,zfb_metro,zfb_external,activation_link"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="C9" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="C10" type="list">
       <formula1>"none,zfb_metro,zfb_external,activation_link"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="D9" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="D10" type="list">
       <formula1>"none,zfb_metro,zfb_external,activation_link"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="E9" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="E10" type="list">
       <formula1>"none,zfb_metro,zfb_external,activation_link"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="F9" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="F10" type="list">
       <formula1>"none,zfb_metro,zfb_external,activation_link"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="G9" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="G10" type="list">
       <formula1>"none,zfb_metro,zfb_external,activation_link"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="B41" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="B42" type="list">
       <formula1>"none,hostname,ip_address,mac_address,nsgateway_id,serial_number,uuid"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="C41" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="C42" type="list">
       <formula1>"none,hostname,ip_address,mac_address,nsgateway_id,serial_number,uuid"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="D41" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="D42" type="list">
       <formula1>"none,hostname,ip_address,mac_address,nsgateway_id,serial_number,uuid"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="E41" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="E42" type="list">
       <formula1>"none,hostname,ip_address,mac_address,nsgateway_id,serial_number,uuid"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="F41" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="F42" type="list">
       <formula1>"none,hostname,ip_address,mac_address,nsgateway_id,serial_number,uuid"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="G41" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="G42" type="list">
       <formula1>"none,hostname,ip_address,mac_address,nsgateway_id,serial_number,uuid"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="B43" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="B44" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="C43" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="C44" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="D43" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="D44" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="E43" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="E44" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="F43" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="F44" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="G43" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="G44" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="B48" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="B49" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="C48" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="C49" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="D48" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="D49" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="E48" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="E49" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="F48" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="F49" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="G48" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="G49" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B59" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="C59" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="D59" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="E59" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="F59" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="G59" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B62" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="C62" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="D62" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="E62" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="F62" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="G62" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B60" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="C60" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="D60" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="E60" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="F60" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="G60" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B63" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="C63" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="D63" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="E63" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="F63" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="G63" type="whole"/>
   </dataValidations>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <legacyDrawing r:id="anysvml"/>

</xml_diff>

<commit_message>
Add VSC schema change
</commit_message>
<xml_diff>
--- a/examples/excel/active_standby_vsds.xlsx
+++ b/examples/excel/active_standby_vsds.xlsx
@@ -2684,6 +2684,7 @@
     <author>cpuset</author>
     <author>enable_hardening</author>
     <author>vsc_config_file_paths</author>
+    <author>override_vsc_config</author>
   </authors>
   <commentList>
     <comment authorId="0" ref="A5" shapeId="0">
@@ -2969,6 +2970,11 @@
     <comment authorId="56" ref="A70" shapeId="0">
       <text>
         <t>Paths to files that can be optionally applied for additional VSC configuration (List items separated by comma.)</t>
+      </text>
+    </comment>
+    <comment authorId="57" ref="A71" shapeId="0">
+      <text>
+        <t>This will override the Metro Provided config on the VSC by the config provided in vsc_config_file_paths [default: False]</t>
       </text>
     </comment>
   </commentList>
@@ -10671,7 +10677,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C70"/>
+  <dimension ref="A1:C71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11281,6 +11287,15 @@
       <c r="B70" s="9" t="n"/>
       <c r="C70" s="9" t="n"/>
     </row>
+    <row r="71">
+      <c r="A71" s="8" t="inlineStr">
+        <is>
+          <t>Override the configuration on VSC</t>
+        </is>
+      </c>
+      <c r="B71" s="9" t="n"/>
+      <c r="C71" s="9" t="n"/>
+    </row>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="A4:C4"/>
@@ -11294,7 +11309,7 @@
     <mergeCell ref="A60:C60"/>
     <mergeCell ref="A67:C67"/>
   </mergeCells>
-  <dataValidations count="20">
+  <dataValidations count="22">
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B7" type="whole"/>
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="C7" type="whole"/>
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B12" type="whole"/>
@@ -11321,6 +11336,12 @@
       <formula1>"true,false"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="C69" type="list">
+      <formula1>"true,false"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="B71" type="list">
+      <formula1>"true,false"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="C71" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Clean up cloudformation template
</commit_message>
<xml_diff>
--- a/examples/excel/active_standby_vsds.xlsx
+++ b/examples/excel/active_standby_vsds.xlsx
@@ -343,6 +343,7 @@
     <author>provision_vpc_nsg_wan_subnet_cidr</author>
     <author>provision_vpc_nsg_lan_subnet_cidr</author>
     <author>provision_vpc_private_subnet_cidr</author>
+    <author>deploy_only_nsgv</author>
     <author>proxy_external_ip</author>
     <author>nsg_organization</author>
     <author>nsg_name</author>
@@ -514,110 +515,115 @@
     </comment>
     <comment authorId="29" ref="A39" shapeId="0">
       <text>
-        <t>IP address of the VNSUtil VM or the NUH used as a proxy for the NSGv on AWS [default: ]</t>
-      </text>
-    </comment>
-    <comment authorId="30" ref="A41" shapeId="0">
+        <t>Whether all components are being deployed on AWS or only the NSGv. Only needed when provision_vpc parameters are provided [default: false]</t>
+      </text>
+    </comment>
+    <comment authorId="30" ref="A40" shapeId="0">
+      <text>
+        <t>Externally routable IP address of the VNSUtil VM or the NUH used as a proxy for the NSGv on AWS. Required when deploying only the NSGv on AWS [default: ]</t>
+      </text>
+    </comment>
+    <comment authorId="31" ref="A42" shapeId="0">
       <text>
         <t>Organization on the VSD to associate with the NSG being bootstrapped, overrides global setting. [default: ]</t>
       </text>
     </comment>
-    <comment authorId="31" ref="A42" shapeId="0">
+    <comment authorId="32" ref="A43" shapeId="0">
       <text>
         <t>Name of the NSG on the VSD [default: ]</t>
       </text>
     </comment>
-    <comment authorId="32" ref="A43" shapeId="0">
+    <comment authorId="33" ref="A44" shapeId="0">
       <text>
         <t>Field type to match against for NSGv activation. [default: none]</t>
       </text>
     </comment>
-    <comment authorId="33" ref="A44" shapeId="0">
+    <comment authorId="34" ref="A45" shapeId="0">
       <text>
         <t>Value to match against for NSGv activation. [default: ]</t>
       </text>
     </comment>
-    <comment authorId="34" ref="A45" shapeId="0">
+    <comment authorId="35" ref="A46" shapeId="0">
       <text>
         <t>Enables SSH on NSGv when set. [default: False]</t>
       </text>
     </comment>
-    <comment authorId="35" ref="A47" shapeId="0">
+    <comment authorId="36" ref="A48" shapeId="0">
       <text>
         <t>Name of the NSG infra profile template on the VSD [default: ]</t>
       </text>
     </comment>
-    <comment authorId="36" ref="A48" shapeId="0">
+    <comment authorId="37" ref="A49" shapeId="0">
       <text>
         <t>Name of the NSG infra profile on the VSD [default: ]</t>
       </text>
     </comment>
-    <comment authorId="37" ref="A49" shapeId="0">
+    <comment authorId="38" ref="A50" shapeId="0">
       <text>
         <t>Name of the NSG infra profile proxy DNS on the VSD [default: ]</t>
       </text>
     </comment>
-    <comment authorId="38" ref="A50" shapeId="0">
+    <comment authorId="39" ref="A51" shapeId="0">
       <text>
         <t>Allows NSGs using this profile to override SSH access. [default: False]</t>
       </text>
     </comment>
-    <comment authorId="39" ref="A52" shapeId="0">
+    <comment authorId="40" ref="A53" shapeId="0">
       <text>
         <t>Name of the VSC infra profile for the NSG on the VSD [default: ]</t>
       </text>
     </comment>
-    <comment authorId="40" ref="A53" shapeId="0">
+    <comment authorId="41" ref="A54" shapeId="0">
       <text>
         <t>Host name or IP address of the VSC infra profile first controller for the NSG [default: ]</t>
       </text>
     </comment>
-    <comment authorId="41" ref="A54" shapeId="0">
+    <comment authorId="42" ref="A55" shapeId="0">
       <text>
         <t>Host name or IP address of the VSC infra profile second controller for the NSG [default: ]</t>
       </text>
     </comment>
-    <comment authorId="42" ref="A55" shapeId="0">
+    <comment authorId="43" ref="A56" shapeId="0">
       <text>
         <t>Name of the network port for the NSG [default: ]</t>
       </text>
     </comment>
-    <comment authorId="43" ref="A57" shapeId="0">
+    <comment authorId="44" ref="A58" shapeId="0">
       <text>
         <t>Physical name of the network port for the NSG [default: port1]</t>
       </text>
     </comment>
-    <comment authorId="44" ref="A58" shapeId="0">
+    <comment authorId="45" ref="A59" shapeId="0">
       <text>
         <t>Name of the access port for the NSG. Deprecated in favor of access_ports [default: ]</t>
       </text>
     </comment>
-    <comment authorId="45" ref="A59" shapeId="0">
+    <comment authorId="46" ref="A60" shapeId="0">
       <text>
         <t>Physical name of the access port for the NSG. Deprecated in favor of access_ports [default: port2]</t>
       </text>
     </comment>
-    <comment authorId="46" ref="A60" shapeId="0">
+    <comment authorId="47" ref="A61" shapeId="0">
       <text>
         <t>VLAN range of the access port for the NSG. Deprecated in favor of access_ports [default: ]</t>
       </text>
     </comment>
-    <comment authorId="47" ref="A61" shapeId="0">
+    <comment authorId="48" ref="A62" shapeId="0">
       <text>
         <t>VLAN number of the NSG access port for the NSG. Deprecated in favor of access_ports [default: 0]</t>
       </text>
     </comment>
-    <comment authorId="48" ref="A62" shapeId="0">
+    <comment authorId="49" ref="A63" shapeId="0">
       <text>
         <t>Name of access ports list. (List items separated by comma.)</t>
       </text>
     </comment>
-    <comment authorId="49" ref="A64" shapeId="0">
+    <comment authorId="50" ref="A65" shapeId="0">
       <text>
         <t>The port for telnet to HV host to access NSGv serial or console terminal [default: 2300]</t>
       </text>
     </comment>
-    <comment authorId="50" ref="A65" shapeId="0">
+    <comment authorId="51" ref="A66" shapeId="0">
       <text>
         <t>Name of the credentials set for the vsd</t>
       </text>
@@ -2203,6 +2209,7 @@
   <authors>
     <author>hostname</author>
     <author>vname</author>
+    <author>target_server_type</author>
     <author>target_server</author>
     <author>mgmt_ip</author>
     <author>mgmt_gateway</author>
@@ -2213,6 +2220,7 @@
     <author>system_ip</author>
     <author>data_ip</author>
     <author>license_file</author>
+    <author>remote_license_file_location</author>
     <author>deploy_cfg_file</author>
     <author>config_file_directory</author>
     <author>credentials_set</author>
@@ -2230,65 +2238,75 @@
     </comment>
     <comment authorId="2" ref="A7" shapeId="0">
       <text>
+        <t>Type of hypervisor environment into which the instance will be created</t>
+      </text>
+    </comment>
+    <comment authorId="3" ref="A8" shapeId="0">
+      <text>
         <t>Hostname or IP address of the KVM hypervisor where the VSR VM will be instantiated</t>
       </text>
     </comment>
-    <comment authorId="3" ref="A9" shapeId="0">
+    <comment authorId="4" ref="A10" shapeId="0">
       <text>
         <t>IP address to apply to the management interface of the VSR VM</t>
       </text>
     </comment>
-    <comment authorId="4" ref="A10" shapeId="0">
+    <comment authorId="5" ref="A11" shapeId="0">
       <text>
         <t>Network gateway of the management network for the VSR VM</t>
       </text>
     </comment>
-    <comment authorId="5" ref="A11" shapeId="0">
+    <comment authorId="6" ref="A12" shapeId="0">
       <text>
         <t>Management network mask prefix length for the VSR VM</t>
       </text>
     </comment>
-    <comment authorId="6" ref="A12" shapeId="0">
+    <comment authorId="7" ref="A13" shapeId="0">
       <text>
         <t>Static routes to apply to the management network for the VSR VM (List items separated by comma.)</t>
       </text>
     </comment>
-    <comment authorId="7" ref="A13" shapeId="0">
+    <comment authorId="8" ref="A14" shapeId="0">
       <text>
         <t/>
       </text>
     </comment>
-    <comment authorId="8" ref="A14" shapeId="0">
+    <comment authorId="9" ref="A15" shapeId="0">
       <text>
         <t xml:space="preserve"> (List items separated by comma.)</t>
       </text>
     </comment>
-    <comment authorId="9" ref="A16" shapeId="0">
+    <comment authorId="10" ref="A17" shapeId="0">
       <text>
         <t>IP address to apply to the system network interface for the VSR VM</t>
       </text>
     </comment>
-    <comment authorId="10" ref="A17" shapeId="0">
-      <text>
-        <t>IP address to apply to the data network interface for the VSR VM</t>
-      </text>
-    </comment>
-    <comment authorId="11" ref="A19" shapeId="0">
+    <comment authorId="11" ref="A18" shapeId="0">
+      <text>
+        <t>IP address to apply to the data network interface for the VSR VM. Use format IP Address/Netmask</t>
+      </text>
+    </comment>
+    <comment authorId="12" ref="A20" shapeId="0">
+      <text>
+        <t>Location of the VSR license file</t>
+      </text>
+    </comment>
+    <comment authorId="13" ref="A21" shapeId="0">
+      <text>
+        <t>Optional location of the VSR license file on the remote ftp or tftp location</t>
+      </text>
+    </comment>
+    <comment authorId="14" ref="A22" shapeId="0">
       <text>
         <t/>
       </text>
     </comment>
-    <comment authorId="12" ref="A20" shapeId="0">
+    <comment authorId="15" ref="A23" shapeId="0">
       <text>
         <t/>
       </text>
     </comment>
-    <comment authorId="13" ref="A21" shapeId="0">
-      <text>
-        <t/>
-      </text>
-    </comment>
-    <comment authorId="14" ref="A22" shapeId="0">
+    <comment authorId="16" ref="A24" shapeId="0">
       <text>
         <t>Name of the credentials set for the vsd</t>
       </text>
@@ -4386,7 +4404,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G65"/>
+  <dimension ref="A1:G66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4839,7 +4857,7 @@
     <row r="39">
       <c r="A39" s="8" t="inlineStr">
         <is>
-          <t>Proxy IP Address</t>
+          <t>Deploy Only NSGv on AWS</t>
         </is>
       </c>
       <c r="B39" s="9" t="n"/>
@@ -4850,29 +4868,29 @@
       <c r="G39" s="9" t="n"/>
     </row>
     <row r="40">
-      <c r="A40" s="3" t="inlineStr">
+      <c r="A40" s="8" t="inlineStr">
+        <is>
+          <t>Proxy IP Address</t>
+        </is>
+      </c>
+      <c r="B40" s="9" t="n"/>
+      <c r="C40" s="9" t="n"/>
+      <c r="D40" s="9" t="n"/>
+      <c r="E40" s="9" t="n"/>
+      <c r="F40" s="9" t="n"/>
+      <c r="G40" s="9" t="n"/>
+    </row>
+    <row r="41">
+      <c r="A41" s="3" t="inlineStr">
         <is>
           <t>NSGv Zero-Factor Bootstrap</t>
         </is>
       </c>
-    </row>
-    <row r="41">
-      <c r="A41" s="8" t="inlineStr">
-        <is>
-          <t>NSG Organization</t>
-        </is>
-      </c>
-      <c r="B41" s="9" t="n"/>
-      <c r="C41" s="9" t="n"/>
-      <c r="D41" s="9" t="n"/>
-      <c r="E41" s="9" t="n"/>
-      <c r="F41" s="9" t="n"/>
-      <c r="G41" s="9" t="n"/>
     </row>
     <row r="42">
       <c r="A42" s="8" t="inlineStr">
         <is>
-          <t>NSG Name</t>
+          <t>NSG Organization</t>
         </is>
       </c>
       <c r="B42" s="9" t="n"/>
@@ -4883,22 +4901,22 @@
       <c r="G42" s="9" t="n"/>
     </row>
     <row r="43">
-      <c r="A43" s="6" t="inlineStr">
-        <is>
-          <t>Activation Matching Type</t>
-        </is>
-      </c>
-      <c r="B43" s="7" t="n"/>
-      <c r="C43" s="7" t="n"/>
-      <c r="D43" s="7" t="n"/>
-      <c r="E43" s="7" t="n"/>
-      <c r="F43" s="7" t="n"/>
-      <c r="G43" s="7" t="n"/>
+      <c r="A43" s="8" t="inlineStr">
+        <is>
+          <t>NSG Name</t>
+        </is>
+      </c>
+      <c r="B43" s="9" t="n"/>
+      <c r="C43" s="9" t="n"/>
+      <c r="D43" s="9" t="n"/>
+      <c r="E43" s="9" t="n"/>
+      <c r="F43" s="9" t="n"/>
+      <c r="G43" s="9" t="n"/>
     </row>
     <row r="44">
       <c r="A44" s="6" t="inlineStr">
         <is>
-          <t>Activation Matching Value</t>
+          <t>Activation Matching Type</t>
         </is>
       </c>
       <c r="B44" s="7" t="n"/>
@@ -4909,42 +4927,42 @@
       <c r="G44" s="7" t="n"/>
     </row>
     <row r="45">
-      <c r="A45" s="8" t="inlineStr">
+      <c r="A45" s="6" t="inlineStr">
+        <is>
+          <t>Activation Matching Value</t>
+        </is>
+      </c>
+      <c r="B45" s="7" t="n"/>
+      <c r="C45" s="7" t="n"/>
+      <c r="D45" s="7" t="n"/>
+      <c r="E45" s="7" t="n"/>
+      <c r="F45" s="7" t="n"/>
+      <c r="G45" s="7" t="n"/>
+    </row>
+    <row r="46">
+      <c r="A46" s="8" t="inlineStr">
         <is>
           <t>Enable SSH on NSGv</t>
         </is>
       </c>
-      <c r="B45" s="9" t="n"/>
-      <c r="C45" s="9" t="n"/>
-      <c r="D45" s="9" t="n"/>
-      <c r="E45" s="9" t="n"/>
-      <c r="F45" s="9" t="n"/>
-      <c r="G45" s="9" t="n"/>
-    </row>
-    <row r="46">
-      <c r="A46" s="3" t="inlineStr">
+      <c r="B46" s="9" t="n"/>
+      <c r="C46" s="9" t="n"/>
+      <c r="D46" s="9" t="n"/>
+      <c r="E46" s="9" t="n"/>
+      <c r="F46" s="9" t="n"/>
+      <c r="G46" s="9" t="n"/>
+    </row>
+    <row r="47">
+      <c r="A47" s="3" t="inlineStr">
         <is>
           <t>NSG Advanced Options</t>
         </is>
       </c>
-    </row>
-    <row r="47">
-      <c r="A47" s="8" t="inlineStr">
-        <is>
-          <t>NSG Infra Profile Template Name</t>
-        </is>
-      </c>
-      <c r="B47" s="9" t="n"/>
-      <c r="C47" s="9" t="n"/>
-      <c r="D47" s="9" t="n"/>
-      <c r="E47" s="9" t="n"/>
-      <c r="F47" s="9" t="n"/>
-      <c r="G47" s="9" t="n"/>
     </row>
     <row r="48">
       <c r="A48" s="8" t="inlineStr">
         <is>
-          <t>NSG Infra Profile Name</t>
+          <t>NSG Infra Profile Template Name</t>
         </is>
       </c>
       <c r="B48" s="9" t="n"/>
@@ -4957,7 +4975,7 @@
     <row r="49">
       <c r="A49" s="8" t="inlineStr">
         <is>
-          <t>NSG Infra Profile Proxy DNS Name</t>
+          <t>NSG Infra Profile Name</t>
         </is>
       </c>
       <c r="B49" s="9" t="n"/>
@@ -4970,7 +4988,7 @@
     <row r="50">
       <c r="A50" s="8" t="inlineStr">
         <is>
-          <t>Allow SSH Access Override</t>
+          <t>NSG Infra Profile Proxy DNS Name</t>
         </is>
       </c>
       <c r="B50" s="9" t="n"/>
@@ -4981,29 +4999,29 @@
       <c r="G50" s="9" t="n"/>
     </row>
     <row r="51">
-      <c r="A51" s="3" t="inlineStr">
+      <c r="A51" s="8" t="inlineStr">
+        <is>
+          <t>Allow SSH Access Override</t>
+        </is>
+      </c>
+      <c r="B51" s="9" t="n"/>
+      <c r="C51" s="9" t="n"/>
+      <c r="D51" s="9" t="n"/>
+      <c r="E51" s="9" t="n"/>
+      <c r="F51" s="9" t="n"/>
+      <c r="G51" s="9" t="n"/>
+    </row>
+    <row r="52">
+      <c r="A52" s="3" t="inlineStr">
         <is>
           <t>VSC Info</t>
         </is>
       </c>
-    </row>
-    <row r="52">
-      <c r="A52" s="8" t="inlineStr">
-        <is>
-          <t>VSC Infra Profile Name</t>
-        </is>
-      </c>
-      <c r="B52" s="9" t="n"/>
-      <c r="C52" s="9" t="n"/>
-      <c r="D52" s="9" t="n"/>
-      <c r="E52" s="9" t="n"/>
-      <c r="F52" s="9" t="n"/>
-      <c r="G52" s="9" t="n"/>
     </row>
     <row r="53">
       <c r="A53" s="8" t="inlineStr">
         <is>
-          <t>VSC Infra Profile First Controller</t>
+          <t>VSC Infra Profile Name</t>
         </is>
       </c>
       <c r="B53" s="9" t="n"/>
@@ -5016,7 +5034,7 @@
     <row r="54">
       <c r="A54" s="8" t="inlineStr">
         <is>
-          <t>VSC Infra Profile Second Controller</t>
+          <t>VSC Infra Profile First Controller</t>
         </is>
       </c>
       <c r="B54" s="9" t="n"/>
@@ -5029,7 +5047,7 @@
     <row r="55">
       <c r="A55" s="8" t="inlineStr">
         <is>
-          <t>NSG Network Port Name</t>
+          <t>VSC Infra Profile Second Controller</t>
         </is>
       </c>
       <c r="B55" s="9" t="n"/>
@@ -5040,29 +5058,29 @@
       <c r="G55" s="9" t="n"/>
     </row>
     <row r="56">
-      <c r="A56" s="3" t="inlineStr">
+      <c r="A56" s="8" t="inlineStr">
+        <is>
+          <t>NSG Network Port Name</t>
+        </is>
+      </c>
+      <c r="B56" s="9" t="n"/>
+      <c r="C56" s="9" t="n"/>
+      <c r="D56" s="9" t="n"/>
+      <c r="E56" s="9" t="n"/>
+      <c r="F56" s="9" t="n"/>
+      <c r="G56" s="9" t="n"/>
+    </row>
+    <row r="57">
+      <c r="A57" s="3" t="inlineStr">
         <is>
           <t>Network and Access Ports</t>
         </is>
       </c>
-    </row>
-    <row r="57">
-      <c r="A57" s="8" t="inlineStr">
-        <is>
-          <t>NSG Network Port Physical Name</t>
-        </is>
-      </c>
-      <c r="B57" s="9" t="n"/>
-      <c r="C57" s="9" t="n"/>
-      <c r="D57" s="9" t="n"/>
-      <c r="E57" s="9" t="n"/>
-      <c r="F57" s="9" t="n"/>
-      <c r="G57" s="9" t="n"/>
     </row>
     <row r="58">
       <c r="A58" s="8" t="inlineStr">
         <is>
-          <t>NSG Access Port Name</t>
+          <t>NSG Network Port Physical Name</t>
         </is>
       </c>
       <c r="B58" s="9" t="n"/>
@@ -5075,7 +5093,7 @@
     <row r="59">
       <c r="A59" s="8" t="inlineStr">
         <is>
-          <t>NSG Access Port Physical Name</t>
+          <t>NSG Access Port Name</t>
         </is>
       </c>
       <c r="B59" s="9" t="n"/>
@@ -5088,7 +5106,7 @@
     <row r="60">
       <c r="A60" s="8" t="inlineStr">
         <is>
-          <t>NSG Access Port VLAN Range</t>
+          <t>NSG Access Port Physical Name</t>
         </is>
       </c>
       <c r="B60" s="9" t="n"/>
@@ -5101,7 +5119,7 @@
     <row r="61">
       <c r="A61" s="8" t="inlineStr">
         <is>
-          <t>NSG Access Port VLAN Number</t>
+          <t>NSG Access Port VLAN Range</t>
         </is>
       </c>
       <c r="B61" s="9" t="n"/>
@@ -5112,42 +5130,42 @@
       <c r="G61" s="9" t="n"/>
     </row>
     <row r="62">
-      <c r="A62" s="6" t="inlineStr">
+      <c r="A62" s="8" t="inlineStr">
+        <is>
+          <t>NSG Access Port VLAN Number</t>
+        </is>
+      </c>
+      <c r="B62" s="9" t="n"/>
+      <c r="C62" s="9" t="n"/>
+      <c r="D62" s="9" t="n"/>
+      <c r="E62" s="9" t="n"/>
+      <c r="F62" s="9" t="n"/>
+      <c r="G62" s="9" t="n"/>
+    </row>
+    <row r="63">
+      <c r="A63" s="6" t="inlineStr">
         <is>
           <t>NSGv Access ports list name</t>
         </is>
       </c>
-      <c r="B62" s="7" t="n"/>
-      <c r="C62" s="7" t="n"/>
-      <c r="D62" s="7" t="n"/>
-      <c r="E62" s="7" t="n"/>
-      <c r="F62" s="7" t="n"/>
-      <c r="G62" s="7" t="n"/>
-    </row>
-    <row r="63">
-      <c r="A63" s="3" t="inlineStr">
+      <c r="B63" s="7" t="n"/>
+      <c r="C63" s="7" t="n"/>
+      <c r="D63" s="7" t="n"/>
+      <c r="E63" s="7" t="n"/>
+      <c r="F63" s="7" t="n"/>
+      <c r="G63" s="7" t="n"/>
+    </row>
+    <row r="64">
+      <c r="A64" s="3" t="inlineStr">
         <is>
           <t>Telnet and Credentials</t>
         </is>
       </c>
-    </row>
-    <row r="64">
-      <c r="A64" s="8" t="inlineStr">
-        <is>
-          <t>Telnet port for console</t>
-        </is>
-      </c>
-      <c r="B64" s="9" t="n"/>
-      <c r="C64" s="9" t="n"/>
-      <c r="D64" s="9" t="n"/>
-      <c r="E64" s="9" t="n"/>
-      <c r="F64" s="9" t="n"/>
-      <c r="G64" s="9" t="n"/>
     </row>
     <row r="65">
       <c r="A65" s="8" t="inlineStr">
         <is>
-          <t>Credentials set name</t>
+          <t>Telnet port for console</t>
         </is>
       </c>
       <c r="B65" s="9" t="n"/>
@@ -5156,6 +5174,19 @@
       <c r="E65" s="9" t="n"/>
       <c r="F65" s="9" t="n"/>
       <c r="G65" s="9" t="n"/>
+    </row>
+    <row r="66">
+      <c r="A66" s="8" t="inlineStr">
+        <is>
+          <t>Credentials set name</t>
+        </is>
+      </c>
+      <c r="B66" s="9" t="n"/>
+      <c r="C66" s="9" t="n"/>
+      <c r="D66" s="9" t="n"/>
+      <c r="E66" s="9" t="n"/>
+      <c r="F66" s="9" t="n"/>
+      <c r="G66" s="9" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -5165,13 +5196,13 @@
     <mergeCell ref="A19:G19"/>
     <mergeCell ref="A25:G25"/>
     <mergeCell ref="A34:G34"/>
-    <mergeCell ref="A40:G40"/>
-    <mergeCell ref="A46:G46"/>
-    <mergeCell ref="A51:G51"/>
-    <mergeCell ref="A56:G56"/>
-    <mergeCell ref="A63:G63"/>
+    <mergeCell ref="A41:G41"/>
+    <mergeCell ref="A47:G47"/>
+    <mergeCell ref="A52:G52"/>
+    <mergeCell ref="A57:G57"/>
+    <mergeCell ref="A64:G64"/>
   </mergeCells>
-  <dataValidations count="48">
+  <dataValidations count="54">
     <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="B6" type="list">
       <formula1>"kvm,vcenter,aws"</formula1>
     </dataValidation>
@@ -5214,72 +5245,90 @@
     <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="G10" type="list">
       <formula1>"none,zfb_metro,zfb_external,activation_link"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="B43" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="B39" type="list">
+      <formula1>"true,false"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="C39" type="list">
+      <formula1>"true,false"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="D39" type="list">
+      <formula1>"true,false"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="E39" type="list">
+      <formula1>"true,false"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="F39" type="list">
+      <formula1>"true,false"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="G39" type="list">
+      <formula1>"true,false"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="B44" type="list">
       <formula1>"none,hostname,ip_address,mac_address,nsgateway_id,serial_number,uuid"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="C43" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="C44" type="list">
       <formula1>"none,hostname,ip_address,mac_address,nsgateway_id,serial_number,uuid"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="D43" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="D44" type="list">
       <formula1>"none,hostname,ip_address,mac_address,nsgateway_id,serial_number,uuid"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="E43" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="E44" type="list">
       <formula1>"none,hostname,ip_address,mac_address,nsgateway_id,serial_number,uuid"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="F43" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="F44" type="list">
       <formula1>"none,hostname,ip_address,mac_address,nsgateway_id,serial_number,uuid"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="G43" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="G44" type="list">
       <formula1>"none,hostname,ip_address,mac_address,nsgateway_id,serial_number,uuid"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="B45" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="B46" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="C45" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="C46" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="D45" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="D46" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="E45" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="E46" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="F45" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="F46" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="G45" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="G46" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="B50" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="B51" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="C50" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="C51" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="D50" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="D51" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="E50" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="E51" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="F50" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="F51" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="G50" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="G51" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B61" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="C61" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="D61" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="E61" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="F61" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="G61" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B64" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="C64" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="D64" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="E64" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="F64" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="G64" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B62" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="C62" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="D62" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="E62" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="F62" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="G62" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B65" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="C65" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="D65" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="E65" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="F65" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="G65" type="whole"/>
   </dataValidations>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <legacyDrawing r:id="anysvml"/>
@@ -9358,7 +9407,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9423,81 +9472,81 @@
       <c r="G6" s="7" t="n"/>
     </row>
     <row r="7">
-      <c r="A7" s="6" t="inlineStr">
+      <c r="A7" s="4" t="inlineStr">
+        <is>
+          <t>Target Server Type</t>
+        </is>
+      </c>
+      <c r="B7" s="5" t="n"/>
+      <c r="C7" s="5" t="n"/>
+      <c r="D7" s="5" t="n"/>
+      <c r="E7" s="5" t="n"/>
+      <c r="F7" s="5" t="n"/>
+      <c r="G7" s="5" t="n"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="4" t="inlineStr">
         <is>
           <t>Target Server IP or FQDN</t>
         </is>
       </c>
-      <c r="B7" s="7" t="n"/>
-      <c r="C7" s="7" t="n"/>
-      <c r="D7" s="7" t="n"/>
-      <c r="E7" s="7" t="n"/>
-      <c r="F7" s="7" t="n"/>
-      <c r="G7" s="7" t="n"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="3" t="inlineStr">
+      <c r="B8" s="5" t="n"/>
+      <c r="C8" s="5" t="n"/>
+      <c r="D8" s="5" t="n"/>
+      <c r="E8" s="5" t="n"/>
+      <c r="F8" s="5" t="n"/>
+      <c r="G8" s="5" t="n"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="3" t="inlineStr">
         <is>
           <t>Management network</t>
         </is>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="6" t="inlineStr">
+    <row r="10">
+      <c r="A10" s="4" t="inlineStr">
         <is>
           <t>Management IP Address</t>
         </is>
       </c>
-      <c r="B9" s="7" t="n"/>
-      <c r="C9" s="7" t="n"/>
-      <c r="D9" s="7" t="n"/>
-      <c r="E9" s="7" t="n"/>
-      <c r="F9" s="7" t="n"/>
-      <c r="G9" s="7" t="n"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="6" t="inlineStr">
+      <c r="B10" s="5" t="n"/>
+      <c r="C10" s="5" t="n"/>
+      <c r="D10" s="5" t="n"/>
+      <c r="E10" s="5" t="n"/>
+      <c r="F10" s="5" t="n"/>
+      <c r="G10" s="5" t="n"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="4" t="inlineStr">
         <is>
           <t>Management Network Gateway</t>
         </is>
       </c>
-      <c r="B10" s="7" t="n"/>
-      <c r="C10" s="7" t="n"/>
-      <c r="D10" s="7" t="n"/>
-      <c r="E10" s="7" t="n"/>
-      <c r="F10" s="7" t="n"/>
-      <c r="G10" s="7" t="n"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="6" t="inlineStr">
+      <c r="B11" s="5" t="n"/>
+      <c r="C11" s="5" t="n"/>
+      <c r="D11" s="5" t="n"/>
+      <c r="E11" s="5" t="n"/>
+      <c r="F11" s="5" t="n"/>
+      <c r="G11" s="5" t="n"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="4" t="inlineStr">
         <is>
           <t>Management Network Mask Prefix Length</t>
         </is>
       </c>
-      <c r="B11" s="7" t="n"/>
-      <c r="C11" s="7" t="n"/>
-      <c r="D11" s="7" t="n"/>
-      <c r="E11" s="7" t="n"/>
-      <c r="F11" s="7" t="n"/>
-      <c r="G11" s="7" t="n"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="6" t="inlineStr">
-        <is>
-          <t>Management Static Route List</t>
-        </is>
-      </c>
-      <c r="B12" s="7" t="n"/>
-      <c r="C12" s="7" t="n"/>
-      <c r="D12" s="7" t="n"/>
-      <c r="E12" s="7" t="n"/>
-      <c r="F12" s="7" t="n"/>
-      <c r="G12" s="7" t="n"/>
+      <c r="B12" s="5" t="n"/>
+      <c r="C12" s="5" t="n"/>
+      <c r="D12" s="5" t="n"/>
+      <c r="E12" s="5" t="n"/>
+      <c r="F12" s="5" t="n"/>
+      <c r="G12" s="5" t="n"/>
     </row>
     <row r="13">
       <c r="A13" s="6" t="inlineStr">
         <is>
-          <t>Management to Hypervisor Bridge</t>
+          <t>Management Static Route List</t>
         </is>
       </c>
       <c r="B13" s="7" t="n"/>
@@ -9510,7 +9559,7 @@
     <row r="14">
       <c r="A14" s="6" t="inlineStr">
         <is>
-          <t>Port to Hypervisor Bridges</t>
+          <t>Management to Hypervisor Bridge</t>
         </is>
       </c>
       <c r="B14" s="7" t="n"/>
@@ -9521,29 +9570,29 @@
       <c r="G14" s="7" t="n"/>
     </row>
     <row r="15">
-      <c r="A15" s="3" t="inlineStr">
+      <c r="A15" s="6" t="inlineStr">
+        <is>
+          <t>Port to Hypervisor Bridges</t>
+        </is>
+      </c>
+      <c r="B15" s="7" t="n"/>
+      <c r="C15" s="7" t="n"/>
+      <c r="D15" s="7" t="n"/>
+      <c r="E15" s="7" t="n"/>
+      <c r="F15" s="7" t="n"/>
+      <c r="G15" s="7" t="n"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="3" t="inlineStr">
         <is>
           <t>System and Data IP</t>
         </is>
       </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="6" t="inlineStr">
-        <is>
-          <t>System IP</t>
-        </is>
-      </c>
-      <c r="B16" s="7" t="n"/>
-      <c r="C16" s="7" t="n"/>
-      <c r="D16" s="7" t="n"/>
-      <c r="E16" s="7" t="n"/>
-      <c r="F16" s="7" t="n"/>
-      <c r="G16" s="7" t="n"/>
     </row>
     <row r="17">
       <c r="A17" s="6" t="inlineStr">
         <is>
-          <t>Data IP</t>
+          <t>System IP</t>
         </is>
       </c>
       <c r="B17" s="7" t="n"/>
@@ -9554,29 +9603,29 @@
       <c r="G17" s="7" t="n"/>
     </row>
     <row r="18">
-      <c r="A18" s="3" t="inlineStr">
+      <c r="A18" s="6" t="inlineStr">
+        <is>
+          <t>Data IP</t>
+        </is>
+      </c>
+      <c r="B18" s="7" t="n"/>
+      <c r="C18" s="7" t="n"/>
+      <c r="D18" s="7" t="n"/>
+      <c r="E18" s="7" t="n"/>
+      <c r="F18" s="7" t="n"/>
+      <c r="G18" s="7" t="n"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="3" t="inlineStr">
         <is>
           <t>System configuration</t>
         </is>
       </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="6" t="inlineStr">
-        <is>
-          <t>License File</t>
-        </is>
-      </c>
-      <c r="B19" s="7" t="n"/>
-      <c r="C19" s="7" t="n"/>
-      <c r="D19" s="7" t="n"/>
-      <c r="E19" s="7" t="n"/>
-      <c r="F19" s="7" t="n"/>
-      <c r="G19" s="7" t="n"/>
     </row>
     <row r="20">
       <c r="A20" s="6" t="inlineStr">
         <is>
-          <t>Deploy Configuration File</t>
+          <t>License File</t>
         </is>
       </c>
       <c r="B20" s="7" t="n"/>
@@ -9587,45 +9636,89 @@
       <c r="G20" s="7" t="n"/>
     </row>
     <row r="21">
-      <c r="A21" s="6" t="inlineStr">
+      <c r="A21" s="8" t="inlineStr">
+        <is>
+          <t>Remote License File Location</t>
+        </is>
+      </c>
+      <c r="B21" s="9" t="n"/>
+      <c r="C21" s="9" t="n"/>
+      <c r="D21" s="9" t="n"/>
+      <c r="E21" s="9" t="n"/>
+      <c r="F21" s="9" t="n"/>
+      <c r="G21" s="9" t="n"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="6" t="inlineStr">
+        <is>
+          <t>Deploy Configuration File</t>
+        </is>
+      </c>
+      <c r="B22" s="7" t="n"/>
+      <c r="C22" s="7" t="n"/>
+      <c r="D22" s="7" t="n"/>
+      <c r="E22" s="7" t="n"/>
+      <c r="F22" s="7" t="n"/>
+      <c r="G22" s="7" t="n"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="6" t="inlineStr">
         <is>
           <t>Config File Directory</t>
         </is>
       </c>
-      <c r="B21" s="7" t="n"/>
-      <c r="C21" s="7" t="n"/>
-      <c r="D21" s="7" t="n"/>
-      <c r="E21" s="7" t="n"/>
-      <c r="F21" s="7" t="n"/>
-      <c r="G21" s="7" t="n"/>
-    </row>
-    <row r="22">
-      <c r="A22" s="8" t="inlineStr">
+      <c r="B23" s="7" t="n"/>
+      <c r="C23" s="7" t="n"/>
+      <c r="D23" s="7" t="n"/>
+      <c r="E23" s="7" t="n"/>
+      <c r="F23" s="7" t="n"/>
+      <c r="G23" s="7" t="n"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="8" t="inlineStr">
         <is>
           <t>Credentials set name</t>
         </is>
       </c>
-      <c r="B22" s="9" t="n"/>
-      <c r="C22" s="9" t="n"/>
-      <c r="D22" s="9" t="n"/>
-      <c r="E22" s="9" t="n"/>
-      <c r="F22" s="9" t="n"/>
-      <c r="G22" s="9" t="n"/>
+      <c r="B24" s="9" t="n"/>
+      <c r="C24" s="9" t="n"/>
+      <c r="D24" s="9" t="n"/>
+      <c r="E24" s="9" t="n"/>
+      <c r="F24" s="9" t="n"/>
+      <c r="G24" s="9" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A4:G4"/>
-    <mergeCell ref="A8:G8"/>
-    <mergeCell ref="A15:G15"/>
-    <mergeCell ref="A18:G18"/>
+    <mergeCell ref="A9:G9"/>
+    <mergeCell ref="A16:G16"/>
+    <mergeCell ref="A19:G19"/>
   </mergeCells>
-  <dataValidations count="6">
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B11" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="C11" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="D11" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="E11" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="F11" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="G11" type="whole"/>
+  <dataValidations count="12">
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="B7" type="list">
+      <formula1>"kvm"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="C7" type="list">
+      <formula1>"kvm"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="D7" type="list">
+      <formula1>"kvm"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="E7" type="list">
+      <formula1>"kvm"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="F7" type="list">
+      <formula1>"kvm"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="G7" type="list">
+      <formula1>"kvm"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B12" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="C12" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="D12" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="E12" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="F12" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="G12" type="whole"/>
   </dataValidations>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <legacyDrawing r:id="anysvml"/>

</xml_diff>

<commit_message>
Update schema and add ignore errors when looking for database backups
</commit_message>
<xml_diff>
--- a/examples/excel/active_standby_vsds.xlsx
+++ b/examples/excel/active_standby_vsds.xlsx
@@ -857,6 +857,8 @@
     <author>sdwan_portal_secure</author>
     <author>portal_version</author>
     <author>upgrade_portal</author>
+    <author>skip_portal_db_backup</author>
+    <author>skip_portal_snapshot</author>
   </authors>
   <commentList>
     <comment authorId="0" ref="A5" shapeId="0">
@@ -947,6 +949,16 @@
     <comment authorId="17" ref="A26" shapeId="0">
       <text>
         <t>Flag to indicate whether to upgrade the SD-WAN Portal(s) [default: False]</t>
+      </text>
+    </comment>
+    <comment authorId="18" ref="A27" shapeId="0">
+      <text>
+        <t>Flag to indicate whether to backup the SD-WAN Portal database [default: False]</t>
+      </text>
+    </comment>
+    <comment authorId="19" ref="A28" shapeId="0">
+      <text>
+        <t>Flag to indicate whether to snapshot the SD-WAN Portal VM prior to upgrade [default: False]</t>
       </text>
     </comment>
   </commentList>
@@ -6014,7 +6026,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6314,6 +6326,32 @@
       <c r="F26" s="7" t="n"/>
       <c r="G26" s="7" t="n"/>
     </row>
+    <row r="27">
+      <c r="A27" s="6" t="inlineStr">
+        <is>
+          <t>Skip Portal Database Backup</t>
+        </is>
+      </c>
+      <c r="B27" s="7" t="n"/>
+      <c r="C27" s="7" t="n"/>
+      <c r="D27" s="7" t="n"/>
+      <c r="E27" s="7" t="n"/>
+      <c r="F27" s="7" t="n"/>
+      <c r="G27" s="7" t="n"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="6" t="inlineStr">
+        <is>
+          <t>Skip Portal VM Snapshot</t>
+        </is>
+      </c>
+      <c r="B28" s="7" t="n"/>
+      <c r="C28" s="7" t="n"/>
+      <c r="D28" s="7" t="n"/>
+      <c r="E28" s="7" t="n"/>
+      <c r="F28" s="7" t="n"/>
+      <c r="G28" s="7" t="n"/>
+    </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A4:G4"/>
@@ -6322,7 +6360,7 @@
     <mergeCell ref="A19:G19"/>
     <mergeCell ref="A23:G23"/>
   </mergeCells>
-  <dataValidations count="36">
+  <dataValidations count="48">
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B7" type="whole"/>
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="C7" type="whole"/>
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="D7" type="whole"/>
@@ -6405,6 +6443,42 @@
       <formula1>"true,false"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="G26" type="list">
+      <formula1>"true,false"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="B27" type="list">
+      <formula1>"true,false"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="C27" type="list">
+      <formula1>"true,false"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="D27" type="list">
+      <formula1>"true,false"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="E27" type="list">
+      <formula1>"true,false"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="F27" type="list">
+      <formula1>"true,false"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="G27" type="list">
+      <formula1>"true,false"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="B28" type="list">
+      <formula1>"true,false"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="C28" type="list">
+      <formula1>"true,false"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="D28" type="list">
+      <formula1>"true,false"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="E28" type="list">
+      <formula1>"true,false"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="F28" type="list">
+      <formula1>"true,false"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="G28" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Move portal upgrade parameters
</commit_message>
<xml_diff>
--- a/examples/excel/active_standby_vsds.xlsx
+++ b/examples/excel/active_standby_vsds.xlsx
@@ -856,8 +856,6 @@
     <author>smtp_secure</author>
     <author>sdwan_portal_secure</author>
     <author>portal_version</author>
-    <author>upgrade_portal</author>
-    <author>skip_portal_db_backup</author>
     <author>skip_portal_snapshot</author>
   </authors>
   <commentList>
@@ -947,16 +945,6 @@
       </text>
     </comment>
     <comment authorId="17" ref="A26" shapeId="0">
-      <text>
-        <t>Flag to indicate whether to upgrade the SD-WAN Portal(s) [default: False]</t>
-      </text>
-    </comment>
-    <comment authorId="18" ref="A27" shapeId="0">
-      <text>
-        <t>Flag to indicate whether to backup the SD-WAN Portal database [default: False]</t>
-      </text>
-    </comment>
-    <comment authorId="19" ref="A28" shapeId="0">
       <text>
         <t>Flag to indicate whether to snapshot the SD-WAN Portal VM prior to upgrade [default: False]</t>
       </text>
@@ -2398,6 +2386,8 @@
     <author>upgrade_to_version</author>
     <author>backup_vsd_host_file</author>
     <author>force_vsc_standalone_upgrade</author>
+    <author>upgrade_portal</author>
+    <author>skip_portal_db_backup</author>
   </authors>
   <commentList>
     <comment authorId="0" ref="A5" shapeId="0">
@@ -2423,6 +2413,16 @@
     <comment authorId="4" ref="A9" shapeId="0">
       <text>
         <t>Force all the vscs to deploy in standalone mode, otherwise the vscs will be deployed in ha mode if there are more than one vscs [default: False]</t>
+      </text>
+    </comment>
+    <comment authorId="5" ref="A10" shapeId="0">
+      <text>
+        <t>Upgrade the SD-WAN Portal or Cluster [default: False]</t>
+      </text>
+    </comment>
+    <comment authorId="6" ref="A11" shapeId="0">
+      <text>
+        <t>Flag to indicate if the SD-WAN Portal database backup should be skipped [default: False]</t>
       </text>
     </comment>
   </commentList>
@@ -6026,7 +6026,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6316,7 +6316,7 @@
     <row r="26">
       <c r="A26" s="6" t="inlineStr">
         <is>
-          <t>Upgrade Portal</t>
+          <t>Skip Portal VM Snapshot</t>
         </is>
       </c>
       <c r="B26" s="7" t="n"/>
@@ -6325,32 +6325,6 @@
       <c r="E26" s="7" t="n"/>
       <c r="F26" s="7" t="n"/>
       <c r="G26" s="7" t="n"/>
-    </row>
-    <row r="27">
-      <c r="A27" s="6" t="inlineStr">
-        <is>
-          <t>Skip Portal Database Backup</t>
-        </is>
-      </c>
-      <c r="B27" s="7" t="n"/>
-      <c r="C27" s="7" t="n"/>
-      <c r="D27" s="7" t="n"/>
-      <c r="E27" s="7" t="n"/>
-      <c r="F27" s="7" t="n"/>
-      <c r="G27" s="7" t="n"/>
-    </row>
-    <row r="28">
-      <c r="A28" s="6" t="inlineStr">
-        <is>
-          <t>Skip Portal VM Snapshot</t>
-        </is>
-      </c>
-      <c r="B28" s="7" t="n"/>
-      <c r="C28" s="7" t="n"/>
-      <c r="D28" s="7" t="n"/>
-      <c r="E28" s="7" t="n"/>
-      <c r="F28" s="7" t="n"/>
-      <c r="G28" s="7" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -6360,7 +6334,7 @@
     <mergeCell ref="A19:G19"/>
     <mergeCell ref="A23:G23"/>
   </mergeCells>
-  <dataValidations count="48">
+  <dataValidations count="36">
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B7" type="whole"/>
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="C7" type="whole"/>
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="D7" type="whole"/>
@@ -6443,42 +6417,6 @@
       <formula1>"true,false"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="G26" type="list">
-      <formula1>"true,false"</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="B27" type="list">
-      <formula1>"true,false"</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="C27" type="list">
-      <formula1>"true,false"</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="D27" type="list">
-      <formula1>"true,false"</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="E27" type="list">
-      <formula1>"true,false"</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="F27" type="list">
-      <formula1>"true,false"</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="G27" type="list">
-      <formula1>"true,false"</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="B28" type="list">
-      <formula1>"true,false"</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="C28" type="list">
-      <formula1>"true,false"</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="D28" type="list">
-      <formula1>"true,false"</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="E28" type="list">
-      <formula1>"true,false"</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="F28" type="list">
-      <formula1>"true,false"</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="G28" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
   </dataValidations>
@@ -10007,7 +9945,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10080,15 +10018,37 @@
       </c>
       <c r="B9" s="7" t="n"/>
     </row>
+    <row r="10">
+      <c r="A10" s="6" t="inlineStr">
+        <is>
+          <t>Upgrade SD-WAN Portal(s)</t>
+        </is>
+      </c>
+      <c r="B10" s="7" t="n"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="6" t="inlineStr">
+        <is>
+          <t>Skip SD-WAN Portal Database Backup</t>
+        </is>
+      </c>
+      <c r="B11" s="7" t="n"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A4:B4"/>
   </mergeCells>
-  <dataValidations count="2">
+  <dataValidations count="4">
     <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="B8" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="B9" type="list">
+      <formula1>"true,false"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="B10" type="list">
+      <formula1>"true,false"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="B11" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Refactor health and preupgrade checks, add health endpoint checks during ha deploy/upgrade
</commit_message>
<xml_diff>
--- a/examples/excel/active_standby_vsds.xlsx
+++ b/examples/excel/active_standby_vsds.xlsx
@@ -2387,7 +2387,6 @@
     <author>backup_vsd_host_file</author>
     <author>force_vsc_standalone_upgrade</author>
     <author>upgrade_portal</author>
-    <author>skip_portal_db_backup</author>
   </authors>
   <commentList>
     <comment authorId="0" ref="A5" shapeId="0">
@@ -2418,11 +2417,6 @@
     <comment authorId="5" ref="A10" shapeId="0">
       <text>
         <t>Upgrade the SD-WAN Portal or Cluster [default: False]</t>
-      </text>
-    </comment>
-    <comment authorId="6" ref="A11" shapeId="0">
-      <text>
-        <t>Flag to indicate if the SD-WAN Portal database backup should be skipped [default: False]</t>
       </text>
     </comment>
   </commentList>
@@ -9945,7 +9939,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10026,19 +10020,11 @@
       </c>
       <c r="B10" s="7" t="n"/>
     </row>
-    <row r="11">
-      <c r="A11" s="6" t="inlineStr">
-        <is>
-          <t>Skip SD-WAN Portal Database Backup</t>
-        </is>
-      </c>
-      <c r="B11" s="7" t="n"/>
-    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A4:B4"/>
   </mergeCells>
-  <dataValidations count="4">
+  <dataValidations count="3">
     <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="B8" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
@@ -10046,9 +10032,6 @@
       <formula1>"true,false"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="B10" type="list">
-      <formula1>"true,false"</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="B11" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Update documentation and menu; add portal upgrade to upgrade everything
</commit_message>
<xml_diff>
--- a/examples/excel/active_standby_vsds.xlsx
+++ b/examples/excel/active_standby_vsds.xlsx
@@ -343,6 +343,8 @@
     <author>provision_vpc_nsg_wan_subnet_cidr</author>
     <author>provision_vpc_nsg_lan_subnet_cidr</author>
     <author>provision_vpc_private_subnet_cidr</author>
+    <author>deploy_only_nsgv</author>
+    <author>proxy_external_ip</author>
     <author>nsg_organization</author>
     <author>nsg_name</author>
     <author>match_type</author>
@@ -511,107 +513,117 @@
         <t>Private Subnet CIDR for provisioning a VPC for the NSGv on AWS [default: ]</t>
       </text>
     </comment>
-    <comment authorId="29" ref="A40" shapeId="0">
+    <comment authorId="29" ref="A39" shapeId="0">
+      <text>
+        <t>Whether all components are being deployed on AWS or only the NSGv. Only needed when provision_vpc parameters are provided [default: false]</t>
+      </text>
+    </comment>
+    <comment authorId="30" ref="A40" shapeId="0">
+      <text>
+        <t>Externally routable IP address of the VNSUtil VM or the NUH used as a proxy for the NSGv on AWS. Required when deploying only the NSGv on AWS [default: ]</t>
+      </text>
+    </comment>
+    <comment authorId="31" ref="A42" shapeId="0">
       <text>
         <t>Organization on the VSD to associate with the NSG being bootstrapped, overrides global setting. [default: ]</t>
       </text>
     </comment>
-    <comment authorId="30" ref="A41" shapeId="0">
+    <comment authorId="32" ref="A43" shapeId="0">
       <text>
         <t>Name of the NSG on the VSD [default: ]</t>
       </text>
     </comment>
-    <comment authorId="31" ref="A42" shapeId="0">
+    <comment authorId="33" ref="A44" shapeId="0">
       <text>
         <t>Field type to match against for NSGv activation. [default: none]</t>
       </text>
     </comment>
-    <comment authorId="32" ref="A43" shapeId="0">
+    <comment authorId="34" ref="A45" shapeId="0">
       <text>
         <t>Value to match against for NSGv activation. [default: ]</t>
       </text>
     </comment>
-    <comment authorId="33" ref="A44" shapeId="0">
+    <comment authorId="35" ref="A46" shapeId="0">
       <text>
         <t>Enables SSH on NSGv when set. [default: False]</t>
       </text>
     </comment>
-    <comment authorId="34" ref="A46" shapeId="0">
+    <comment authorId="36" ref="A48" shapeId="0">
       <text>
         <t>Name of the NSG infra profile template on the VSD [default: ]</t>
       </text>
     </comment>
-    <comment authorId="35" ref="A47" shapeId="0">
+    <comment authorId="37" ref="A49" shapeId="0">
       <text>
         <t>Name of the NSG infra profile on the VSD [default: ]</t>
       </text>
     </comment>
-    <comment authorId="36" ref="A48" shapeId="0">
+    <comment authorId="38" ref="A50" shapeId="0">
       <text>
         <t>Name of the NSG infra profile proxy DNS on the VSD [default: ]</t>
       </text>
     </comment>
-    <comment authorId="37" ref="A49" shapeId="0">
+    <comment authorId="39" ref="A51" shapeId="0">
       <text>
         <t>Allows NSGs using this profile to override SSH access. [default: False]</t>
       </text>
     </comment>
-    <comment authorId="38" ref="A51" shapeId="0">
+    <comment authorId="40" ref="A53" shapeId="0">
       <text>
         <t>Name of the VSC infra profile for the NSG on the VSD [default: ]</t>
       </text>
     </comment>
-    <comment authorId="39" ref="A52" shapeId="0">
+    <comment authorId="41" ref="A54" shapeId="0">
       <text>
         <t>Host name or IP address of the VSC infra profile first controller for the NSG [default: ]</t>
       </text>
     </comment>
-    <comment authorId="40" ref="A53" shapeId="0">
+    <comment authorId="42" ref="A55" shapeId="0">
       <text>
         <t>Host name or IP address of the VSC infra profile second controller for the NSG [default: ]</t>
       </text>
     </comment>
-    <comment authorId="41" ref="A54" shapeId="0">
+    <comment authorId="43" ref="A56" shapeId="0">
       <text>
         <t>Name of the network port for the NSG [default: ]</t>
       </text>
     </comment>
-    <comment authorId="42" ref="A56" shapeId="0">
+    <comment authorId="44" ref="A58" shapeId="0">
       <text>
         <t>Physical name of the network port for the NSG [default: port1]</t>
       </text>
     </comment>
-    <comment authorId="43" ref="A57" shapeId="0">
+    <comment authorId="45" ref="A59" shapeId="0">
       <text>
         <t>Name of the access port for the NSG. Deprecated in favor of access_ports [default: ]</t>
       </text>
     </comment>
-    <comment authorId="44" ref="A58" shapeId="0">
+    <comment authorId="46" ref="A60" shapeId="0">
       <text>
         <t>Physical name of the access port for the NSG. Deprecated in favor of access_ports [default: port2]</t>
       </text>
     </comment>
-    <comment authorId="45" ref="A59" shapeId="0">
+    <comment authorId="47" ref="A61" shapeId="0">
       <text>
         <t>VLAN range of the access port for the NSG. Deprecated in favor of access_ports [default: ]</t>
       </text>
     </comment>
-    <comment authorId="46" ref="A60" shapeId="0">
+    <comment authorId="48" ref="A62" shapeId="0">
       <text>
         <t>VLAN number of the NSG access port for the NSG. Deprecated in favor of access_ports [default: 0]</t>
       </text>
     </comment>
-    <comment authorId="47" ref="A61" shapeId="0">
+    <comment authorId="49" ref="A63" shapeId="0">
       <text>
         <t>Name of access ports list. (List items separated by comma.)</t>
       </text>
     </comment>
-    <comment authorId="48" ref="A63" shapeId="0">
+    <comment authorId="50" ref="A65" shapeId="0">
       <text>
         <t>The port for telnet to HV host to access NSGv serial or console terminal [default: 2300]</t>
       </text>
     </comment>
-    <comment authorId="49" ref="A64" shapeId="0">
+    <comment authorId="51" ref="A66" shapeId="0">
       <text>
         <t>Name of the credentials set for the vsd</t>
       </text>
@@ -856,7 +868,6 @@
     <author>smtp_secure</author>
     <author>sdwan_portal_secure</author>
     <author>portal_version</author>
-    <author>skip_portal_snapshot</author>
   </authors>
   <commentList>
     <comment authorId="0" ref="A5" shapeId="0">
@@ -942,11 +953,6 @@
     <comment authorId="16" ref="A25" shapeId="0">
       <text>
         <t>Portal version to be pulled from Docker hub [default: ]</t>
-      </text>
-    </comment>
-    <comment authorId="17" ref="A26" shapeId="0">
-      <text>
-        <t>Flag to indicate whether to snapshot the SD-WAN Portal VM prior to upgrade [default: False]</t>
       </text>
     </comment>
   </commentList>
@@ -4410,7 +4416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G64"/>
+  <dimension ref="A1:G66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4861,16 +4867,22 @@
       <c r="G38" s="9" t="n"/>
     </row>
     <row r="39">
-      <c r="A39" s="3" t="inlineStr">
-        <is>
-          <t>NSGv Zero-Factor Bootstrap</t>
-        </is>
-      </c>
+      <c r="A39" s="8" t="inlineStr">
+        <is>
+          <t>Deploy Only NSGv on AWS</t>
+        </is>
+      </c>
+      <c r="B39" s="9" t="n"/>
+      <c r="C39" s="9" t="n"/>
+      <c r="D39" s="9" t="n"/>
+      <c r="E39" s="9" t="n"/>
+      <c r="F39" s="9" t="n"/>
+      <c r="G39" s="9" t="n"/>
     </row>
     <row r="40">
       <c r="A40" s="8" t="inlineStr">
         <is>
-          <t>NSG Organization</t>
+          <t>Proxy IP Address</t>
         </is>
       </c>
       <c r="B40" s="9" t="n"/>
@@ -4881,68 +4893,68 @@
       <c r="G40" s="9" t="n"/>
     </row>
     <row r="41">
-      <c r="A41" s="8" t="inlineStr">
+      <c r="A41" s="3" t="inlineStr">
+        <is>
+          <t>NSGv Zero-Factor Bootstrap</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="8" t="inlineStr">
+        <is>
+          <t>NSG Organization</t>
+        </is>
+      </c>
+      <c r="B42" s="9" t="n"/>
+      <c r="C42" s="9" t="n"/>
+      <c r="D42" s="9" t="n"/>
+      <c r="E42" s="9" t="n"/>
+      <c r="F42" s="9" t="n"/>
+      <c r="G42" s="9" t="n"/>
+    </row>
+    <row r="43">
+      <c r="A43" s="8" t="inlineStr">
         <is>
           <t>NSG Name</t>
         </is>
       </c>
-      <c r="B41" s="9" t="n"/>
-      <c r="C41" s="9" t="n"/>
-      <c r="D41" s="9" t="n"/>
-      <c r="E41" s="9" t="n"/>
-      <c r="F41" s="9" t="n"/>
-      <c r="G41" s="9" t="n"/>
-    </row>
-    <row r="42">
-      <c r="A42" s="6" t="inlineStr">
+      <c r="B43" s="9" t="n"/>
+      <c r="C43" s="9" t="n"/>
+      <c r="D43" s="9" t="n"/>
+      <c r="E43" s="9" t="n"/>
+      <c r="F43" s="9" t="n"/>
+      <c r="G43" s="9" t="n"/>
+    </row>
+    <row r="44">
+      <c r="A44" s="6" t="inlineStr">
         <is>
           <t>Activation Matching Type</t>
         </is>
       </c>
-      <c r="B42" s="7" t="n"/>
-      <c r="C42" s="7" t="n"/>
-      <c r="D42" s="7" t="n"/>
-      <c r="E42" s="7" t="n"/>
-      <c r="F42" s="7" t="n"/>
-      <c r="G42" s="7" t="n"/>
-    </row>
-    <row r="43">
-      <c r="A43" s="6" t="inlineStr">
+      <c r="B44" s="7" t="n"/>
+      <c r="C44" s="7" t="n"/>
+      <c r="D44" s="7" t="n"/>
+      <c r="E44" s="7" t="n"/>
+      <c r="F44" s="7" t="n"/>
+      <c r="G44" s="7" t="n"/>
+    </row>
+    <row r="45">
+      <c r="A45" s="6" t="inlineStr">
         <is>
           <t>Activation Matching Value</t>
         </is>
       </c>
-      <c r="B43" s="7" t="n"/>
-      <c r="C43" s="7" t="n"/>
-      <c r="D43" s="7" t="n"/>
-      <c r="E43" s="7" t="n"/>
-      <c r="F43" s="7" t="n"/>
-      <c r="G43" s="7" t="n"/>
-    </row>
-    <row r="44">
-      <c r="A44" s="8" t="inlineStr">
-        <is>
-          <t>Enable SSH on NSGv</t>
-        </is>
-      </c>
-      <c r="B44" s="9" t="n"/>
-      <c r="C44" s="9" t="n"/>
-      <c r="D44" s="9" t="n"/>
-      <c r="E44" s="9" t="n"/>
-      <c r="F44" s="9" t="n"/>
-      <c r="G44" s="9" t="n"/>
-    </row>
-    <row r="45">
-      <c r="A45" s="3" t="inlineStr">
-        <is>
-          <t>NSG Advanced Options</t>
-        </is>
-      </c>
+      <c r="B45" s="7" t="n"/>
+      <c r="C45" s="7" t="n"/>
+      <c r="D45" s="7" t="n"/>
+      <c r="E45" s="7" t="n"/>
+      <c r="F45" s="7" t="n"/>
+      <c r="G45" s="7" t="n"/>
     </row>
     <row r="46">
       <c r="A46" s="8" t="inlineStr">
         <is>
-          <t>NSG Infra Profile Template Name</t>
+          <t>Enable SSH on NSGv</t>
         </is>
       </c>
       <c r="B46" s="9" t="n"/>
@@ -4953,22 +4965,16 @@
       <c r="G46" s="9" t="n"/>
     </row>
     <row r="47">
-      <c r="A47" s="8" t="inlineStr">
-        <is>
-          <t>NSG Infra Profile Name</t>
-        </is>
-      </c>
-      <c r="B47" s="9" t="n"/>
-      <c r="C47" s="9" t="n"/>
-      <c r="D47" s="9" t="n"/>
-      <c r="E47" s="9" t="n"/>
-      <c r="F47" s="9" t="n"/>
-      <c r="G47" s="9" t="n"/>
+      <c r="A47" s="3" t="inlineStr">
+        <is>
+          <t>NSG Advanced Options</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="8" t="inlineStr">
         <is>
-          <t>NSG Infra Profile Proxy DNS Name</t>
+          <t>NSG Infra Profile Template Name</t>
         </is>
       </c>
       <c r="B48" s="9" t="n"/>
@@ -4981,7 +4987,7 @@
     <row r="49">
       <c r="A49" s="8" t="inlineStr">
         <is>
-          <t>Allow SSH Access Override</t>
+          <t>NSG Infra Profile Name</t>
         </is>
       </c>
       <c r="B49" s="9" t="n"/>
@@ -4992,16 +4998,22 @@
       <c r="G49" s="9" t="n"/>
     </row>
     <row r="50">
-      <c r="A50" s="3" t="inlineStr">
-        <is>
-          <t>VSC Info</t>
-        </is>
-      </c>
+      <c r="A50" s="8" t="inlineStr">
+        <is>
+          <t>NSG Infra Profile Proxy DNS Name</t>
+        </is>
+      </c>
+      <c r="B50" s="9" t="n"/>
+      <c r="C50" s="9" t="n"/>
+      <c r="D50" s="9" t="n"/>
+      <c r="E50" s="9" t="n"/>
+      <c r="F50" s="9" t="n"/>
+      <c r="G50" s="9" t="n"/>
     </row>
     <row r="51">
       <c r="A51" s="8" t="inlineStr">
         <is>
-          <t>VSC Infra Profile Name</t>
+          <t>Allow SSH Access Override</t>
         </is>
       </c>
       <c r="B51" s="9" t="n"/>
@@ -5012,22 +5024,16 @@
       <c r="G51" s="9" t="n"/>
     </row>
     <row r="52">
-      <c r="A52" s="8" t="inlineStr">
-        <is>
-          <t>VSC Infra Profile First Controller</t>
-        </is>
-      </c>
-      <c r="B52" s="9" t="n"/>
-      <c r="C52" s="9" t="n"/>
-      <c r="D52" s="9" t="n"/>
-      <c r="E52" s="9" t="n"/>
-      <c r="F52" s="9" t="n"/>
-      <c r="G52" s="9" t="n"/>
+      <c r="A52" s="3" t="inlineStr">
+        <is>
+          <t>VSC Info</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="8" t="inlineStr">
         <is>
-          <t>VSC Infra Profile Second Controller</t>
+          <t>VSC Infra Profile Name</t>
         </is>
       </c>
       <c r="B53" s="9" t="n"/>
@@ -5040,7 +5046,7 @@
     <row r="54">
       <c r="A54" s="8" t="inlineStr">
         <is>
-          <t>NSG Network Port Name</t>
+          <t>VSC Infra Profile First Controller</t>
         </is>
       </c>
       <c r="B54" s="9" t="n"/>
@@ -5051,16 +5057,22 @@
       <c r="G54" s="9" t="n"/>
     </row>
     <row r="55">
-      <c r="A55" s="3" t="inlineStr">
-        <is>
-          <t>Network and Access Ports</t>
-        </is>
-      </c>
+      <c r="A55" s="8" t="inlineStr">
+        <is>
+          <t>VSC Infra Profile Second Controller</t>
+        </is>
+      </c>
+      <c r="B55" s="9" t="n"/>
+      <c r="C55" s="9" t="n"/>
+      <c r="D55" s="9" t="n"/>
+      <c r="E55" s="9" t="n"/>
+      <c r="F55" s="9" t="n"/>
+      <c r="G55" s="9" t="n"/>
     </row>
     <row r="56">
       <c r="A56" s="8" t="inlineStr">
         <is>
-          <t>NSG Network Port Physical Name</t>
+          <t>NSG Network Port Name</t>
         </is>
       </c>
       <c r="B56" s="9" t="n"/>
@@ -5071,22 +5083,16 @@
       <c r="G56" s="9" t="n"/>
     </row>
     <row r="57">
-      <c r="A57" s="8" t="inlineStr">
-        <is>
-          <t>NSG Access Port Name</t>
-        </is>
-      </c>
-      <c r="B57" s="9" t="n"/>
-      <c r="C57" s="9" t="n"/>
-      <c r="D57" s="9" t="n"/>
-      <c r="E57" s="9" t="n"/>
-      <c r="F57" s="9" t="n"/>
-      <c r="G57" s="9" t="n"/>
+      <c r="A57" s="3" t="inlineStr">
+        <is>
+          <t>Network and Access Ports</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="8" t="inlineStr">
         <is>
-          <t>NSG Access Port Physical Name</t>
+          <t>NSG Network Port Physical Name</t>
         </is>
       </c>
       <c r="B58" s="9" t="n"/>
@@ -5099,7 +5105,7 @@
     <row r="59">
       <c r="A59" s="8" t="inlineStr">
         <is>
-          <t>NSG Access Port VLAN Range</t>
+          <t>NSG Access Port Name</t>
         </is>
       </c>
       <c r="B59" s="9" t="n"/>
@@ -5112,7 +5118,7 @@
     <row r="60">
       <c r="A60" s="8" t="inlineStr">
         <is>
-          <t>NSG Access Port VLAN Number</t>
+          <t>NSG Access Port Physical Name</t>
         </is>
       </c>
       <c r="B60" s="9" t="n"/>
@@ -5123,50 +5129,76 @@
       <c r="G60" s="9" t="n"/>
     </row>
     <row r="61">
-      <c r="A61" s="6" t="inlineStr">
+      <c r="A61" s="8" t="inlineStr">
+        <is>
+          <t>NSG Access Port VLAN Range</t>
+        </is>
+      </c>
+      <c r="B61" s="9" t="n"/>
+      <c r="C61" s="9" t="n"/>
+      <c r="D61" s="9" t="n"/>
+      <c r="E61" s="9" t="n"/>
+      <c r="F61" s="9" t="n"/>
+      <c r="G61" s="9" t="n"/>
+    </row>
+    <row r="62">
+      <c r="A62" s="8" t="inlineStr">
+        <is>
+          <t>NSG Access Port VLAN Number</t>
+        </is>
+      </c>
+      <c r="B62" s="9" t="n"/>
+      <c r="C62" s="9" t="n"/>
+      <c r="D62" s="9" t="n"/>
+      <c r="E62" s="9" t="n"/>
+      <c r="F62" s="9" t="n"/>
+      <c r="G62" s="9" t="n"/>
+    </row>
+    <row r="63">
+      <c r="A63" s="6" t="inlineStr">
         <is>
           <t>NSGv Access ports list name</t>
         </is>
       </c>
-      <c r="B61" s="7" t="n"/>
-      <c r="C61" s="7" t="n"/>
-      <c r="D61" s="7" t="n"/>
-      <c r="E61" s="7" t="n"/>
-      <c r="F61" s="7" t="n"/>
-      <c r="G61" s="7" t="n"/>
-    </row>
-    <row r="62">
-      <c r="A62" s="3" t="inlineStr">
+      <c r="B63" s="7" t="n"/>
+      <c r="C63" s="7" t="n"/>
+      <c r="D63" s="7" t="n"/>
+      <c r="E63" s="7" t="n"/>
+      <c r="F63" s="7" t="n"/>
+      <c r="G63" s="7" t="n"/>
+    </row>
+    <row r="64">
+      <c r="A64" s="3" t="inlineStr">
         <is>
           <t>Telnet and Credentials</t>
         </is>
       </c>
     </row>
-    <row r="63">
-      <c r="A63" s="8" t="inlineStr">
+    <row r="65">
+      <c r="A65" s="8" t="inlineStr">
         <is>
           <t>Telnet port for console</t>
         </is>
       </c>
-      <c r="B63" s="9" t="n"/>
-      <c r="C63" s="9" t="n"/>
-      <c r="D63" s="9" t="n"/>
-      <c r="E63" s="9" t="n"/>
-      <c r="F63" s="9" t="n"/>
-      <c r="G63" s="9" t="n"/>
-    </row>
-    <row r="64">
-      <c r="A64" s="8" t="inlineStr">
+      <c r="B65" s="9" t="n"/>
+      <c r="C65" s="9" t="n"/>
+      <c r="D65" s="9" t="n"/>
+      <c r="E65" s="9" t="n"/>
+      <c r="F65" s="9" t="n"/>
+      <c r="G65" s="9" t="n"/>
+    </row>
+    <row r="66">
+      <c r="A66" s="8" t="inlineStr">
         <is>
           <t>Credentials set name</t>
         </is>
       </c>
-      <c r="B64" s="9" t="n"/>
-      <c r="C64" s="9" t="n"/>
-      <c r="D64" s="9" t="n"/>
-      <c r="E64" s="9" t="n"/>
-      <c r="F64" s="9" t="n"/>
-      <c r="G64" s="9" t="n"/>
+      <c r="B66" s="9" t="n"/>
+      <c r="C66" s="9" t="n"/>
+      <c r="D66" s="9" t="n"/>
+      <c r="E66" s="9" t="n"/>
+      <c r="F66" s="9" t="n"/>
+      <c r="G66" s="9" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -5176,13 +5208,13 @@
     <mergeCell ref="A19:G19"/>
     <mergeCell ref="A25:G25"/>
     <mergeCell ref="A34:G34"/>
-    <mergeCell ref="A39:G39"/>
-    <mergeCell ref="A45:G45"/>
-    <mergeCell ref="A50:G50"/>
-    <mergeCell ref="A55:G55"/>
-    <mergeCell ref="A62:G62"/>
+    <mergeCell ref="A41:G41"/>
+    <mergeCell ref="A47:G47"/>
+    <mergeCell ref="A52:G52"/>
+    <mergeCell ref="A57:G57"/>
+    <mergeCell ref="A64:G64"/>
   </mergeCells>
-  <dataValidations count="48">
+  <dataValidations count="54">
     <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="B6" type="list">
       <formula1>"kvm,vcenter,aws"</formula1>
     </dataValidation>
@@ -5225,72 +5257,90 @@
     <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="G10" type="list">
       <formula1>"none,zfb_metro,zfb_external,activation_link"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="B42" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="B39" type="list">
+      <formula1>"true,false"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="C39" type="list">
+      <formula1>"true,false"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="D39" type="list">
+      <formula1>"true,false"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="E39" type="list">
+      <formula1>"true,false"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="F39" type="list">
+      <formula1>"true,false"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="G39" type="list">
+      <formula1>"true,false"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="B44" type="list">
       <formula1>"none,hostname,ip_address,mac_address,nsgateway_id,serial_number,uuid"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="C42" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="C44" type="list">
       <formula1>"none,hostname,ip_address,mac_address,nsgateway_id,serial_number,uuid"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="D42" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="D44" type="list">
       <formula1>"none,hostname,ip_address,mac_address,nsgateway_id,serial_number,uuid"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="E42" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="E44" type="list">
       <formula1>"none,hostname,ip_address,mac_address,nsgateway_id,serial_number,uuid"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="F42" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="F44" type="list">
       <formula1>"none,hostname,ip_address,mac_address,nsgateway_id,serial_number,uuid"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="G42" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="G44" type="list">
       <formula1>"none,hostname,ip_address,mac_address,nsgateway_id,serial_number,uuid"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="B44" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="B46" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="C44" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="C46" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="D44" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="D46" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="E44" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="E46" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="F44" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="F46" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="G44" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="G46" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="B49" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="B51" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="C49" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="C51" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="D49" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="D51" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="E49" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="E51" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="F49" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="F51" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="G49" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="G51" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B60" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="C60" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="D60" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="E60" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="F60" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="G60" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B63" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="C63" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="D63" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="E63" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="F63" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="G63" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B62" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="C62" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="D62" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="E62" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="F62" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="G62" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B65" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="C65" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="D65" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="E65" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="F65" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="G65" type="whole"/>
   </dataValidations>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <legacyDrawing r:id="anysvml"/>
@@ -6020,7 +6070,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6307,19 +6357,6 @@
       <c r="F25" s="7" t="n"/>
       <c r="G25" s="7" t="n"/>
     </row>
-    <row r="26">
-      <c r="A26" s="6" t="inlineStr">
-        <is>
-          <t>Skip Portal VM Snapshot</t>
-        </is>
-      </c>
-      <c r="B26" s="7" t="n"/>
-      <c r="C26" s="7" t="n"/>
-      <c r="D26" s="7" t="n"/>
-      <c r="E26" s="7" t="n"/>
-      <c r="F26" s="7" t="n"/>
-      <c r="G26" s="7" t="n"/>
-    </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A4:G4"/>
@@ -6328,7 +6365,7 @@
     <mergeCell ref="A19:G19"/>
     <mergeCell ref="A23:G23"/>
   </mergeCells>
-  <dataValidations count="36">
+  <dataValidations count="30">
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B7" type="whole"/>
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="C7" type="whole"/>
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="D7" type="whole"/>
@@ -6393,24 +6430,6 @@
       <formula1>"true,false"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="G24" type="list">
-      <formula1>"true,false"</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="B26" type="list">
-      <formula1>"true,false"</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="C26" type="list">
-      <formula1>"true,false"</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="D26" type="list">
-      <formula1>"true,false"</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="E26" type="list">
-      <formula1>"true,false"</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="F26" type="list">
-      <formula1>"true,false"</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="G26" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Add skip disable stats collection
</commit_message>
<xml_diff>
--- a/examples/excel/active_standby_vsds.xlsx
+++ b/examples/excel/active_standby_vsds.xlsx
@@ -2397,6 +2397,7 @@
     <author>upgrade_from_version</author>
     <author>upgrade_to_version</author>
     <author>backup_vsd_host_file</author>
+    <author>skip_disable_stats_collection</author>
     <author>force_vsc_standalone_upgrade</author>
     <author>upgrade_portal</author>
   </authors>
@@ -2423,10 +2424,15 @@
     </comment>
     <comment authorId="4" ref="A9" shapeId="0">
       <text>
+        <t>Stats collection should be disabled during VSD upgrade. If for some reason, you would like to disable stats collection outside of MetroAE, change this to true. [default: False]</t>
+      </text>
+    </comment>
+    <comment authorId="5" ref="A10" shapeId="0">
+      <text>
         <t>Force all the vscs to deploy in standalone mode, otherwise the vscs will be deployed in ha mode if there are more than one vscs [default: False]</t>
       </text>
     </comment>
-    <comment authorId="5" ref="A10" shapeId="0">
+    <comment authorId="6" ref="A11" shapeId="0">
       <text>
         <t>Upgrade the SD-WAN Portal or Cluster [default: False]</t>
       </text>
@@ -9975,7 +9981,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10041,26 +10047,34 @@
       <c r="B8" s="9" t="n"/>
     </row>
     <row r="9">
-      <c r="A9" s="6" t="inlineStr">
-        <is>
-          <t>Force vscs standalone</t>
-        </is>
-      </c>
-      <c r="B9" s="7" t="n"/>
+      <c r="A9" s="8" t="inlineStr">
+        <is>
+          <t>Skip stats collection disable before upgrade</t>
+        </is>
+      </c>
+      <c r="B9" s="9" t="n"/>
     </row>
     <row r="10">
       <c r="A10" s="6" t="inlineStr">
         <is>
+          <t>Force vscs standalone</t>
+        </is>
+      </c>
+      <c r="B10" s="7" t="n"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="6" t="inlineStr">
+        <is>
           <t>Upgrade SD-WAN Portal(s)</t>
         </is>
       </c>
-      <c r="B10" s="7" t="n"/>
+      <c r="B11" s="7" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A4:B4"/>
   </mergeCells>
-  <dataValidations count="3">
+  <dataValidations count="4">
     <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="B8" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
@@ -10068,6 +10082,9 @@
       <formula1>"true,false"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="B10" type="list">
+      <formula1>"true,false"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="B11" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Generate all from schema
</commit_message>
<xml_diff>
--- a/examples/excel/active_standby_vsds.xlsx
+++ b/examples/excel/active_standby_vsds.xlsx
@@ -2339,6 +2339,8 @@
     <author>target_server_type</author>
     <author>target_server</author>
     <author>cpuset</author>
+    <author>cert_name</author>
+    <author>run_incompass_operation</author>
   </authors>
   <commentList>
     <comment authorId="0" ref="A5" shapeId="0">
@@ -2384,6 +2386,16 @@
     <comment authorId="8" ref="A14" shapeId="0">
       <text>
         <t>Cpuset information for cpu pinning on KVM. For example, Webfilter requires 2 cores and sample values will be of the form [1, 2] (List items separated by comma.)</t>
+      </text>
+    </comment>
+    <comment authorId="9" ref="A16" shapeId="0">
+      <text>
+        <t>Certificate Username</t>
+      </text>
+    </comment>
+    <comment authorId="10" ref="A17" shapeId="0">
+      <text>
+        <t>Run incompass operation command. This is enabled by default and may take up to 20 minutes and requires internet connection. [default: True]</t>
       </text>
     </comment>
   </commentList>
@@ -9789,7 +9801,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9951,12 +9963,46 @@
       <c r="F14" s="9" t="n"/>
       <c r="G14" s="9" t="n"/>
     </row>
+    <row r="15">
+      <c r="A15" s="3" t="inlineStr">
+        <is>
+          <t>Webfilter details</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="8" t="inlineStr">
+        <is>
+          <t>Certificate Username</t>
+        </is>
+      </c>
+      <c r="B16" s="9" t="n"/>
+      <c r="C16" s="9" t="n"/>
+      <c r="D16" s="9" t="n"/>
+      <c r="E16" s="9" t="n"/>
+      <c r="F16" s="9" t="n"/>
+      <c r="G16" s="9" t="n"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="8" t="inlineStr">
+        <is>
+          <t>Run incompass operation command</t>
+        </is>
+      </c>
+      <c r="B17" s="9" t="n"/>
+      <c r="C17" s="9" t="n"/>
+      <c r="D17" s="9" t="n"/>
+      <c r="E17" s="9" t="n"/>
+      <c r="F17" s="9" t="n"/>
+      <c r="G17" s="9" t="n"/>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A4:G4"/>
     <mergeCell ref="A10:G10"/>
+    <mergeCell ref="A15:G15"/>
   </mergeCells>
-  <dataValidations count="12">
+  <dataValidations count="18">
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B7" type="whole"/>
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="C7" type="whole"/>
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="D7" type="whole"/>
@@ -9980,6 +10026,24 @@
     </dataValidation>
     <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="G12" type="list">
       <formula1>"kvm"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="B17" type="list">
+      <formula1>"true,false"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="C17" type="list">
+      <formula1>"true,false"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="D17" type="list">
+      <formula1>"true,false"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="E17" type="list">
+      <formula1>"true,false"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="F17" type="list">
+      <formula1>"true,false"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="G17" type="list">
+      <formula1>"true,false"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>

<commit_message>
added schema files from jenkins job
Signed-off-by: caso <devops@nuagenetworks.net>
</commit_message>
<xml_diff>
--- a/examples/excel/active_standby_vsds.xlsx
+++ b/examples/excel/active_standby_vsds.xlsx
@@ -1,37 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Deployment" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Common" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Upgrade" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Vsds" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Vscs" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Vstats" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="Credentials" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="Dnss" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="Netconf managers" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="Nsgv access ports" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="Nsgv bootstrap" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet name="Nsgvs" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet name="Nuh common" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet name="Nuh external interfaces" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet name="Nuh vrrp" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet name="Nuhs" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet name="Portals" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet name="Proxys" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet name="Stcv global" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet name="Stcvs" sheetId="20" state="visible" r:id="rId20"/>
-    <sheet name="Vcins" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet name="Vnsutils" sheetId="22" state="visible" r:id="rId22"/>
-    <sheet name="Vrss" sheetId="23" state="visible" r:id="rId23"/>
-    <sheet name="Vsrs" sheetId="24" state="visible" r:id="rId24"/>
-    <sheet name="Webfilters" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Deployment" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Common" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Upgrade" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Vsds" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Vscs" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Vstats" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Credentials" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Dnss" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Netconf managers" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Nsgv access ports" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Nsgv bootstrap" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Nsgvs" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Nuh common" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Nuh external interfaces" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Nuh vrrp" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Nuhs" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Portals" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Proxys" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Stcv global" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Stcvs" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Vcins" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Vnsutils" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Vrss" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Vsrs" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Webfilters" sheetId="25" state="visible" r:id="rId25"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -758,6 +758,7 @@
     <author>target_server</author>
     <author>target_server_type</author>
     <author>timezone</author>
+    <author>timezone2</author>
     <author>custom_configuration_file_location</author>
     <author>skip_vsd_installed_check</author>
     <author>health_monitoring_agent</author>
@@ -831,45 +832,50 @@
     </comment>
     <comment authorId="12" ref="A20" shapeId="0">
       <text>
+        <t>Timezone of the NUH [default: America/Toronto]</t>
+      </text>
+    </comment>
+    <comment authorId="13" ref="A21" shapeId="0">
+      <text>
         <t>Optional user specified location of the yaml based configuration file for the NUH. This will replace the default yaml configuration file added by MetroAE</t>
       </text>
     </comment>
-    <comment authorId="13" ref="A21" shapeId="0">
+    <comment authorId="14" ref="A22" shapeId="0">
       <text>
         <t>Enable this option to install NUH in situations where no VSD is present [default: False]</t>
       </text>
     </comment>
-    <comment authorId="14" ref="A22" shapeId="0">
+    <comment authorId="15" ref="A23" shapeId="0">
       <text>
         <t>Enables setup of a health monitoring agent [default: none]</t>
       </text>
     </comment>
-    <comment authorId="15" ref="A23" shapeId="0">
+    <comment authorId="16" ref="A24" shapeId="0">
       <text>
         <t>Cpuset information for cpu pinning on KVM. For example, NUH requires 4 cores and sample values will be of the form [ 0, 1, 2, 3 ] (List items separated by comma.)</t>
       </text>
     </comment>
-    <comment authorId="16" ref="A25" shapeId="0">
+    <comment authorId="17" ref="A26" shapeId="0">
       <text>
         <t>Network Bridge used for the management interface on the NUH. This will be a Linux network bridge when deploying on KVM. Defaults to the global setting [default: (global Bridge interface)]</t>
       </text>
     </comment>
-    <comment authorId="17" ref="A26" shapeId="0">
+    <comment authorId="18" ref="A27" shapeId="0">
       <text>
         <t>Network Bridge used for the internal network on the NUH. This will be a Linux network bridge when deploying on KVM. Defaults to using management bridge [default: (management bridge)]</t>
       </text>
     </comment>
-    <comment authorId="18" ref="A28" shapeId="0">
+    <comment authorId="19" ref="A29" shapeId="0">
       <text>
         <t>Name of the vCenter Datacenter on which the VSD VM will be deployed. Defaults to the common vCenter Datacenter Name if not defined here. [default: (global vCenter Datacenter Name)]</t>
       </text>
     </comment>
-    <comment authorId="19" ref="A29" shapeId="0">
+    <comment authorId="20" ref="A30" shapeId="0">
       <text>
         <t>Name of the vCenter Cluster on which the VSD VM will be deployed. Defaults to the common vCenter Cluster Name if not defined here. [default: (global vCenter Cluster Name)]</t>
       </text>
     </comment>
-    <comment authorId="20" ref="A30" shapeId="0">
+    <comment authorId="21" ref="A31" shapeId="0">
       <text>
         <t>Name of the vCenter Datastore on which the VSD VM will be deployed. Defaults to the common vCenter Datastore Name if not defined here. [default: (global vCenter Datastore Name)]</t>
       </text>
@@ -4093,7 +4099,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -4152,12 +4158,12 @@
     <mergeCell ref="A4:B4"/>
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <legacyDrawing r:id="anysvml"/>
+  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -4278,12 +4284,12 @@
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="G8" type="whole"/>
   </dataValidations>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <legacyDrawing r:id="anysvml"/>
+  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -4460,12 +4466,12 @@
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B20" type="whole"/>
   </dataValidations>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <legacyDrawing r:id="anysvml"/>
+  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -5397,12 +5403,12 @@
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="G65" type="whole"/>
   </dataValidations>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <legacyDrawing r:id="anysvml"/>
+  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -5469,12 +5475,12 @@
     </dataValidation>
   </dataValidations>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <legacyDrawing r:id="anysvml"/>
+  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -5640,12 +5646,12 @@
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="G9" type="whole"/>
   </dataValidations>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <legacyDrawing r:id="anysvml"/>
+  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -5771,17 +5777,17 @@
     </dataValidation>
   </dataValidations>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <legacyDrawing r:id="anysvml"/>
+  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5999,7 +6005,7 @@
     <row r="20">
       <c r="A20" s="8" t="inlineStr">
         <is>
-          <t>Custom NUH configuration file location</t>
+          <t>Timezone 2</t>
         </is>
       </c>
       <c r="B20" s="9" t="n"/>
@@ -6012,7 +6018,7 @@
     <row r="21">
       <c r="A21" s="8" t="inlineStr">
         <is>
-          <t>Skip VSD installed check</t>
+          <t>Custom NUH configuration file location</t>
         </is>
       </c>
       <c r="B21" s="9" t="n"/>
@@ -6025,7 +6031,7 @@
     <row r="22">
       <c r="A22" s="8" t="inlineStr">
         <is>
-          <t>Health monitoring agent</t>
+          <t>Skip VSD installed check</t>
         </is>
       </c>
       <c r="B22" s="9" t="n"/>
@@ -6038,7 +6044,7 @@
     <row r="23">
       <c r="A23" s="8" t="inlineStr">
         <is>
-          <t>KVM cpuset information</t>
+          <t>Health monitoring agent</t>
         </is>
       </c>
       <c r="B23" s="9" t="n"/>
@@ -6049,62 +6055,62 @@
       <c r="G23" s="9" t="n"/>
     </row>
     <row r="24">
-      <c r="A24" s="3" t="inlineStr">
+      <c r="A24" s="8" t="inlineStr">
+        <is>
+          <t>KVM cpuset information</t>
+        </is>
+      </c>
+      <c r="B24" s="9" t="n"/>
+      <c r="C24" s="9" t="n"/>
+      <c r="D24" s="9" t="n"/>
+      <c r="E24" s="9" t="n"/>
+      <c r="F24" s="9" t="n"/>
+      <c r="G24" s="9" t="n"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="3" t="inlineStr">
         <is>
           <t>Bridge details</t>
         </is>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" s="6" t="inlineStr">
+    <row r="26">
+      <c r="A26" s="6" t="inlineStr">
         <is>
           <t>Management Network Bridge</t>
         </is>
       </c>
-      <c r="B25" s="7" t="n"/>
-      <c r="C25" s="7" t="n"/>
-      <c r="D25" s="7" t="n"/>
-      <c r="E25" s="7" t="n"/>
-      <c r="F25" s="7" t="n"/>
-      <c r="G25" s="7" t="n"/>
-    </row>
-    <row r="26">
-      <c r="A26" s="8" t="inlineStr">
+      <c r="B26" s="7" t="n"/>
+      <c r="C26" s="7" t="n"/>
+      <c r="D26" s="7" t="n"/>
+      <c r="E26" s="7" t="n"/>
+      <c r="F26" s="7" t="n"/>
+      <c r="G26" s="7" t="n"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="8" t="inlineStr">
         <is>
           <t>Internal Network Bridge</t>
         </is>
       </c>
-      <c r="B26" s="9" t="n"/>
-      <c r="C26" s="9" t="n"/>
-      <c r="D26" s="9" t="n"/>
-      <c r="E26" s="9" t="n"/>
-      <c r="F26" s="9" t="n"/>
-      <c r="G26" s="9" t="n"/>
-    </row>
-    <row r="27">
-      <c r="A27" s="3" t="inlineStr">
+      <c r="B27" s="9" t="n"/>
+      <c r="C27" s="9" t="n"/>
+      <c r="D27" s="9" t="n"/>
+      <c r="E27" s="9" t="n"/>
+      <c r="F27" s="9" t="n"/>
+      <c r="G27" s="9" t="n"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="3" t="inlineStr">
         <is>
           <t>vCenter Parameters</t>
         </is>
       </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="8" t="inlineStr">
-        <is>
-          <t>vCenter Datacenter Name</t>
-        </is>
-      </c>
-      <c r="B28" s="9" t="n"/>
-      <c r="C28" s="9" t="n"/>
-      <c r="D28" s="9" t="n"/>
-      <c r="E28" s="9" t="n"/>
-      <c r="F28" s="9" t="n"/>
-      <c r="G28" s="9" t="n"/>
     </row>
     <row r="29">
       <c r="A29" s="8" t="inlineStr">
         <is>
-          <t>vCenter Cluster Name</t>
+          <t>vCenter Datacenter Name</t>
         </is>
       </c>
       <c r="B29" s="9" t="n"/>
@@ -6117,7 +6123,7 @@
     <row r="30">
       <c r="A30" s="8" t="inlineStr">
         <is>
-          <t>vCenter Datastore Name</t>
+          <t>vCenter Cluster Name</t>
         </is>
       </c>
       <c r="B30" s="9" t="n"/>
@@ -6127,14 +6133,27 @@
       <c r="F30" s="9" t="n"/>
       <c r="G30" s="9" t="n"/>
     </row>
+    <row r="31">
+      <c r="A31" s="8" t="inlineStr">
+        <is>
+          <t>vCenter Datastore Name</t>
+        </is>
+      </c>
+      <c r="B31" s="9" t="n"/>
+      <c r="C31" s="9" t="n"/>
+      <c r="D31" s="9" t="n"/>
+      <c r="E31" s="9" t="n"/>
+      <c r="F31" s="9" t="n"/>
+      <c r="G31" s="9" t="n"/>
+    </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="A4:G4"/>
     <mergeCell ref="A7:G7"/>
     <mergeCell ref="A11:G11"/>
     <mergeCell ref="A16:G16"/>
-    <mergeCell ref="A24:G24"/>
-    <mergeCell ref="A27:G27"/>
+    <mergeCell ref="A25:G25"/>
+    <mergeCell ref="A28:G28"/>
   </mergeCells>
   <dataValidations count="30">
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B9" type="whole"/>
@@ -6167,50 +6186,50 @@
     <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="G18" type="list">
       <formula1>"kvm,vcenter,none"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="B21" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="B22" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="C21" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="C22" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="D21" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="D22" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="E21" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="E22" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="F21" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="F22" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="G21" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="G22" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="B22" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="B23" type="list">
       <formula1>"none,zabbix"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="C22" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="C23" type="list">
       <formula1>"none,zabbix"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="D22" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="D23" type="list">
       <formula1>"none,zabbix"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="E22" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="E23" type="list">
       <formula1>"none,zabbix"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="F22" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="F23" type="list">
       <formula1>"none,zabbix"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="G22" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="G23" type="list">
       <formula1>"none,zabbix"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <legacyDrawing r:id="anysvml"/>
+  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -6579,12 +6598,12 @@
     </dataValidation>
   </dataValidations>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <legacyDrawing r:id="anysvml"/>
+  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -6870,12 +6889,12 @@
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="G17" type="whole"/>
   </dataValidations>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <legacyDrawing r:id="anysvml"/>
+  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -6942,12 +6961,12 @@
     <mergeCell ref="A4:B4"/>
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <legacyDrawing r:id="anysvml"/>
+  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -8076,12 +8095,12 @@
     </dataValidation>
   </dataValidations>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <legacyDrawing r:id="anysvml"/>
+  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -8360,12 +8379,12 @@
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="G20" type="whole"/>
   </dataValidations>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <legacyDrawing r:id="anysvml"/>
+  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -8658,12 +8677,12 @@
     </dataValidation>
   </dataValidations>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <legacyDrawing r:id="anysvml"/>
+  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -9352,12 +9371,12 @@
     </dataValidation>
   </dataValidations>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <legacyDrawing r:id="anysvml"/>
+  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -9576,12 +9595,12 @@
     </dataValidation>
   </dataValidations>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <legacyDrawing r:id="anysvml"/>
+  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -9900,12 +9919,12 @@
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="G12" type="whole"/>
   </dataValidations>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <legacyDrawing r:id="anysvml"/>
+  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -10104,12 +10123,12 @@
     </dataValidation>
   </dataValidations>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <legacyDrawing r:id="anysvml"/>
+  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -10222,12 +10241,12 @@
     </dataValidation>
   </dataValidations>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <legacyDrawing r:id="anysvml"/>
+  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -11098,12 +11117,12 @@
     </dataValidation>
   </dataValidations>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <legacyDrawing r:id="anysvml"/>
+  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -11777,12 +11796,12 @@
     </dataValidation>
   </dataValidations>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <legacyDrawing r:id="anysvml"/>
+  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -12535,12 +12554,12 @@
     </dataValidation>
   </dataValidations>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <legacyDrawing r:id="anysvml"/>
+  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -13363,12 +13382,12 @@
     <mergeCell ref="A65:G65"/>
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <legacyDrawing r:id="anysvml"/>
+  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -13721,12 +13740,12 @@
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="G12" type="whole"/>
   </dataValidations>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <legacyDrawing r:id="anysvml"/>
+  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -13826,6 +13845,6 @@
     <mergeCell ref="A4:G4"/>
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <legacyDrawing r:id="anysvml"/>
+  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update titles and descriptions
</commit_message>
<xml_diff>
--- a/examples/excel/active_standby_vsds.xlsx
+++ b/examples/excel/active_standby_vsds.xlsx
@@ -1555,185 +1555,185 @@
     </comment>
     <comment authorId="67" ref="A86" shapeId="0">
       <text>
-        <t>Amount of VSD RAM to allocate, in GB. Valid only for KVM and VCenter deployments. Note: Values smaller than the default are for lab and PoC only. Production deployments must use a value greater than or equal to the default. [default: 24]</t>
+        <t>For KVM and VCenter deployments: amount of VSD RAM to allocate, in GB. Note: Values smaller than the default are for lab and PoC only. Production deployments must use a value greater than or equal to the default. [default: 24]</t>
       </text>
     </comment>
     <comment authorId="68" ref="A87" shapeId="0">
       <text>
-        <t>Amount of VSC RAM to allocate, in GB. Valid only for KVM and VCenter deployments. Note: Values smaller than the default are for lab and PoC only. Production deployments must use a value greater than or equal to the default. [default: 4]</t>
+        <t>For KVM and VCenter deployments: amount of VSC RAM to allocate, in GB. Note: Values smaller than the default are for lab and PoC only. Production deployments must use a value greater than or equal to the default. [default: 4]</t>
       </text>
     </comment>
     <comment authorId="69" ref="A88" shapeId="0">
       <text>
-        <t>Amount of VSTAT RAM to allocate, in GB. Valid only for KVM and VCenter deployments. Note: Values smaller than the default are for lab and PoC only. Production deployments must use a value greater than or equal to the default. [default: 16]</t>
-      </text>
-    </comment>
-    <comment authorId="70" ref="A89" shapeId="0">
+        <t>For KVM and VCenter deployments: amount of VSTAT RAM to allocate, in GB. Note: Values smaller than the default are for lab and PoC only. Production deployments must use a value greater than or equal to the default. [default: 16]</t>
+      </text>
+    </comment>
+    <comment authorId="70" ref="A90" shapeId="0">
       <text>
         <t>Amount of VCIN RAM to allocate, in GB. Valid only for KVM deployments. Note: Values smaller than the default are for lab and PoC only. Production deployments must use a value greater than or equal to the default. [default: 24]</t>
       </text>
     </comment>
-    <comment authorId="71" ref="A90" shapeId="0">
+    <comment authorId="71" ref="A91" shapeId="0">
       <text>
         <t>Amount of NUH RAM to allocate, in GB. Valid only for KVM deployments. Note: Values smaller than the default are for lab and PoC only. Production deployments must use a value greater than or equal to the default. [default: 8]</t>
       </text>
     </comment>
-    <comment authorId="72" ref="A91" shapeId="0">
+    <comment authorId="72" ref="A92" shapeId="0">
       <text>
         <t>Amount of Webfilter RAM to allocate, in GB. Valid only for KVM deployments. Note: Values smaller than the default are for lab and PoC only. Production deployments must use a value greater than or equal to the default. [default: 8]</t>
       </text>
     </comment>
-    <comment authorId="73" ref="A92" shapeId="0">
+    <comment authorId="73" ref="A93" shapeId="0">
       <text>
         <t>Amount of Portal RAM to allocate, in GB. Valid only for KVM deployments. Note: Values smaller than the default are for lab and PoC only. Production deployments must use a value greater than or equal to the default. [default: 24]</t>
       </text>
     </comment>
-    <comment authorId="74" ref="A94" shapeId="0">
-      <text>
-        <t>Number of CPU's for VSD. Valid only for KVM and VCenter deployments [default: 6]</t>
-      </text>
-    </comment>
-    <comment authorId="75" ref="A95" shapeId="0">
-      <text>
-        <t>Number of CPU's for VSC. Valid only for KVM and VCenter deployments [default: 6]</t>
-      </text>
-    </comment>
-    <comment authorId="76" ref="A96" shapeId="0">
-      <text>
-        <t>Number of CPU's for VSTAT. Valid only for KVM and VCenter deployments [default: 6]</t>
-      </text>
-    </comment>
-    <comment authorId="77" ref="A97" shapeId="0">
-      <text>
-        <t>Number of CPU's for VNSUTIL. Valid only for KVM and VCenter deployments [default: 2]</t>
-      </text>
-    </comment>
-    <comment authorId="78" ref="A98" shapeId="0">
+    <comment authorId="74" ref="A95" shapeId="0">
+      <text>
+        <t>For KVM and VCenter deployments: number of CPU's for VSD. [default: 6]</t>
+      </text>
+    </comment>
+    <comment authorId="75" ref="A96" shapeId="0">
+      <text>
+        <t>For KVM and VCenter deployments: number of CPU's for VSC. [default: 6]</t>
+      </text>
+    </comment>
+    <comment authorId="76" ref="A97" shapeId="0">
+      <text>
+        <t>For KVM and VCenter deployments: number of CPU's for VSTAT. [default: 6]</t>
+      </text>
+    </comment>
+    <comment authorId="77" ref="A98" shapeId="0">
+      <text>
+        <t>For KVM and VCenter deployments: number of CPU's for VNSUTIL. [default: 2]</t>
+      </text>
+    </comment>
+    <comment authorId="78" ref="A100" shapeId="0">
       <text>
         <t>Number of CPU's for NUH. Valid only for KVM deployments [default: 2]</t>
       </text>
     </comment>
-    <comment authorId="79" ref="A99" shapeId="0">
+    <comment authorId="79" ref="A101" shapeId="0">
       <text>
         <t>Number of CPU's for VCIN. Valid only for KVM deployments [default: 6]</t>
       </text>
     </comment>
-    <comment authorId="80" ref="A100" shapeId="0">
+    <comment authorId="80" ref="A102" shapeId="0">
       <text>
         <t>Number of CPU's for Portal vm. Valid only for KVM deployments [default: 6]</t>
       </text>
     </comment>
-    <comment authorId="81" ref="A101" shapeId="0">
+    <comment authorId="81" ref="A103" shapeId="0">
       <text>
         <t>Number of CPU's for Webfilter vm. Valid only for KVM deployments [default: 2]</t>
       </text>
     </comment>
-    <comment authorId="82" ref="A103" shapeId="0">
+    <comment authorId="82" ref="A105" shapeId="0">
       <text>
         <t>VSD Architect URL. Required for tasks during Upgrade, Health Checks etc [default: https://(vsd_fqdn):8443]</t>
       </text>
     </comment>
-    <comment authorId="83" ref="A104" shapeId="0">
+    <comment authorId="83" ref="A106" shapeId="0">
       <text>
         <t>Enterprise name used for authentication with VSD Architect. Required for tasks during Upgrade, Health Checks etc [default: csp]</t>
       </text>
     </comment>
-    <comment authorId="84" ref="A105" shapeId="0">
+    <comment authorId="84" ref="A107" shapeId="0">
       <text>
         <t>VCIN URL used for API interaction. Required for tasks like VRS-E upgrade (through VCIN) [default: https://(vcin_ip_address):8443]</t>
       </text>
     </comment>
-    <comment authorId="85" ref="A106" shapeId="0">
+    <comment authorId="85" ref="A108" shapeId="0">
       <text>
         <t>Enterprise name used for authentication with VCIN. Required for tasks like VRS-E upgrade (through VCIN) [default: csp]</t>
       </text>
     </comment>
-    <comment authorId="86" ref="A108" shapeId="0">
+    <comment authorId="86" ref="A110" shapeId="0">
       <text>
         <t>List of hooks files (List items separated by comma.)</t>
       </text>
     </comment>
-    <comment authorId="87" ref="A109" shapeId="0">
+    <comment authorId="87" ref="A111" shapeId="0">
       <text>
         <t>Skip tasks and playbooks (List items separated by comma.)</t>
       </text>
     </comment>
-    <comment authorId="88" ref="A111" shapeId="0">
+    <comment authorId="88" ref="A113" shapeId="0">
       <text>
         <t>Address of SMTP server to be used if emailing health results</t>
       </text>
     </comment>
-    <comment authorId="89" ref="A112" shapeId="0">
+    <comment authorId="89" ref="A114" shapeId="0">
       <text>
         <t>Port to be used on the SMTP Server [default: 25]</t>
       </text>
     </comment>
-    <comment authorId="90" ref="A113" shapeId="0">
+    <comment authorId="90" ref="A115" shapeId="0">
       <text>
         <t>Email address from which health report will be sent</t>
       </text>
     </comment>
-    <comment authorId="91" ref="A114" shapeId="0">
+    <comment authorId="91" ref="A116" shapeId="0">
       <text>
         <t>List of destination email addresses (List items separated by comma.)</t>
       </text>
     </comment>
-    <comment authorId="92" ref="A116" shapeId="0">
+    <comment authorId="92" ref="A118" shapeId="0">
       <text>
         <t>Address of the mail server to be used to receive monit alerts via email</t>
       </text>
     </comment>
-    <comment authorId="93" ref="A117" shapeId="0">
+    <comment authorId="93" ref="A119" shapeId="0">
       <text>
         <t>Port on mail server to be used for monit alerts [default: 25]</t>
       </text>
     </comment>
-    <comment authorId="94" ref="A118" shapeId="0">
+    <comment authorId="94" ref="A120" shapeId="0">
       <text>
         <t>Encryption to be used when sending monit alerts via email</t>
       </text>
     </comment>
-    <comment authorId="95" ref="A119" shapeId="0">
+    <comment authorId="95" ref="A121" shapeId="0">
       <text>
         <t>Enables use of monit eventqueue to store alerts if email alerts fail to send [default: True]</t>
       </text>
     </comment>
-    <comment authorId="96" ref="A120" shapeId="0">
+    <comment authorId="96" ref="A122" shapeId="0">
       <text>
         <t>Email address from which monit alerts will be sent</t>
       </text>
     </comment>
-    <comment authorId="97" ref="A121" shapeId="0">
+    <comment authorId="97" ref="A123" shapeId="0">
       <text>
         <t>Email address to reply to monit alert emails</t>
       </text>
     </comment>
-    <comment authorId="98" ref="A122" shapeId="0">
+    <comment authorId="98" ref="A124" shapeId="0">
       <text>
         <t>Email subject for alert emails. Overrides monit default alert subject</t>
       </text>
     </comment>
-    <comment authorId="99" ref="A123" shapeId="0">
+    <comment authorId="99" ref="A125" shapeId="0">
       <text>
         <t>Email message for alert emails. Overrides monit default alert message</t>
       </text>
     </comment>
-    <comment authorId="100" ref="A124" shapeId="0">
+    <comment authorId="100" ref="A126" shapeId="0">
       <text>
         <t>Destination email address for monit alerts</t>
       </text>
     </comment>
-    <comment authorId="101" ref="A125" shapeId="0">
+    <comment authorId="101" ref="A127" shapeId="0">
       <text>
         <t>Specific events for which alerts should be sent. One string can be used to hold multiple events, separated by commas</t>
       </text>
     </comment>
-    <comment authorId="102" ref="A126" shapeId="0">
+    <comment authorId="102" ref="A128" shapeId="0">
       <text>
         <t>Events for which alerts should not be sent. One string can be used to hold multiple events, separated by commas</t>
       </text>
     </comment>
-    <comment authorId="103" ref="A127" shapeId="0">
+    <comment authorId="103" ref="A129" shapeId="0">
       <text>
         <t>Allowing VSD in-place upgrade during Installation [default: False]</t>
       </text>
@@ -6952,7 +6952,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B127"/>
+  <dimension ref="A1:B129"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7643,14 +7643,14 @@
     <row r="85">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>KVM RAM</t>
+          <t>KVM and VCenter RAM</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="8" t="inlineStr">
         <is>
-          <t>VSD RAM</t>
+          <t>KVM VSD RAM</t>
         </is>
       </c>
       <c r="B86" s="9" t="n"/>
@@ -7658,7 +7658,7 @@
     <row r="87">
       <c r="A87" s="8" t="inlineStr">
         <is>
-          <t>VSC RAM</t>
+          <t>KVM VSC RAM</t>
         </is>
       </c>
       <c r="B87" s="9" t="n"/>
@@ -7666,23 +7666,22 @@
     <row r="88">
       <c r="A88" s="8" t="inlineStr">
         <is>
-          <t>VSTAT RAM</t>
+          <t>KVM VSTAT RAM</t>
         </is>
       </c>
       <c r="B88" s="9" t="n"/>
     </row>
     <row r="89">
-      <c r="A89" s="8" t="inlineStr">
-        <is>
-          <t>KVM VCIN RAM</t>
-        </is>
-      </c>
-      <c r="B89" s="9" t="n"/>
+      <c r="A89" s="3" t="inlineStr">
+        <is>
+          <t>KVM RAM</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" s="8" t="inlineStr">
         <is>
-          <t>KVM NUH RAM</t>
+          <t>KVM VCIN RAM</t>
         </is>
       </c>
       <c r="B90" s="9" t="n"/>
@@ -7690,7 +7689,7 @@
     <row r="91">
       <c r="A91" s="8" t="inlineStr">
         <is>
-          <t>KVM Webfilter RAM</t>
+          <t>KVM NUH RAM</t>
         </is>
       </c>
       <c r="B91" s="9" t="n"/>
@@ -7698,30 +7697,30 @@
     <row r="92">
       <c r="A92" s="8" t="inlineStr">
         <is>
+          <t>KVM Webfilter RAM</t>
+        </is>
+      </c>
+      <c r="B92" s="9" t="n"/>
+    </row>
+    <row r="93">
+      <c r="A93" s="8" t="inlineStr">
+        <is>
           <t>KVM Portal RAM</t>
         </is>
       </c>
-      <c r="B92" s="9" t="n"/>
-    </row>
-    <row r="93">
-      <c r="A93" s="3" t="inlineStr">
-        <is>
-          <t>CPU</t>
-        </is>
-      </c>
+      <c r="B93" s="9" t="n"/>
     </row>
     <row r="94">
-      <c r="A94" s="8" t="inlineStr">
-        <is>
-          <t>VSD CPU cores</t>
-        </is>
-      </c>
-      <c r="B94" s="9" t="n"/>
+      <c r="A94" s="3" t="inlineStr">
+        <is>
+          <t>KVM and VCenter CPU</t>
+        </is>
+      </c>
     </row>
     <row r="95">
       <c r="A95" s="8" t="inlineStr">
         <is>
-          <t>VSC CPU cores</t>
+          <t>KVM VSD CPU cores</t>
         </is>
       </c>
       <c r="B95" s="9" t="n"/>
@@ -7729,7 +7728,7 @@
     <row r="96">
       <c r="A96" s="8" t="inlineStr">
         <is>
-          <t>VSTAT CPU cores</t>
+          <t>KVM VSC CPU cores</t>
         </is>
       </c>
       <c r="B96" s="9" t="n"/>
@@ -7737,7 +7736,7 @@
     <row r="97">
       <c r="A97" s="8" t="inlineStr">
         <is>
-          <t>VNSUTIL CPU cores</t>
+          <t>KVM VSTAT CPU cores</t>
         </is>
       </c>
       <c r="B97" s="9" t="n"/>
@@ -7745,23 +7744,22 @@
     <row r="98">
       <c r="A98" s="8" t="inlineStr">
         <is>
-          <t>KVM NUH CPU cores</t>
+          <t>KVM VNSUTIL CPU cores</t>
         </is>
       </c>
       <c r="B98" s="9" t="n"/>
     </row>
     <row r="99">
-      <c r="A99" s="8" t="inlineStr">
-        <is>
-          <t>KVM VCIN CPU cores</t>
-        </is>
-      </c>
-      <c r="B99" s="9" t="n"/>
+      <c r="A99" s="3" t="inlineStr">
+        <is>
+          <t>KVM CPU</t>
+        </is>
+      </c>
     </row>
     <row r="100">
       <c r="A100" s="8" t="inlineStr">
         <is>
-          <t>KVM Portal VM CPU cores</t>
+          <t>KVM NUH CPU cores</t>
         </is>
       </c>
       <c r="B100" s="9" t="n"/>
@@ -7769,38 +7767,38 @@
     <row r="101">
       <c r="A101" s="8" t="inlineStr">
         <is>
-          <t>KVM Webfilter VM CPU cores</t>
+          <t>KVM VCIN CPU cores</t>
         </is>
       </c>
       <c r="B101" s="9" t="n"/>
     </row>
     <row r="102">
-      <c r="A102" s="3" t="inlineStr">
-        <is>
-          <t>Authentication</t>
-        </is>
-      </c>
+      <c r="A102" s="8" t="inlineStr">
+        <is>
+          <t>KVM Portal VM CPU cores</t>
+        </is>
+      </c>
+      <c r="B102" s="9" t="n"/>
     </row>
     <row r="103">
       <c r="A103" s="8" t="inlineStr">
         <is>
-          <t>VSD Architect URL</t>
+          <t>KVM Webfilter VM CPU cores</t>
         </is>
       </c>
       <c r="B103" s="9" t="n"/>
     </row>
     <row r="104">
-      <c r="A104" s="8" t="inlineStr">
-        <is>
-          <t>VSD Enterprise</t>
-        </is>
-      </c>
-      <c r="B104" s="9" t="n"/>
+      <c r="A104" s="3" t="inlineStr">
+        <is>
+          <t>Authentication</t>
+        </is>
+      </c>
     </row>
     <row r="105">
       <c r="A105" s="8" t="inlineStr">
         <is>
-          <t>VCIN URL</t>
+          <t>VSD Architect URL</t>
         </is>
       </c>
       <c r="B105" s="9" t="n"/>
@@ -7808,61 +7806,61 @@
     <row r="106">
       <c r="A106" s="8" t="inlineStr">
         <is>
-          <t>VCIN Enterprise</t>
+          <t>VSD Enterprise</t>
         </is>
       </c>
       <c r="B106" s="9" t="n"/>
     </row>
     <row r="107">
-      <c r="A107" s="3" t="inlineStr">
-        <is>
-          <t>Hooks</t>
-        </is>
-      </c>
+      <c r="A107" s="8" t="inlineStr">
+        <is>
+          <t>VCIN URL</t>
+        </is>
+      </c>
+      <c r="B107" s="9" t="n"/>
     </row>
     <row r="108">
       <c r="A108" s="8" t="inlineStr">
         <is>
+          <t>VCIN Enterprise</t>
+        </is>
+      </c>
+      <c r="B108" s="9" t="n"/>
+    </row>
+    <row r="109">
+      <c r="A109" s="3" t="inlineStr">
+        <is>
+          <t>Hooks</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="8" t="inlineStr">
+        <is>
           <t>hooks</t>
         </is>
       </c>
-      <c r="B108" s="9" t="n"/>
-    </row>
-    <row r="109">
-      <c r="A109" s="8" t="inlineStr">
-        <is>
-          <t>skip actions</t>
-        </is>
-      </c>
-      <c r="B109" s="9" t="n"/>
-    </row>
-    <row r="110">
-      <c r="A110" s="3" t="inlineStr">
-        <is>
-          <t>Component Health Report Email Options</t>
-        </is>
-      </c>
+      <c r="B110" s="9" t="n"/>
     </row>
     <row r="111">
       <c r="A111" s="8" t="inlineStr">
         <is>
-          <t>Health Report SMTP Server</t>
+          <t>skip actions</t>
         </is>
       </c>
       <c r="B111" s="9" t="n"/>
     </row>
     <row r="112">
-      <c r="A112" s="8" t="inlineStr">
-        <is>
-          <t>Health Report SMTP Server Port</t>
-        </is>
-      </c>
-      <c r="B112" s="9" t="n"/>
+      <c r="A112" s="3" t="inlineStr">
+        <is>
+          <t>Component Health Report Email Options</t>
+        </is>
+      </c>
     </row>
     <row r="113">
       <c r="A113" s="8" t="inlineStr">
         <is>
-          <t>Health Report Email From Address</t>
+          <t>Health Report SMTP Server</t>
         </is>
       </c>
       <c r="B113" s="9" t="n"/>
@@ -7870,38 +7868,38 @@
     <row r="114">
       <c r="A114" s="8" t="inlineStr">
         <is>
-          <t>Health Report Destination Email Address(es)</t>
+          <t>Health Report SMTP Server Port</t>
         </is>
       </c>
       <c r="B114" s="9" t="n"/>
     </row>
     <row r="115">
-      <c r="A115" s="3" t="inlineStr">
-        <is>
-          <t>VSD Monit Email Alerts Configuration</t>
-        </is>
-      </c>
+      <c r="A115" s="8" t="inlineStr">
+        <is>
+          <t>Health Report Email From Address</t>
+        </is>
+      </c>
+      <c r="B115" s="9" t="n"/>
     </row>
     <row r="116">
       <c r="A116" s="8" t="inlineStr">
         <is>
-          <t>VSD Monit Mail Server</t>
+          <t>Health Report Destination Email Address(es)</t>
         </is>
       </c>
       <c r="B116" s="9" t="n"/>
     </row>
     <row r="117">
-      <c r="A117" s="8" t="inlineStr">
-        <is>
-          <t>VSD Monit Mail Server Port</t>
-        </is>
-      </c>
-      <c r="B117" s="9" t="n"/>
+      <c r="A117" s="3" t="inlineStr">
+        <is>
+          <t>VSD Monit Email Alerts Configuration</t>
+        </is>
+      </c>
     </row>
     <row r="118">
       <c r="A118" s="8" t="inlineStr">
         <is>
-          <t>VSD Monit Mail Server Encryption Type</t>
+          <t>VSD Monit Mail Server</t>
         </is>
       </c>
       <c r="B118" s="9" t="n"/>
@@ -7909,7 +7907,7 @@
     <row r="119">
       <c r="A119" s="8" t="inlineStr">
         <is>
-          <t>Use VSD Monit Eventqueue</t>
+          <t>VSD Monit Mail Server Port</t>
         </is>
       </c>
       <c r="B119" s="9" t="n"/>
@@ -7917,7 +7915,7 @@
     <row r="120">
       <c r="A120" s="8" t="inlineStr">
         <is>
-          <t>VSD Monit From Email Address</t>
+          <t>VSD Monit Mail Server Encryption Type</t>
         </is>
       </c>
       <c r="B120" s="9" t="n"/>
@@ -7925,7 +7923,7 @@
     <row r="121">
       <c r="A121" s="8" t="inlineStr">
         <is>
-          <t>VSD Monit Reply-To Email Address</t>
+          <t>Use VSD Monit Eventqueue</t>
         </is>
       </c>
       <c r="B121" s="9" t="n"/>
@@ -7933,7 +7931,7 @@
     <row r="122">
       <c r="A122" s="8" t="inlineStr">
         <is>
-          <t>VSD Monit Email Alert Subject</t>
+          <t>VSD Monit From Email Address</t>
         </is>
       </c>
       <c r="B122" s="9" t="n"/>
@@ -7941,7 +7939,7 @@
     <row r="123">
       <c r="A123" s="8" t="inlineStr">
         <is>
-          <t>VSD Monit Email Alert Message</t>
+          <t>VSD Monit Reply-To Email Address</t>
         </is>
       </c>
       <c r="B123" s="9" t="n"/>
@@ -7949,7 +7947,7 @@
     <row r="124">
       <c r="A124" s="8" t="inlineStr">
         <is>
-          <t>VSD Monit Destination Email Address</t>
+          <t>VSD Monit Email Alert Subject</t>
         </is>
       </c>
       <c r="B124" s="9" t="n"/>
@@ -7957,7 +7955,7 @@
     <row r="125">
       <c r="A125" s="8" t="inlineStr">
         <is>
-          <t>VSD Monit Only Alert On</t>
+          <t>VSD Monit Email Alert Message</t>
         </is>
       </c>
       <c r="B125" s="9" t="n"/>
@@ -7965,7 +7963,7 @@
     <row r="126">
       <c r="A126" s="8" t="inlineStr">
         <is>
-          <t>VSD Monit Do Not Alert On</t>
+          <t>VSD Monit Destination Email Address</t>
         </is>
       </c>
       <c r="B126" s="9" t="n"/>
@@ -7973,13 +7971,29 @@
     <row r="127">
       <c r="A127" s="8" t="inlineStr">
         <is>
+          <t>VSD Monit Only Alert On</t>
+        </is>
+      </c>
+      <c r="B127" s="9" t="n"/>
+    </row>
+    <row r="128">
+      <c r="A128" s="8" t="inlineStr">
+        <is>
+          <t>VSD Monit Do Not Alert On</t>
+        </is>
+      </c>
+      <c r="B128" s="9" t="n"/>
+    </row>
+    <row r="129">
+      <c r="A129" s="8" t="inlineStr">
+        <is>
           <t xml:space="preserve">VSD In-place upgrade during Install </t>
         </is>
       </c>
-      <c r="B127" s="9" t="n"/>
+      <c r="B129" s="9" t="n"/>
     </row>
   </sheetData>
-  <mergeCells count="20">
+  <mergeCells count="22">
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A16:B16"/>
@@ -7995,11 +8009,13 @@
     <mergeCell ref="A72:B72"/>
     <mergeCell ref="A78:B78"/>
     <mergeCell ref="A85:B85"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="A102:B102"/>
-    <mergeCell ref="A107:B107"/>
-    <mergeCell ref="A110:B110"/>
-    <mergeCell ref="A115:B115"/>
+    <mergeCell ref="A89:B89"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="A99:B99"/>
+    <mergeCell ref="A104:B104"/>
+    <mergeCell ref="A109:B109"/>
+    <mergeCell ref="A112:B112"/>
+    <mergeCell ref="A117:B117"/>
   </mergeCells>
   <dataValidations count="42">
     <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="B24" type="list">
@@ -8054,24 +8070,24 @@
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B86" type="whole"/>
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B87" type="whole"/>
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B88" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B89" type="whole"/>
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B90" type="whole"/>
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B91" type="whole"/>
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B92" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B94" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B93" type="whole"/>
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B95" type="whole"/>
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B96" type="whole"/>
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B97" type="whole"/>
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B98" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B99" type="whole"/>
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B100" type="whole"/>
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B101" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B112" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B117" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="B119" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B102" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B103" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B114" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B119" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="B121" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="B127" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="B129" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Description update, remove target server type
</commit_message>
<xml_diff>
--- a/examples/excel/active_standby_vsds.xlsx
+++ b/examples/excel/active_standby_vsds.xlsx
@@ -1555,17 +1555,17 @@
     </comment>
     <comment authorId="67" ref="A86" shapeId="0">
       <text>
-        <t>For KVM and VCenter deployments: amount of VSD RAM to allocate, in GB. Note: Values smaller than the default are for lab and PoC only. Production deployments must use a value greater than or equal to the default. [default: 24]</t>
+        <t>Valid for only KVM and VCenter deployments. Amount of VSD RAM to allocate, in GB. Note: Values smaller than the default are for lab and PoC only. Production deployments must use a value greater than or equal to the default. [default: 24]</t>
       </text>
     </comment>
     <comment authorId="68" ref="A87" shapeId="0">
       <text>
-        <t>For KVM and VCenter deployments: amount of VSC RAM to allocate, in GB. Note: Values smaller than the default are for lab and PoC only. Production deployments must use a value greater than or equal to the default. [default: 4]</t>
+        <t>Valid for only KVM and VCenter deployments: amount of VSC RAM to allocate, in GB. Note: Values smaller than the default are for lab and PoC only. Production deployments must use a value greater than or equal to the default. [default: 4]</t>
       </text>
     </comment>
     <comment authorId="69" ref="A88" shapeId="0">
       <text>
-        <t>For KVM and VCenter deployments: amount of VSTAT RAM to allocate, in GB. Note: Values smaller than the default are for lab and PoC only. Production deployments must use a value greater than or equal to the default. [default: 16]</t>
+        <t>Valid for only KVM and VCenter deployments: amount of VSTAT RAM to allocate, in GB. Note: Values smaller than the default are for lab and PoC only. Production deployments must use a value greater than or equal to the default. [default: 16]</t>
       </text>
     </comment>
     <comment authorId="70" ref="A90" shapeId="0">
@@ -1590,22 +1590,22 @@
     </comment>
     <comment authorId="74" ref="A95" shapeId="0">
       <text>
-        <t>For KVM and VCenter deployments: number of CPU's for VSD. [default: 6]</t>
+        <t>Valid for only KVM and VCenter deployments: number of CPU's for VSD. [default: 6]</t>
       </text>
     </comment>
     <comment authorId="75" ref="A96" shapeId="0">
       <text>
-        <t>For KVM and VCenter deployments: number of CPU's for VSC. [default: 6]</t>
+        <t>Valid for only KVM and VCenter deployments: number of CPU's for VSC. [default: 6]</t>
       </text>
     </comment>
     <comment authorId="76" ref="A97" shapeId="0">
       <text>
-        <t>For KVM and VCenter deployments: number of CPU's for VSTAT. [default: 6]</t>
+        <t>Valid for only KVM and VCenter deployments: number of CPU's for VSTAT. [default: 6]</t>
       </text>
     </comment>
     <comment authorId="77" ref="A98" shapeId="0">
       <text>
-        <t>For KVM and VCenter deployments: number of CPU's for VNSUTIL. [default: 2]</t>
+        <t>Valid for only KVM and VCenter deployments: number of CPU's for VNSUTIL. [default: 2]</t>
       </text>
     </comment>
     <comment authorId="78" ref="A100" shapeId="0">

</xml_diff>

<commit_message>
Allow extra disk device and mount point to be specified
</commit_message>
<xml_diff>
--- a/examples/excel/active_standby_vsds.xlsx
+++ b/examples/excel/active_standby_vsds.xlsx
@@ -3121,6 +3121,8 @@
     <author>repo_name</author>
     <author>add_extra_disk</author>
     <author>extra_disk_size_gb</author>
+    <author>extra_disk_device</author>
+    <author>extra_disk_mount_point</author>
     <author>extra_disk_image_path</author>
     <author>extra_disk_image_file_name</author>
     <author>cpuset</author>
@@ -3306,30 +3308,40 @@
     </comment>
     <comment authorId="35" ref="A46" shapeId="0">
       <text>
+        <t>Device for extra disk [default: vdb]</t>
+      </text>
+    </comment>
+    <comment authorId="36" ref="A47" shapeId="0">
+      <text>
+        <t>Mount point for extra disk [default: /var/lib/elasticsearch/]</t>
+      </text>
+    </comment>
+    <comment authorId="37" ref="A48" shapeId="0">
+      <text>
         <t>Path on the hypervisor to store the extra disk image. Supported on KVM only. [default: /var/lib/libvirt/images]</t>
       </text>
     </comment>
-    <comment authorId="36" ref="A47" shapeId="0">
+    <comment authorId="38" ref="A49" shapeId="0">
       <text>
         <t>Name of the extra disk image file. Supported on KVM only. [default: extra-disk-(hostname)]</t>
       </text>
     </comment>
-    <comment authorId="37" ref="A49" shapeId="0">
+    <comment authorId="39" ref="A51" shapeId="0">
       <text>
         <t>Cpuset information for cpu pinning on KVM. For example, VSTAT requires 6 cores and sample values will be of the form [ 0, 1, 2, 3, 4, 5 ] (List items separated by comma.)</t>
       </text>
     </comment>
-    <comment authorId="38" ref="A50" shapeId="0">
+    <comment authorId="40" ref="A52" shapeId="0">
       <text>
         <t>Enable the setup of the Virtualized Security Services UI [default: False]</t>
       </text>
     </comment>
-    <comment authorId="39" ref="A51" shapeId="0">
+    <comment authorId="41" ref="A53" shapeId="0">
       <text>
         <t>Enables setup of a health monitoring agent [default: none]</t>
       </text>
     </comment>
-    <comment authorId="40" ref="A52" shapeId="0">
+    <comment authorId="42" ref="A54" shapeId="0">
       <text>
         <t>Name of the credentials set for the vsd</t>
       </text>
@@ -11803,7 +11815,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G52"/>
+  <dimension ref="A1:G54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12341,7 +12353,7 @@
     <row r="46">
       <c r="A46" s="6" t="inlineStr">
         <is>
-          <t>Extra disk image path on hypervisor</t>
+          <t>Extra Disk Device</t>
         </is>
       </c>
       <c r="B46" s="7" t="n"/>
@@ -12354,7 +12366,7 @@
     <row r="47">
       <c r="A47" s="6" t="inlineStr">
         <is>
-          <t>Extra disk image file prefix</t>
+          <t>Extra Disk Mount Point</t>
         </is>
       </c>
       <c r="B47" s="7" t="n"/>
@@ -12365,42 +12377,42 @@
       <c r="G47" s="7" t="n"/>
     </row>
     <row r="48">
-      <c r="A48" s="3" t="inlineStr">
+      <c r="A48" s="6" t="inlineStr">
+        <is>
+          <t>Extra disk image path on hypervisor</t>
+        </is>
+      </c>
+      <c r="B48" s="7" t="n"/>
+      <c r="C48" s="7" t="n"/>
+      <c r="D48" s="7" t="n"/>
+      <c r="E48" s="7" t="n"/>
+      <c r="F48" s="7" t="n"/>
+      <c r="G48" s="7" t="n"/>
+    </row>
+    <row r="49">
+      <c r="A49" s="6" t="inlineStr">
+        <is>
+          <t>Extra disk image file prefix</t>
+        </is>
+      </c>
+      <c r="B49" s="7" t="n"/>
+      <c r="C49" s="7" t="n"/>
+      <c r="D49" s="7" t="n"/>
+      <c r="E49" s="7" t="n"/>
+      <c r="F49" s="7" t="n"/>
+      <c r="G49" s="7" t="n"/>
+    </row>
+    <row r="50">
+      <c r="A50" s="3" t="inlineStr">
         <is>
           <t>Other configuration</t>
         </is>
       </c>
-    </row>
-    <row r="49">
-      <c r="A49" s="8" t="inlineStr">
-        <is>
-          <t>KVM cpuset information</t>
-        </is>
-      </c>
-      <c r="B49" s="9" t="n"/>
-      <c r="C49" s="9" t="n"/>
-      <c r="D49" s="9" t="n"/>
-      <c r="E49" s="9" t="n"/>
-      <c r="F49" s="9" t="n"/>
-      <c r="G49" s="9" t="n"/>
-    </row>
-    <row r="50">
-      <c r="A50" s="8" t="inlineStr">
-        <is>
-          <t>Enable VSS UI</t>
-        </is>
-      </c>
-      <c r="B50" s="9" t="n"/>
-      <c r="C50" s="9" t="n"/>
-      <c r="D50" s="9" t="n"/>
-      <c r="E50" s="9" t="n"/>
-      <c r="F50" s="9" t="n"/>
-      <c r="G50" s="9" t="n"/>
     </row>
     <row r="51">
       <c r="A51" s="8" t="inlineStr">
         <is>
-          <t>Health monitoring agent</t>
+          <t>KVM cpuset information</t>
         </is>
       </c>
       <c r="B51" s="9" t="n"/>
@@ -12413,7 +12425,7 @@
     <row r="52">
       <c r="A52" s="8" t="inlineStr">
         <is>
-          <t>Credentials set name</t>
+          <t>Enable VSS UI</t>
         </is>
       </c>
       <c r="B52" s="9" t="n"/>
@@ -12422,6 +12434,32 @@
       <c r="E52" s="9" t="n"/>
       <c r="F52" s="9" t="n"/>
       <c r="G52" s="9" t="n"/>
+    </row>
+    <row r="53">
+      <c r="A53" s="8" t="inlineStr">
+        <is>
+          <t>Health monitoring agent</t>
+        </is>
+      </c>
+      <c r="B53" s="9" t="n"/>
+      <c r="C53" s="9" t="n"/>
+      <c r="D53" s="9" t="n"/>
+      <c r="E53" s="9" t="n"/>
+      <c r="F53" s="9" t="n"/>
+      <c r="G53" s="9" t="n"/>
+    </row>
+    <row r="54">
+      <c r="A54" s="8" t="inlineStr">
+        <is>
+          <t>Credentials set name</t>
+        </is>
+      </c>
+      <c r="B54" s="9" t="n"/>
+      <c r="C54" s="9" t="n"/>
+      <c r="D54" s="9" t="n"/>
+      <c r="E54" s="9" t="n"/>
+      <c r="F54" s="9" t="n"/>
+      <c r="G54" s="9" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -12432,7 +12470,7 @@
     <mergeCell ref="A30:G30"/>
     <mergeCell ref="A38:G38"/>
     <mergeCell ref="A43:G43"/>
-    <mergeCell ref="A48:G48"/>
+    <mergeCell ref="A50:G50"/>
   </mergeCells>
   <dataValidations count="54">
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B7" type="whole"/>
@@ -12513,40 +12551,40 @@
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="E45" type="whole"/>
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="F45" type="whole"/>
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="G45" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="B50" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="B52" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="C50" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="C52" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="D50" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="D52" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="E50" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="E52" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="F50" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="F52" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="G50" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="G52" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="B51" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="B53" type="list">
       <formula1>"none,zabbix"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="C51" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="C53" type="list">
       <formula1>"none,zabbix"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="D51" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="D53" type="list">
       <formula1>"none,zabbix"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="E51" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="E53" type="list">
       <formula1>"none,zabbix"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="F51" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="F53" type="list">
       <formula1>"none,zabbix"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="G51" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="G53" type="list">
       <formula1>"none,zabbix"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
generate files and update docs
</commit_message>
<xml_diff>
--- a/examples/excel/active_standby_vsds.xlsx
+++ b/examples/excel/active_standby_vsds.xlsx
@@ -1,37 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Deployment" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Common" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Upgrade" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Vsds" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Vscs" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Vstats" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Credentials" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Dnss" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Netconf managers" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Nsgv access ports" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Nsgv bootstrap" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Nsgvs" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Nuh common" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Nuh external interfaces" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Nuh vrrp" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Nuhs" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Portals" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Proxys" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Stcv global" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Stcvs" sheetId="20" state="visible" r:id="rId20"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Vcins" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Vnsutils" sheetId="22" state="visible" r:id="rId22"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Vrss" sheetId="23" state="visible" r:id="rId23"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Vsrs" sheetId="24" state="visible" r:id="rId24"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Webfilters" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet name="Deployment" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Common" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Upgrade" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Vsds" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Vscs" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Vstats" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Credentials" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Dnss" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Netconf managers" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="Nsgv access ports" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="Nsgv bootstrap" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="Nsgvs" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="Nuh common" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="Nuh external interfaces" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="Nuh vrrp" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="Nuhs" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="Portals" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="Proxys" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="Stcv global" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet name="Stcvs" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet name="Vcins" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet name="Vnsutils" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet name="Vrss" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet name="Vsrs" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet name="Webfilters" sheetId="25" state="visible" r:id="rId25"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -4135,7 +4135,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -4194,12 +4194,12 @@
     <mergeCell ref="A4:B4"/>
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
+  <legacyDrawing r:id="anysvml"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -4320,12 +4320,12 @@
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="G8" type="whole"/>
   </dataValidations>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
+  <legacyDrawing r:id="anysvml"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -4502,12 +4502,12 @@
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B20" type="whole"/>
   </dataValidations>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
+  <legacyDrawing r:id="anysvml"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -5439,12 +5439,12 @@
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="G65" type="whole"/>
   </dataValidations>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
+  <legacyDrawing r:id="anysvml"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -5511,12 +5511,12 @@
     </dataValidation>
   </dataValidations>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
+  <legacyDrawing r:id="anysvml"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -5682,12 +5682,12 @@
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="G9" type="whole"/>
   </dataValidations>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
+  <legacyDrawing r:id="anysvml"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -5813,12 +5813,12 @@
     </dataValidation>
   </dataValidations>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
+  <legacyDrawing r:id="anysvml"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -6247,12 +6247,12 @@
     </dataValidation>
   </dataValidations>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
+  <legacyDrawing r:id="anysvml"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -6621,12 +6621,12 @@
     </dataValidation>
   </dataValidations>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
+  <legacyDrawing r:id="anysvml"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -6912,12 +6912,12 @@
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="G17" type="whole"/>
   </dataValidations>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
+  <legacyDrawing r:id="anysvml"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -6984,12 +6984,12 @@
     <mergeCell ref="A4:B4"/>
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
+  <legacyDrawing r:id="anysvml"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -8134,12 +8134,12 @@
     </dataValidation>
   </dataValidations>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
+  <legacyDrawing r:id="anysvml"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -8418,12 +8418,12 @@
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="G20" type="whole"/>
   </dataValidations>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
+  <legacyDrawing r:id="anysvml"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -8716,12 +8716,12 @@
     </dataValidation>
   </dataValidations>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
+  <legacyDrawing r:id="anysvml"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -9410,12 +9410,12 @@
     </dataValidation>
   </dataValidations>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
+  <legacyDrawing r:id="anysvml"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -9634,12 +9634,12 @@
     </dataValidation>
   </dataValidations>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
+  <legacyDrawing r:id="anysvml"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -9958,12 +9958,12 @@
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="G12" type="whole"/>
   </dataValidations>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
+  <legacyDrawing r:id="anysvml"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -10214,12 +10214,12 @@
     </dataValidation>
   </dataValidations>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
+  <legacyDrawing r:id="anysvml"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -10332,12 +10332,12 @@
     </dataValidation>
   </dataValidations>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
+  <legacyDrawing r:id="anysvml"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -11208,12 +11208,12 @@
     </dataValidation>
   </dataValidations>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
+  <legacyDrawing r:id="anysvml"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -11926,12 +11926,12 @@
     </dataValidation>
   </dataValidations>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
+  <legacyDrawing r:id="anysvml"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -12710,12 +12710,12 @@
     </dataValidation>
   </dataValidations>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
+  <legacyDrawing r:id="anysvml"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -13538,12 +13538,12 @@
     <mergeCell ref="A65:G65"/>
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
+  <legacyDrawing r:id="anysvml"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -13896,12 +13896,12 @@
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="G12" type="whole"/>
   </dataValidations>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
+  <legacyDrawing r:id="anysvml"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -14001,6 +14001,6 @@
     <mergeCell ref="A4:G4"/>
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
+  <legacyDrawing r:id="anysvml"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add variable for custom script path
</commit_message>
<xml_diff>
--- a/examples/excel/active_standby_vsds.xlsx
+++ b/examples/excel/active_standby_vsds.xlsx
@@ -2442,6 +2442,7 @@
     <author>skip_disable_stats_collection</author>
     <author>force_vsc_standalone_upgrade</author>
     <author>upgrade_portal</author>
+    <author>vsd_preupgrade_db_script_path</author>
   </authors>
   <commentList>
     <comment authorId="0" ref="A5" shapeId="0">
@@ -2477,6 +2478,11 @@
     <comment authorId="6" ref="A11" shapeId="0">
       <text>
         <t>Upgrade the SD-WAN Portal or Cluster [default: False]</t>
+      </text>
+    </comment>
+    <comment authorId="7" ref="A12" shapeId="0">
+      <text>
+        <t>Path to the VSD pre-upgrade database check script. [default: /media/CDROM]</t>
       </text>
     </comment>
   </commentList>
@@ -10224,7 +10230,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10312,6 +10318,14 @@
         </is>
       </c>
       <c r="B11" s="7" t="n"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="6" t="inlineStr">
+        <is>
+          <t>VSD Pre-upgrade Database Check Script Path</t>
+        </is>
+      </c>
+      <c r="B12" s="7" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Add VSTAT License file
</commit_message>
<xml_diff>
--- a/examples/excel/active_standby_vsds.xlsx
+++ b/examples/excel/active_standby_vsds.xlsx
@@ -1166,6 +1166,7 @@
     <author>vsd_license_required_days_left</author>
     <author>vsd_continue_on_license_failure</author>
     <author>vsd_ejabberd_license_file</author>
+    <author>vstat_license_file</author>
     <author>portal_license_file</author>
     <author>nuh_license_file</author>
     <author>yum_update</author>
@@ -1490,250 +1491,255 @@
     </comment>
     <comment authorId="54" ref="A70" shapeId="0">
       <text>
+        <t>Optional License File for Elasticsearch [default: ]</t>
+      </text>
+    </comment>
+    <comment authorId="55" ref="A71" shapeId="0">
+      <text>
         <t>Path to the license file for the SD-WAN Portal including the file name [default: ]</t>
       </text>
     </comment>
-    <comment authorId="55" ref="A71" shapeId="0">
+    <comment authorId="56" ref="A72" shapeId="0">
       <text>
         <t>Path to the license file for the NUH including the file name [default: ]</t>
       </text>
     </comment>
-    <comment authorId="56" ref="A73" shapeId="0">
+    <comment authorId="57" ref="A74" shapeId="0">
       <text>
         <t>Flag to indicate whether to perform a Yum update on VSD during the installation [default: True]</t>
       </text>
     </comment>
-    <comment authorId="57" ref="A74" shapeId="0">
+    <comment authorId="58" ref="A75" shapeId="0">
       <text>
         <t>Flag to indicate whether to perform a Yum update on VSTAT during the installation [default: False]</t>
       </text>
     </comment>
-    <comment authorId="58" ref="A75" shapeId="0">
+    <comment authorId="59" ref="A76" shapeId="0">
       <text>
         <t>Proxy URL to be used if Yum repositories cannot be directly reached [default: NONE]</t>
       </text>
     </comment>
-    <comment authorId="59" ref="A76" shapeId="0">
+    <comment authorId="60" ref="A77" shapeId="0">
       <text>
         <t>Username of the SSH proxy host if one is used [default: root]</t>
       </text>
     </comment>
-    <comment authorId="60" ref="A77" shapeId="0">
+    <comment authorId="61" ref="A78" shapeId="0">
       <text>
         <t>IP Address or Hostname of the SSH host if one is used [default: sshhost]</t>
       </text>
     </comment>
-    <comment authorId="61" ref="A79" shapeId="0">
+    <comment authorId="62" ref="A80" shapeId="0">
       <text>
         <t>Amount of VSD disk space to pre-allocate, in GB. Note: Values smaller than the default are for lab and PoC only. Production deployments must use a value greater than or equal to the default. [default: 285]</t>
       </text>
     </comment>
-    <comment authorId="62" ref="A80" shapeId="0">
+    <comment authorId="63" ref="A81" shapeId="0">
       <text>
         <t>Amount of VSC disk space to pre-allocate, in GB. The only valid values are 0 and 1. When undefined or 0, file size allocation will be skipped. Production deployments should set this value to 1. [default: 0]</t>
       </text>
     </comment>
-    <comment authorId="63" ref="A81" shapeId="0">
+    <comment authorId="64" ref="A82" shapeId="0">
       <text>
         <t>Amount of VSTAT disk space to pre-allocate, in GB. Note: Values smaller than the default are for lab and PoC only. Production deployments should not modify this value. [default: 100]</t>
       </text>
     </comment>
-    <comment authorId="64" ref="A82" shapeId="0">
+    <comment authorId="65" ref="A83" shapeId="0">
       <text>
         <t>Amount of Portal disk space to pre-allocate, in GB. Note: Values smaller than the default are for lab and PoC only. Production deployments should not modify this value. [default: 16]</t>
       </text>
     </comment>
-    <comment authorId="65" ref="A83" shapeId="0">
+    <comment authorId="66" ref="A84" shapeId="0">
       <text>
         <t>Amount of VCIN disk space to pre-allocate, in GB. Note: Values smaller than the default are for lab and PoC only. Production deployments should not modify this value. [default: 285]</t>
       </text>
     </comment>
-    <comment authorId="66" ref="A84" shapeId="0">
+    <comment authorId="67" ref="A85" shapeId="0">
       <text>
         <t>Amount of NSGV disk space to pre-allocate, in GB. Note: Values smaller than the default are for lab and PoC only. Production deployments should not modify this value. [default: 4]</t>
       </text>
     </comment>
-    <comment authorId="67" ref="A86" shapeId="0">
+    <comment authorId="68" ref="A87" shapeId="0">
       <text>
         <t>Valid for only KVM and VCenter deployments. Amount of VSD RAM to allocate, in GB. Note: Values smaller than the default are for lab and PoC only. Production deployments must use a value greater than or equal to the default. [default: 24]</t>
       </text>
     </comment>
-    <comment authorId="68" ref="A87" shapeId="0">
+    <comment authorId="69" ref="A88" shapeId="0">
       <text>
         <t>Valid for only KVM and VCenter deployments. Amount of VSC RAM to allocate, in GB. Note: Values smaller than the default are for lab and PoC only. Production deployments must use a value greater than or equal to the default. [default: 4]</t>
       </text>
     </comment>
-    <comment authorId="69" ref="A88" shapeId="0">
+    <comment authorId="70" ref="A89" shapeId="0">
       <text>
         <t>Valid for only KVM and VCenter deployments. Amount of VSTAT RAM to allocate, in GB. Note: Values smaller than the default are for lab and PoC only. Production deployments must use a value greater than or equal to the default. [default: 16]</t>
       </text>
     </comment>
-    <comment authorId="70" ref="A90" shapeId="0">
+    <comment authorId="71" ref="A91" shapeId="0">
       <text>
         <t>Amount of VCIN RAM to allocate, in GB. Valid only for KVM deployments. Note: Values smaller than the default are for lab and PoC only. Production deployments must use a value greater than or equal to the default. [default: 24]</t>
       </text>
     </comment>
-    <comment authorId="71" ref="A91" shapeId="0">
+    <comment authorId="72" ref="A92" shapeId="0">
       <text>
         <t>Amount of NUH RAM to allocate, in GB. Valid only for KVM deployments. Note: Values smaller than the default are for lab and PoC only. Production deployments must use a value greater than or equal to the default. [default: 8]</t>
       </text>
     </comment>
-    <comment authorId="72" ref="A92" shapeId="0">
+    <comment authorId="73" ref="A93" shapeId="0">
       <text>
         <t>Amount of Webfilter RAM to allocate, in GB. Valid only for KVM deployments. Note: Values smaller than the default are for lab and PoC only. Production deployments must use a value greater than or equal to the default. [default: 8]</t>
       </text>
     </comment>
-    <comment authorId="73" ref="A93" shapeId="0">
+    <comment authorId="74" ref="A94" shapeId="0">
       <text>
         <t>Amount of Portal RAM to allocate, in GB. Valid only for KVM deployments. Note: Values smaller than the default are for lab and PoC only. Production deployments must use a value greater than or equal to the default. [default: 24]</t>
       </text>
     </comment>
-    <comment authorId="74" ref="A95" shapeId="0">
+    <comment authorId="75" ref="A96" shapeId="0">
       <text>
         <t>Valid for only KVM and VCenter deployments. Number of CPU's for VSD. [default: 6]</t>
       </text>
     </comment>
-    <comment authorId="75" ref="A96" shapeId="0">
+    <comment authorId="76" ref="A97" shapeId="0">
       <text>
         <t>Valid for only KVM and VCenter deployments. Number of CPU's for VSC. [default: 6]</t>
       </text>
     </comment>
-    <comment authorId="76" ref="A97" shapeId="0">
+    <comment authorId="77" ref="A98" shapeId="0">
       <text>
         <t>Valid for only KVM and VCenter deployments. Number of CPU's for VSTAT. [default: 6]</t>
       </text>
     </comment>
-    <comment authorId="77" ref="A98" shapeId="0">
+    <comment authorId="78" ref="A99" shapeId="0">
       <text>
         <t>Valid for only KVM and VCenter deployments. Number of CPU's for VNSUTIL. [default: 2]</t>
       </text>
     </comment>
-    <comment authorId="78" ref="A100" shapeId="0">
+    <comment authorId="79" ref="A101" shapeId="0">
       <text>
         <t>Number of CPU's for NUH. Valid only for KVM deployments [default: 2]</t>
       </text>
     </comment>
-    <comment authorId="79" ref="A101" shapeId="0">
+    <comment authorId="80" ref="A102" shapeId="0">
       <text>
         <t>Number of CPU's for VCIN. Valid only for KVM deployments [default: 6]</t>
       </text>
     </comment>
-    <comment authorId="80" ref="A102" shapeId="0">
+    <comment authorId="81" ref="A103" shapeId="0">
       <text>
         <t>Number of CPU's for Portal vm. Valid only for KVM deployments [default: 6]</t>
       </text>
     </comment>
-    <comment authorId="81" ref="A103" shapeId="0">
+    <comment authorId="82" ref="A104" shapeId="0">
       <text>
         <t>Number of CPU's for Webfilter vm. Valid only for KVM deployments [default: 2]</t>
       </text>
     </comment>
-    <comment authorId="82" ref="A105" shapeId="0">
+    <comment authorId="83" ref="A106" shapeId="0">
       <text>
         <t>VSD Architect URL. Required for tasks during Upgrade, Health Checks etc [default: https://(vsd_fqdn):8443]</t>
       </text>
     </comment>
-    <comment authorId="83" ref="A106" shapeId="0">
+    <comment authorId="84" ref="A107" shapeId="0">
       <text>
         <t>Enterprise name used for authentication with VSD Architect. Required for tasks during Upgrade, Health Checks etc [default: csp]</t>
       </text>
     </comment>
-    <comment authorId="84" ref="A107" shapeId="0">
+    <comment authorId="85" ref="A108" shapeId="0">
       <text>
         <t>VCIN URL used for API interaction. Required for tasks like VRS-E upgrade (through VCIN) [default: https://(vcin_ip_address):8443]</t>
       </text>
     </comment>
-    <comment authorId="85" ref="A108" shapeId="0">
+    <comment authorId="86" ref="A109" shapeId="0">
       <text>
         <t>Enterprise name used for authentication with VCIN. Required for tasks like VRS-E upgrade (through VCIN) [default: csp]</t>
       </text>
     </comment>
-    <comment authorId="86" ref="A110" shapeId="0">
+    <comment authorId="87" ref="A111" shapeId="0">
       <text>
         <t>List of hooks files (List items separated by comma.)</t>
       </text>
     </comment>
-    <comment authorId="87" ref="A111" shapeId="0">
+    <comment authorId="88" ref="A112" shapeId="0">
       <text>
         <t>Skip tasks and playbooks (List items separated by comma.)</t>
       </text>
     </comment>
-    <comment authorId="88" ref="A113" shapeId="0">
+    <comment authorId="89" ref="A114" shapeId="0">
       <text>
         <t>Address of SMTP server to be used if emailing health results</t>
       </text>
     </comment>
-    <comment authorId="89" ref="A114" shapeId="0">
+    <comment authorId="90" ref="A115" shapeId="0">
       <text>
         <t>Port to be used on the SMTP Server [default: 25]</t>
       </text>
     </comment>
-    <comment authorId="90" ref="A115" shapeId="0">
+    <comment authorId="91" ref="A116" shapeId="0">
       <text>
         <t>Email address from which health report will be sent</t>
       </text>
     </comment>
-    <comment authorId="91" ref="A116" shapeId="0">
+    <comment authorId="92" ref="A117" shapeId="0">
       <text>
         <t>List of destination email addresses (List items separated by comma.)</t>
       </text>
     </comment>
-    <comment authorId="92" ref="A118" shapeId="0">
+    <comment authorId="93" ref="A119" shapeId="0">
       <text>
         <t>Address of the mail server to be used to receive monit alerts via email</t>
       </text>
     </comment>
-    <comment authorId="93" ref="A119" shapeId="0">
+    <comment authorId="94" ref="A120" shapeId="0">
       <text>
         <t>Port on mail server to be used for monit alerts [default: 25]</t>
       </text>
     </comment>
-    <comment authorId="94" ref="A120" shapeId="0">
+    <comment authorId="95" ref="A121" shapeId="0">
       <text>
         <t>Encryption to be used when sending monit alerts via email</t>
       </text>
     </comment>
-    <comment authorId="95" ref="A121" shapeId="0">
+    <comment authorId="96" ref="A122" shapeId="0">
       <text>
         <t>Enables use of monit eventqueue to store alerts if email alerts fail to send [default: True]</t>
       </text>
     </comment>
-    <comment authorId="96" ref="A122" shapeId="0">
+    <comment authorId="97" ref="A123" shapeId="0">
       <text>
         <t>Email address from which monit alerts will be sent</t>
       </text>
     </comment>
-    <comment authorId="97" ref="A123" shapeId="0">
+    <comment authorId="98" ref="A124" shapeId="0">
       <text>
         <t>Email address to reply to monit alert emails</t>
       </text>
     </comment>
-    <comment authorId="98" ref="A124" shapeId="0">
+    <comment authorId="99" ref="A125" shapeId="0">
       <text>
         <t>Email subject for alert emails. Overrides monit default alert subject</t>
       </text>
     </comment>
-    <comment authorId="99" ref="A125" shapeId="0">
+    <comment authorId="100" ref="A126" shapeId="0">
       <text>
         <t>Email message for alert emails. Overrides monit default alert message</t>
       </text>
     </comment>
-    <comment authorId="100" ref="A126" shapeId="0">
+    <comment authorId="101" ref="A127" shapeId="0">
       <text>
         <t>Destination email address for monit alerts</t>
       </text>
     </comment>
-    <comment authorId="101" ref="A127" shapeId="0">
+    <comment authorId="102" ref="A128" shapeId="0">
       <text>
         <t>Specific events for which alerts should be sent. One string can be used to hold multiple events, separated by commas</t>
       </text>
     </comment>
-    <comment authorId="102" ref="A128" shapeId="0">
+    <comment authorId="103" ref="A129" shapeId="0">
       <text>
         <t>Events for which alerts should not be sent. One string can be used to hold multiple events, separated by commas</t>
       </text>
     </comment>
-    <comment authorId="103" ref="A129" shapeId="0">
+    <comment authorId="104" ref="A130" shapeId="0">
       <text>
         <t>Allowing VSD in-place upgrade during Installation [default: False]</t>
       </text>
@@ -6994,7 +7000,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B129"/>
+  <dimension ref="A1:B130"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7567,7 +7573,7 @@
     <row r="70">
       <c r="A70" s="8" t="inlineStr">
         <is>
-          <t>SD-WAN Portal License File</t>
+          <t>VSTAT License File</t>
         </is>
       </c>
       <c r="B70" s="9" t="n"/>
@@ -7575,30 +7581,30 @@
     <row r="71">
       <c r="A71" s="8" t="inlineStr">
         <is>
+          <t>SD-WAN Portal License File</t>
+        </is>
+      </c>
+      <c r="B71" s="9" t="n"/>
+    </row>
+    <row r="72">
+      <c r="A72" s="8" t="inlineStr">
+        <is>
           <t>NUH License File</t>
         </is>
       </c>
-      <c r="B71" s="9" t="n"/>
-    </row>
-    <row r="72">
-      <c r="A72" s="3" t="inlineStr">
+      <c r="B72" s="9" t="n"/>
+    </row>
+    <row r="73">
+      <c r="A73" s="3" t="inlineStr">
         <is>
           <t>Yum and SSH Proxy</t>
         </is>
       </c>
-    </row>
-    <row r="73">
-      <c r="A73" s="8" t="inlineStr">
-        <is>
-          <t>VSD yum update</t>
-        </is>
-      </c>
-      <c r="B73" s="9" t="n"/>
     </row>
     <row r="74">
       <c r="A74" s="8" t="inlineStr">
         <is>
-          <t>VSTAT yum update</t>
+          <t>VSD yum update</t>
         </is>
       </c>
       <c r="B74" s="9" t="n"/>
@@ -7606,7 +7612,7 @@
     <row r="75">
       <c r="A75" s="8" t="inlineStr">
         <is>
-          <t>Proxy for Yum Updates</t>
+          <t>VSTAT yum update</t>
         </is>
       </c>
       <c r="B75" s="9" t="n"/>
@@ -7614,7 +7620,7 @@
     <row r="76">
       <c r="A76" s="8" t="inlineStr">
         <is>
-          <t>SSH proxy configuration username</t>
+          <t>Proxy for Yum Updates</t>
         </is>
       </c>
       <c r="B76" s="9" t="n"/>
@@ -7622,30 +7628,30 @@
     <row r="77">
       <c r="A77" s="8" t="inlineStr">
         <is>
+          <t>SSH proxy configuration username</t>
+        </is>
+      </c>
+      <c r="B77" s="9" t="n"/>
+    </row>
+    <row r="78">
+      <c r="A78" s="8" t="inlineStr">
+        <is>
           <t>SSH proxy configuration host</t>
         </is>
       </c>
-      <c r="B77" s="9" t="n"/>
-    </row>
-    <row r="78">
-      <c r="A78" s="3" t="inlineStr">
+      <c r="B78" s="9" t="n"/>
+    </row>
+    <row r="79">
+      <c r="A79" s="3" t="inlineStr">
         <is>
           <t>Disk Space</t>
         </is>
       </c>
-    </row>
-    <row r="79">
-      <c r="A79" s="8" t="inlineStr">
-        <is>
-          <t>VSD Disk Size</t>
-        </is>
-      </c>
-      <c r="B79" s="9" t="n"/>
     </row>
     <row r="80">
       <c r="A80" s="8" t="inlineStr">
         <is>
-          <t>VSC Disk Size</t>
+          <t>VSD Disk Size</t>
         </is>
       </c>
       <c r="B80" s="9" t="n"/>
@@ -7653,7 +7659,7 @@
     <row r="81">
       <c r="A81" s="8" t="inlineStr">
         <is>
-          <t>VSTAT Disk Size</t>
+          <t>VSC Disk Size</t>
         </is>
       </c>
       <c r="B81" s="9" t="n"/>
@@ -7661,7 +7667,7 @@
     <row r="82">
       <c r="A82" s="8" t="inlineStr">
         <is>
-          <t>Portal Disk Size</t>
+          <t>VSTAT Disk Size</t>
         </is>
       </c>
       <c r="B82" s="9" t="n"/>
@@ -7669,7 +7675,7 @@
     <row r="83">
       <c r="A83" s="8" t="inlineStr">
         <is>
-          <t>VCIN Disk Size</t>
+          <t>Portal Disk Size</t>
         </is>
       </c>
       <c r="B83" s="9" t="n"/>
@@ -7677,30 +7683,30 @@
     <row r="84">
       <c r="A84" s="8" t="inlineStr">
         <is>
+          <t>VCIN Disk Size</t>
+        </is>
+      </c>
+      <c r="B84" s="9" t="n"/>
+    </row>
+    <row r="85">
+      <c r="A85" s="8" t="inlineStr">
+        <is>
           <t>NSGV Disk Size</t>
         </is>
       </c>
-      <c r="B84" s="9" t="n"/>
-    </row>
-    <row r="85">
-      <c r="A85" s="3" t="inlineStr">
+      <c r="B85" s="9" t="n"/>
+    </row>
+    <row r="86">
+      <c r="A86" s="3" t="inlineStr">
         <is>
           <t>KVM and VCenter RAM</t>
         </is>
       </c>
-    </row>
-    <row r="86">
-      <c r="A86" s="8" t="inlineStr">
-        <is>
-          <t>KVM VSD RAM</t>
-        </is>
-      </c>
-      <c r="B86" s="9" t="n"/>
     </row>
     <row r="87">
       <c r="A87" s="8" t="inlineStr">
         <is>
-          <t>KVM VSC RAM</t>
+          <t>KVM VSD RAM</t>
         </is>
       </c>
       <c r="B87" s="9" t="n"/>
@@ -7708,30 +7714,30 @@
     <row r="88">
       <c r="A88" s="8" t="inlineStr">
         <is>
+          <t>KVM VSC RAM</t>
+        </is>
+      </c>
+      <c r="B88" s="9" t="n"/>
+    </row>
+    <row r="89">
+      <c r="A89" s="8" t="inlineStr">
+        <is>
           <t>KVM VSTAT RAM</t>
         </is>
       </c>
-      <c r="B88" s="9" t="n"/>
-    </row>
-    <row r="89">
-      <c r="A89" s="3" t="inlineStr">
+      <c r="B89" s="9" t="n"/>
+    </row>
+    <row r="90">
+      <c r="A90" s="3" t="inlineStr">
         <is>
           <t>KVM RAM</t>
         </is>
       </c>
-    </row>
-    <row r="90">
-      <c r="A90" s="8" t="inlineStr">
-        <is>
-          <t>KVM VCIN RAM</t>
-        </is>
-      </c>
-      <c r="B90" s="9" t="n"/>
     </row>
     <row r="91">
       <c r="A91" s="8" t="inlineStr">
         <is>
-          <t>KVM NUH RAM</t>
+          <t>KVM VCIN RAM</t>
         </is>
       </c>
       <c r="B91" s="9" t="n"/>
@@ -7739,7 +7745,7 @@
     <row r="92">
       <c r="A92" s="8" t="inlineStr">
         <is>
-          <t>KVM Webfilter RAM</t>
+          <t>KVM NUH RAM</t>
         </is>
       </c>
       <c r="B92" s="9" t="n"/>
@@ -7747,30 +7753,30 @@
     <row r="93">
       <c r="A93" s="8" t="inlineStr">
         <is>
+          <t>KVM Webfilter RAM</t>
+        </is>
+      </c>
+      <c r="B93" s="9" t="n"/>
+    </row>
+    <row r="94">
+      <c r="A94" s="8" t="inlineStr">
+        <is>
           <t>KVM Portal RAM</t>
         </is>
       </c>
-      <c r="B93" s="9" t="n"/>
-    </row>
-    <row r="94">
-      <c r="A94" s="3" t="inlineStr">
+      <c r="B94" s="9" t="n"/>
+    </row>
+    <row r="95">
+      <c r="A95" s="3" t="inlineStr">
         <is>
           <t>KVM and VCenter CPU</t>
         </is>
       </c>
-    </row>
-    <row r="95">
-      <c r="A95" s="8" t="inlineStr">
-        <is>
-          <t>KVM VSD CPU cores</t>
-        </is>
-      </c>
-      <c r="B95" s="9" t="n"/>
     </row>
     <row r="96">
       <c r="A96" s="8" t="inlineStr">
         <is>
-          <t>KVM VSC CPU cores</t>
+          <t>KVM VSD CPU cores</t>
         </is>
       </c>
       <c r="B96" s="9" t="n"/>
@@ -7778,7 +7784,7 @@
     <row r="97">
       <c r="A97" s="8" t="inlineStr">
         <is>
-          <t>KVM VSTAT CPU cores</t>
+          <t>KVM VSC CPU cores</t>
         </is>
       </c>
       <c r="B97" s="9" t="n"/>
@@ -7786,30 +7792,30 @@
     <row r="98">
       <c r="A98" s="8" t="inlineStr">
         <is>
+          <t>KVM VSTAT CPU cores</t>
+        </is>
+      </c>
+      <c r="B98" s="9" t="n"/>
+    </row>
+    <row r="99">
+      <c r="A99" s="8" t="inlineStr">
+        <is>
           <t>KVM VNSUTIL CPU cores</t>
         </is>
       </c>
-      <c r="B98" s="9" t="n"/>
-    </row>
-    <row r="99">
-      <c r="A99" s="3" t="inlineStr">
+      <c r="B99" s="9" t="n"/>
+    </row>
+    <row r="100">
+      <c r="A100" s="3" t="inlineStr">
         <is>
           <t>KVM CPU</t>
         </is>
       </c>
-    </row>
-    <row r="100">
-      <c r="A100" s="8" t="inlineStr">
-        <is>
-          <t>KVM NUH CPU cores</t>
-        </is>
-      </c>
-      <c r="B100" s="9" t="n"/>
     </row>
     <row r="101">
       <c r="A101" s="8" t="inlineStr">
         <is>
-          <t>KVM VCIN CPU cores</t>
+          <t>KVM NUH CPU cores</t>
         </is>
       </c>
       <c r="B101" s="9" t="n"/>
@@ -7817,7 +7823,7 @@
     <row r="102">
       <c r="A102" s="8" t="inlineStr">
         <is>
-          <t>KVM Portal VM CPU cores</t>
+          <t>KVM VCIN CPU cores</t>
         </is>
       </c>
       <c r="B102" s="9" t="n"/>
@@ -7825,30 +7831,30 @@
     <row r="103">
       <c r="A103" s="8" t="inlineStr">
         <is>
+          <t>KVM Portal VM CPU cores</t>
+        </is>
+      </c>
+      <c r="B103" s="9" t="n"/>
+    </row>
+    <row r="104">
+      <c r="A104" s="8" t="inlineStr">
+        <is>
           <t>KVM Webfilter VM CPU cores</t>
         </is>
       </c>
-      <c r="B103" s="9" t="n"/>
-    </row>
-    <row r="104">
-      <c r="A104" s="3" t="inlineStr">
+      <c r="B104" s="9" t="n"/>
+    </row>
+    <row r="105">
+      <c r="A105" s="3" t="inlineStr">
         <is>
           <t>Authentication</t>
         </is>
       </c>
-    </row>
-    <row r="105">
-      <c r="A105" s="8" t="inlineStr">
-        <is>
-          <t>VSD Architect URL</t>
-        </is>
-      </c>
-      <c r="B105" s="9" t="n"/>
     </row>
     <row r="106">
       <c r="A106" s="8" t="inlineStr">
         <is>
-          <t>VSD Enterprise</t>
+          <t>VSD Architect URL</t>
         </is>
       </c>
       <c r="B106" s="9" t="n"/>
@@ -7856,7 +7862,7 @@
     <row r="107">
       <c r="A107" s="8" t="inlineStr">
         <is>
-          <t>VCIN URL</t>
+          <t>VSD Enterprise</t>
         </is>
       </c>
       <c r="B107" s="9" t="n"/>
@@ -7864,53 +7870,53 @@
     <row r="108">
       <c r="A108" s="8" t="inlineStr">
         <is>
+          <t>VCIN URL</t>
+        </is>
+      </c>
+      <c r="B108" s="9" t="n"/>
+    </row>
+    <row r="109">
+      <c r="A109" s="8" t="inlineStr">
+        <is>
           <t>VCIN Enterprise</t>
         </is>
       </c>
-      <c r="B108" s="9" t="n"/>
-    </row>
-    <row r="109">
-      <c r="A109" s="3" t="inlineStr">
+      <c r="B109" s="9" t="n"/>
+    </row>
+    <row r="110">
+      <c r="A110" s="3" t="inlineStr">
         <is>
           <t>Hooks</t>
         </is>
       </c>
-    </row>
-    <row r="110">
-      <c r="A110" s="8" t="inlineStr">
-        <is>
-          <t>hooks</t>
-        </is>
-      </c>
-      <c r="B110" s="9" t="n"/>
     </row>
     <row r="111">
       <c r="A111" s="8" t="inlineStr">
         <is>
+          <t>hooks</t>
+        </is>
+      </c>
+      <c r="B111" s="9" t="n"/>
+    </row>
+    <row r="112">
+      <c r="A112" s="8" t="inlineStr">
+        <is>
           <t>skip actions</t>
         </is>
       </c>
-      <c r="B111" s="9" t="n"/>
-    </row>
-    <row r="112">
-      <c r="A112" s="3" t="inlineStr">
+      <c r="B112" s="9" t="n"/>
+    </row>
+    <row r="113">
+      <c r="A113" s="3" t="inlineStr">
         <is>
           <t>Component Health Report Email Options</t>
         </is>
       </c>
-    </row>
-    <row r="113">
-      <c r="A113" s="8" t="inlineStr">
-        <is>
-          <t>Health Report SMTP Server</t>
-        </is>
-      </c>
-      <c r="B113" s="9" t="n"/>
     </row>
     <row r="114">
       <c r="A114" s="8" t="inlineStr">
         <is>
-          <t>Health Report SMTP Server Port</t>
+          <t>Health Report SMTP Server</t>
         </is>
       </c>
       <c r="B114" s="9" t="n"/>
@@ -7918,7 +7924,7 @@
     <row r="115">
       <c r="A115" s="8" t="inlineStr">
         <is>
-          <t>Health Report Email From Address</t>
+          <t>Health Report SMTP Server Port</t>
         </is>
       </c>
       <c r="B115" s="9" t="n"/>
@@ -7926,30 +7932,30 @@
     <row r="116">
       <c r="A116" s="8" t="inlineStr">
         <is>
+          <t>Health Report Email From Address</t>
+        </is>
+      </c>
+      <c r="B116" s="9" t="n"/>
+    </row>
+    <row r="117">
+      <c r="A117" s="8" t="inlineStr">
+        <is>
           <t>Health Report Destination Email Address(es)</t>
         </is>
       </c>
-      <c r="B116" s="9" t="n"/>
-    </row>
-    <row r="117">
-      <c r="A117" s="3" t="inlineStr">
+      <c r="B117" s="9" t="n"/>
+    </row>
+    <row r="118">
+      <c r="A118" s="3" t="inlineStr">
         <is>
           <t>VSD Monit Email Alerts Configuration</t>
         </is>
       </c>
-    </row>
-    <row r="118">
-      <c r="A118" s="8" t="inlineStr">
-        <is>
-          <t>VSD Monit Mail Server</t>
-        </is>
-      </c>
-      <c r="B118" s="9" t="n"/>
     </row>
     <row r="119">
       <c r="A119" s="8" t="inlineStr">
         <is>
-          <t>VSD Monit Mail Server Port</t>
+          <t>VSD Monit Mail Server</t>
         </is>
       </c>
       <c r="B119" s="9" t="n"/>
@@ -7957,7 +7963,7 @@
     <row r="120">
       <c r="A120" s="8" t="inlineStr">
         <is>
-          <t>VSD Monit Mail Server Encryption Type</t>
+          <t>VSD Monit Mail Server Port</t>
         </is>
       </c>
       <c r="B120" s="9" t="n"/>
@@ -7965,7 +7971,7 @@
     <row r="121">
       <c r="A121" s="8" t="inlineStr">
         <is>
-          <t>Use VSD Monit Eventqueue</t>
+          <t>VSD Monit Mail Server Encryption Type</t>
         </is>
       </c>
       <c r="B121" s="9" t="n"/>
@@ -7973,7 +7979,7 @@
     <row r="122">
       <c r="A122" s="8" t="inlineStr">
         <is>
-          <t>VSD Monit From Email Address</t>
+          <t>Use VSD Monit Eventqueue</t>
         </is>
       </c>
       <c r="B122" s="9" t="n"/>
@@ -7981,7 +7987,7 @@
     <row r="123">
       <c r="A123" s="8" t="inlineStr">
         <is>
-          <t>VSD Monit Reply-To Email Address</t>
+          <t>VSD Monit From Email Address</t>
         </is>
       </c>
       <c r="B123" s="9" t="n"/>
@@ -7989,7 +7995,7 @@
     <row r="124">
       <c r="A124" s="8" t="inlineStr">
         <is>
-          <t>VSD Monit Email Alert Subject</t>
+          <t>VSD Monit Reply-To Email Address</t>
         </is>
       </c>
       <c r="B124" s="9" t="n"/>
@@ -7997,7 +8003,7 @@
     <row r="125">
       <c r="A125" s="8" t="inlineStr">
         <is>
-          <t>VSD Monit Email Alert Message</t>
+          <t>VSD Monit Email Alert Subject</t>
         </is>
       </c>
       <c r="B125" s="9" t="n"/>
@@ -8005,7 +8011,7 @@
     <row r="126">
       <c r="A126" s="8" t="inlineStr">
         <is>
-          <t>VSD Monit Destination Email Address</t>
+          <t>VSD Monit Email Alert Message</t>
         </is>
       </c>
       <c r="B126" s="9" t="n"/>
@@ -8013,7 +8019,7 @@
     <row r="127">
       <c r="A127" s="8" t="inlineStr">
         <is>
-          <t>VSD Monit Only Alert On</t>
+          <t>VSD Monit Destination Email Address</t>
         </is>
       </c>
       <c r="B127" s="9" t="n"/>
@@ -8021,7 +8027,7 @@
     <row r="128">
       <c r="A128" s="8" t="inlineStr">
         <is>
-          <t>VSD Monit Do Not Alert On</t>
+          <t>VSD Monit Only Alert On</t>
         </is>
       </c>
       <c r="B128" s="9" t="n"/>
@@ -8029,10 +8035,18 @@
     <row r="129">
       <c r="A129" s="8" t="inlineStr">
         <is>
+          <t>VSD Monit Do Not Alert On</t>
+        </is>
+      </c>
+      <c r="B129" s="9" t="n"/>
+    </row>
+    <row r="130">
+      <c r="A130" s="8" t="inlineStr">
+        <is>
           <t xml:space="preserve">VSD In-place upgrade during Install </t>
         </is>
       </c>
-      <c r="B129" s="9" t="n"/>
+      <c r="B130" s="9" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="22">
@@ -8048,16 +8062,16 @@
     <mergeCell ref="A54:B54"/>
     <mergeCell ref="A60:B60"/>
     <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="A89:B89"/>
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="A99:B99"/>
-    <mergeCell ref="A104:B104"/>
-    <mergeCell ref="A109:B109"/>
-    <mergeCell ref="A112:B112"/>
-    <mergeCell ref="A117:B117"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="A100:B100"/>
+    <mergeCell ref="A105:B105"/>
+    <mergeCell ref="A110:B110"/>
+    <mergeCell ref="A113:B113"/>
+    <mergeCell ref="A118:B118"/>
   </mergeCells>
   <dataValidations count="42">
     <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="B24" type="list">
@@ -8097,39 +8111,39 @@
     <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="B68" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="B73" type="list">
-      <formula1>"true,false"</formula1>
-    </dataValidation>
     <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="B74" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B79" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="B75" type="list">
+      <formula1>"true,false"</formula1>
+    </dataValidation>
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B80" type="whole"/>
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B81" type="whole"/>
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B82" type="whole"/>
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B83" type="whole"/>
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B84" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B86" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B85" type="whole"/>
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B87" type="whole"/>
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B88" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B90" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B89" type="whole"/>
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B91" type="whole"/>
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B92" type="whole"/>
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B93" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B95" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B94" type="whole"/>
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B96" type="whole"/>
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B97" type="whole"/>
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B98" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B100" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B99" type="whole"/>
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B101" type="whole"/>
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B102" type="whole"/>
     <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B103" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B114" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B119" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="B121" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B104" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B115" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B120" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="B122" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="B129" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="B130" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Changes to VSC Schema
</commit_message>
<xml_diff>
--- a/examples/excel/active_standby_vsds.xlsx
+++ b/examples/excel/active_standby_vsds.xlsx
@@ -16,23 +16,24 @@
     <sheet name="Credentials" sheetId="7" state="visible" r:id="rId7"/>
     <sheet name="Dnss" sheetId="8" state="visible" r:id="rId8"/>
     <sheet name="Netconf managers" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="Nsgv access ports" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="Nsgv bootstrap" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet name="Nsgv network port vlans" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet name="Nsgvs" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet name="Nuh common" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet name="Nuh external interfaces" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet name="Nuh vrrp" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet name="Nuhs" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet name="Portals" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet name="Proxys" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet name="Stcv global" sheetId="20" state="visible" r:id="rId20"/>
-    <sheet name="Stcvs" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet name="Vcins" sheetId="22" state="visible" r:id="rId22"/>
-    <sheet name="Vnsutils" sheetId="23" state="visible" r:id="rId23"/>
-    <sheet name="Vrss" sheetId="24" state="visible" r:id="rId24"/>
-    <sheet name="Vsrs" sheetId="25" state="visible" r:id="rId25"/>
-    <sheet name="Webfilters" sheetId="26" state="visible" r:id="rId26"/>
+    <sheet name="Nfss" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="Nsgv access ports" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="Nsgv bootstrap" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="Nsgv network port vlans" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="Nsgvs" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="Nuh common" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="Nuh external interfaces" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="Nuh vrrp" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="Nuhs" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="Portals" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet name="Proxys" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet name="Stcv global" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet name="Stcvs" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet name="Vcins" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet name="Vnsutils" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet name="Vrss" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet name="Vsrs" sheetId="26" state="visible" r:id="rId26"/>
+    <sheet name="Webfilters" sheetId="27" state="visible" r:id="rId27"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -189,6 +190,33 @@
 <file path=xl/comments/comment10.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
+    <author>hostname</author>
+    <author>nfs_ip</author>
+    <author>mount_directory_location</author>
+  </authors>
+  <commentList>
+    <comment authorId="0" ref="A5" shapeId="0">
+      <text>
+        <t>Hostname of NFS Server</t>
+      </text>
+    </comment>
+    <comment authorId="1" ref="A6" shapeId="0">
+      <text>
+        <t>IP address of the NFS server.</t>
+      </text>
+    </comment>
+    <comment authorId="2" ref="A7" shapeId="0">
+      <text>
+        <t>Optional user specified location of the mount directory to export for the NFS. Defaults to /nfs. [default: /nfs]</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments/comment11.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
     <author>name</author>
     <author>physical_name</author>
     <author>vlan_range</author>
@@ -225,7 +253,7 @@
 </comments>
 </file>
 
-<file path=xl/comments/comment11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments/comment12.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>nsgv_organization</author>
@@ -312,7 +340,7 @@
 </comments>
 </file>
 
-<file path=xl/comments/comment12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments/comment13.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>name</author>
@@ -357,7 +385,7 @@
 </comments>
 </file>
 
-<file path=xl/comments/comment13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments/comment14.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>vmname</author>
@@ -684,7 +712,7 @@
 </comments>
 </file>
 
-<file path=xl/comments/comment14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments/comment15.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>vsdconfig_enable</author>
@@ -705,7 +733,7 @@
 </comments>
 </file>
 
-<file path=xl/comments/comment15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments/comment16.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>name</author>
@@ -762,7 +790,7 @@
 </comments>
 </file>
 
-<file path=xl/comments/comment16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments/comment17.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>router_id</author>
@@ -795,7 +823,7 @@
 </comments>
 </file>
 
-<file path=xl/comments/comment17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments/comment18.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>hostname</author>
@@ -930,7 +958,7 @@
 </comments>
 </file>
 
-<file path=xl/comments/comment18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments/comment19.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>hostname</author>
@@ -1035,99 +1063,6 @@
     <comment authorId="16" ref="A25" shapeId="0">
       <text>
         <t>Portal version to be pulled from Docker hub [default: ]</t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments/comment19.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>hostname</author>
-    <author>vmname</author>
-    <author>target_server_type</author>
-    <author>target_server</author>
-    <author>mgmt_ip</author>
-    <author>mgmt_gateway</author>
-    <author>mgmt_netmask</author>
-    <author>proxy_vm_qcow2_path</author>
-    <author>proxy_vm_qcow2_file_name</author>
-    <author>vcpus</author>
-    <author>ram</author>
-    <author>vsd1_fqdn</author>
-    <author>vsd2_fqdn</author>
-    <author>vsd3_fqdn</author>
-  </authors>
-  <commentList>
-    <comment authorId="0" ref="A5" shapeId="0">
-      <text>
-        <t>Hostname to assign to the PROXY VM</t>
-      </text>
-    </comment>
-    <comment authorId="1" ref="A6" shapeId="0">
-      <text>
-        <t>Vmname to assign to the PROXY VM</t>
-      </text>
-    </comment>
-    <comment authorId="2" ref="A7" shapeId="0">
-      <text>
-        <t>Type of hypervisor environment into which the instance will be created</t>
-      </text>
-    </comment>
-    <comment authorId="3" ref="A8" shapeId="0">
-      <text>
-        <t>Hostname or IP address of the KVM hypervisor where the PROXY VM will be instantiated</t>
-      </text>
-    </comment>
-    <comment authorId="4" ref="A10" shapeId="0">
-      <text>
-        <t>IP address to assign to the management network interface of the PROXY VM</t>
-      </text>
-    </comment>
-    <comment authorId="5" ref="A11" shapeId="0">
-      <text>
-        <t>IP address of the network gateway for the management network interface of the PROXY VM</t>
-      </text>
-    </comment>
-    <comment authorId="6" ref="A12" shapeId="0">
-      <text>
-        <t>Management network netmask for the PROXY VM</t>
-      </text>
-    </comment>
-    <comment authorId="7" ref="A14" shapeId="0">
-      <text>
-        <t>Path to the Proxy qcow2 image</t>
-      </text>
-    </comment>
-    <comment authorId="8" ref="A15" shapeId="0">
-      <text>
-        <t>File name of the Proxy qcow2 image</t>
-      </text>
-    </comment>
-    <comment authorId="9" ref="A16" shapeId="0">
-      <text>
-        <t>Number of vCPUs to apply to the Proxy VM</t>
-      </text>
-    </comment>
-    <comment authorId="10" ref="A17" shapeId="0">
-      <text>
-        <t>Amount of RAM to apply to the Proxy VM</t>
-      </text>
-    </comment>
-    <comment authorId="11" ref="A19" shapeId="0">
-      <text>
-        <t>The FQDN value that VSD1 VM holds</t>
-      </text>
-    </comment>
-    <comment authorId="12" ref="A20" shapeId="0">
-      <text>
-        <t>The FQDN value that VSD2 VM holds</t>
-      </text>
-    </comment>
-    <comment authorId="13" ref="A21" shapeId="0">
-      <text>
-        <t>The FQDN value that VSD3 VM holds</t>
       </text>
     </comment>
   </commentList>
@@ -1345,7 +1280,7 @@
     </comment>
     <comment authorId="20" ref="A30" shapeId="0">
       <text>
-        <t>When true, do not validate the RTT between VSDs in a cluster is less than max RTT [default: False]</t>
+        <t>When true, continue MetroAE execution upon error and do not validate the RTT between VSDs in a cluster is less than max RTT, else stop MetroAE execution upon error [default: False]</t>
       </text>
     </comment>
     <comment authorId="21" ref="A31" shapeId="0">
@@ -1380,7 +1315,7 @@
     </comment>
     <comment authorId="27" ref="A37" shapeId="0">
       <text>
-        <t>When true, ignore the results of the VSD disk performance test [default: False]</t>
+        <t>When true, continue MetroAE execution upon error and ignore the results of the VSD disk performance test, else stop MetroAE execution upon error [default: False]</t>
       </text>
     </comment>
     <comment authorId="28" ref="A38" shapeId="0">
@@ -1768,6 +1703,99 @@
 </file>
 
 <file path=xl/comments/comment20.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>hostname</author>
+    <author>vmname</author>
+    <author>target_server_type</author>
+    <author>target_server</author>
+    <author>mgmt_ip</author>
+    <author>mgmt_gateway</author>
+    <author>mgmt_netmask</author>
+    <author>proxy_vm_qcow2_path</author>
+    <author>proxy_vm_qcow2_file_name</author>
+    <author>vcpus</author>
+    <author>ram</author>
+    <author>vsd1_fqdn</author>
+    <author>vsd2_fqdn</author>
+    <author>vsd3_fqdn</author>
+  </authors>
+  <commentList>
+    <comment authorId="0" ref="A5" shapeId="0">
+      <text>
+        <t>Hostname to assign to the PROXY VM</t>
+      </text>
+    </comment>
+    <comment authorId="1" ref="A6" shapeId="0">
+      <text>
+        <t>Vmname to assign to the PROXY VM</t>
+      </text>
+    </comment>
+    <comment authorId="2" ref="A7" shapeId="0">
+      <text>
+        <t>Type of hypervisor environment into which the instance will be created</t>
+      </text>
+    </comment>
+    <comment authorId="3" ref="A8" shapeId="0">
+      <text>
+        <t>Hostname or IP address of the KVM hypervisor where the PROXY VM will be instantiated</t>
+      </text>
+    </comment>
+    <comment authorId="4" ref="A10" shapeId="0">
+      <text>
+        <t>IP address to assign to the management network interface of the PROXY VM</t>
+      </text>
+    </comment>
+    <comment authorId="5" ref="A11" shapeId="0">
+      <text>
+        <t>IP address of the network gateway for the management network interface of the PROXY VM</t>
+      </text>
+    </comment>
+    <comment authorId="6" ref="A12" shapeId="0">
+      <text>
+        <t>Management network netmask for the PROXY VM</t>
+      </text>
+    </comment>
+    <comment authorId="7" ref="A14" shapeId="0">
+      <text>
+        <t>Path to the Proxy qcow2 image</t>
+      </text>
+    </comment>
+    <comment authorId="8" ref="A15" shapeId="0">
+      <text>
+        <t>File name of the Proxy qcow2 image</t>
+      </text>
+    </comment>
+    <comment authorId="9" ref="A16" shapeId="0">
+      <text>
+        <t>Number of vCPUs to apply to the Proxy VM</t>
+      </text>
+    </comment>
+    <comment authorId="10" ref="A17" shapeId="0">
+      <text>
+        <t>Amount of RAM to apply to the Proxy VM</t>
+      </text>
+    </comment>
+    <comment authorId="11" ref="A19" shapeId="0">
+      <text>
+        <t>The FQDN value that VSD1 VM holds</t>
+      </text>
+    </comment>
+    <comment authorId="12" ref="A20" shapeId="0">
+      <text>
+        <t>The FQDN value that VSD2 VM holds</t>
+      </text>
+    </comment>
+    <comment authorId="13" ref="A21" shapeId="0">
+      <text>
+        <t>The FQDN value that VSD3 VM holds</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments/comment21.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>stcv_image_path</author>
@@ -1794,7 +1822,7 @@
 </comments>
 </file>
 
-<file path=xl/comments/comment21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments/comment22.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>target_server</author>
@@ -1881,7 +1909,7 @@
 </comments>
 </file>
 
-<file path=xl/comments/comment22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments/comment23.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>hostname</author>
@@ -1980,7 +2008,7 @@
 </comments>
 </file>
 
-<file path=xl/comments/comment23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments/comment24.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>hostname</author>
@@ -2235,7 +2263,7 @@
 </comments>
 </file>
 
-<file path=xl/comments/comment24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments/comment25.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>vrs_os_type</author>
@@ -2298,7 +2326,7 @@
 </comments>
 </file>
 
-<file path=xl/comments/comment25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments/comment26.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>hostname</author>
@@ -2409,7 +2437,7 @@
 </comments>
 </file>
 
-<file path=xl/comments/comment26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments/comment27.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>hostname</author>
@@ -2422,6 +2450,9 @@
     <author>target_server</author>
     <author>cpuset</author>
     <author>cert_name</author>
+    <author>web_http_proxy</author>
+    <author>web_proxy_host</author>
+    <author>web_proxy_port</author>
     <author>run_incompass_operation</author>
   </authors>
   <commentList>
@@ -2476,6 +2507,21 @@
       </text>
     </comment>
     <comment authorId="10" ref="A17" shapeId="0">
+      <text>
+        <t>Optional HTTP Proxy for webfilter VM [default: ]</t>
+      </text>
+    </comment>
+    <comment authorId="11" ref="A18" shapeId="0">
+      <text>
+        <t>HTTP Proxy host for webfilter proxy [default: ]</t>
+      </text>
+    </comment>
+    <comment authorId="12" ref="A19" shapeId="0">
+      <text>
+        <t>HTTP Proxy port for webfilter proxy [default: ]</t>
+      </text>
+    </comment>
+    <comment authorId="13" ref="A20" shapeId="0">
       <text>
         <t>Run incompass operation command. This is enabled by default and may take up to 20 minutes and requires internet connection. [default: True]</t>
       </text>
@@ -2878,6 +2924,7 @@
     <author>enable_hardening</author>
     <author>vsc_config_file_paths</author>
     <author>override_vsc_config</author>
+    <author>custom_vsc_config_filename</author>
   </authors>
   <commentList>
     <comment authorId="0" ref="A5" shapeId="0">
@@ -3183,6 +3230,11 @@
     <comment authorId="60" ref="A75" shapeId="0">
       <text>
         <t>This will override the Metro Provided config on the VSC by the config provided in vsc_config_file_paths [default: False]</t>
+      </text>
+    </comment>
+    <comment authorId="61" ref="A76" shapeId="0">
+      <text>
+        <t>Custom VSC Config Filename. Used only for upgrades</t>
       </text>
     </comment>
   </commentList>
@@ -3516,6 +3568,7 @@
     <author>portal_custom_password</author>
     <author>smtp_auth_username</author>
     <author>smtp_auth_password</author>
+    <author>nfs_custom_username</author>
     <author>netconf_vm_username</author>
     <author>netconf_vm_password</author>
     <author>netconf_username</author>
@@ -3725,62 +3778,67 @@
         <t>Password for SMTP authentication [default: ]</t>
       </text>
     </comment>
-    <comment authorId="39" ref="A55" shapeId="0">
+    <comment authorId="39" ref="A54" shapeId="0">
+      <text>
+        <t>NFS username to login into command line. Default user is root [default: root]</t>
+      </text>
+    </comment>
+    <comment authorId="40" ref="A56" shapeId="0">
       <text>
         <t>Username for NETCONF Manager VM. Default user is root [default: root]</t>
       </text>
     </comment>
-    <comment authorId="40" ref="A56" shapeId="0">
+    <comment authorId="41" ref="A57" shapeId="0">
       <text>
         <t>Password for NETCONF manager VM [default: ]</t>
       </text>
     </comment>
-    <comment authorId="41" ref="A57" shapeId="0">
+    <comment authorId="42" ref="A58" shapeId="0">
       <text>
         <t>Username for NETCONF Manager user [default: netconfmgr]</t>
       </text>
     </comment>
-    <comment authorId="42" ref="A58" shapeId="0">
+    <comment authorId="43" ref="A59" shapeId="0">
       <text>
         <t>Password for NETCONF manager user [default: password]</t>
       </text>
     </comment>
-    <comment authorId="43" ref="A60" shapeId="0">
+    <comment authorId="44" ref="A61" shapeId="0">
       <text>
         <t>Username for SMTP Server</t>
       </text>
     </comment>
-    <comment authorId="44" ref="A61" shapeId="0">
+    <comment authorId="45" ref="A62" shapeId="0">
       <text>
         <t>Password for SMTP Server</t>
       </text>
     </comment>
-    <comment authorId="45" ref="A63" shapeId="0">
+    <comment authorId="46" ref="A64" shapeId="0">
       <text>
         <t>Username for the monit mail server</t>
       </text>
     </comment>
-    <comment authorId="46" ref="A64" shapeId="0">
+    <comment authorId="47" ref="A65" shapeId="0">
       <text>
         <t>Password for the monit mail server</t>
       </text>
     </comment>
-    <comment authorId="47" ref="A66" shapeId="0">
+    <comment authorId="48" ref="A67" shapeId="0">
       <text>
         <t>Username for NUH notification application</t>
       </text>
     </comment>
-    <comment authorId="48" ref="A67" shapeId="0">
+    <comment authorId="49" ref="A68" shapeId="0">
       <text>
         <t>Password for NUH notification application</t>
       </text>
     </comment>
-    <comment authorId="49" ref="A68" shapeId="0">
+    <comment authorId="50" ref="A69" shapeId="0">
       <text>
         <t>Username for NUH notification application</t>
       </text>
     </comment>
-    <comment authorId="50" ref="A69" shapeId="0">
+    <comment authorId="51" ref="A70" shapeId="0">
       <text>
         <t>Password for NUH notification application</t>
       </text>
@@ -4298,6 +4356,98 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col customWidth="1" max="1" min="1" width="70"/>
+    <col customWidth="1" max="2" min="2" width="25"/>
+    <col customWidth="1" max="3" min="3" width="25"/>
+    <col customWidth="1" max="4" min="4" width="25"/>
+    <col customWidth="1" max="5" min="5" width="25"/>
+    <col customWidth="1" max="6" min="6" width="25"/>
+    <col customWidth="1" max="7" min="7" width="25"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>NFS Server VM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>Configure NFS Server VM using MetroAE. Note: Metroae will not bring up the NFS server, it will configure it for Elasticsearch mounting.</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="inlineStr">
+        <is>
+          <t>NFS parameters</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="4" t="inlineStr">
+        <is>
+          <t>Hostname</t>
+        </is>
+      </c>
+      <c r="B5" s="5" t="n"/>
+      <c r="C5" s="5" t="n"/>
+      <c r="D5" s="5" t="n"/>
+      <c r="E5" s="5" t="n"/>
+      <c r="F5" s="5" t="n"/>
+      <c r="G5" s="5" t="n"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="inlineStr">
+        <is>
+          <t>NFS server IP address</t>
+        </is>
+      </c>
+      <c r="B6" s="5" t="n"/>
+      <c r="C6" s="5" t="n"/>
+      <c r="D6" s="5" t="n"/>
+      <c r="E6" s="5" t="n"/>
+      <c r="F6" s="5" t="n"/>
+      <c r="G6" s="5" t="n"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="8" t="inlineStr">
+        <is>
+          <t>NFS mount directory location</t>
+        </is>
+      </c>
+      <c r="B7" s="9" t="n"/>
+      <c r="C7" s="9" t="n"/>
+      <c r="D7" s="9" t="n"/>
+      <c r="E7" s="9" t="n"/>
+      <c r="F7" s="9" t="n"/>
+      <c r="G7" s="9" t="n"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A4:G4"/>
+  </mergeCells>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <legacyDrawing r:id="anysvml"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4418,7 +4568,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4600,7 +4750,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4757,7 +4907,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -5707,7 +5857,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -5779,7 +5929,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -5950,7 +6100,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -6081,7 +6231,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -6515,7 +6665,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -6883,297 +7033,6 @@
     <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="G24" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
-  </dataValidations>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <legacyDrawing r:id="anysvml"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col customWidth="1" max="1" min="1" width="70"/>
-    <col customWidth="1" max="2" min="2" width="25"/>
-    <col customWidth="1" max="3" min="3" width="25"/>
-    <col customWidth="1" max="4" min="4" width="25"/>
-    <col customWidth="1" max="5" min="5" width="25"/>
-    <col customWidth="1" max="6" min="6" width="25"/>
-    <col customWidth="1" max="7" min="7" width="25"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Proxy VM</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="inlineStr">
-        <is>
-          <t>Specify configuration for Proxy to Architect</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="3" t="inlineStr">
-        <is>
-          <t>Host and target server info</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="6" t="inlineStr">
-        <is>
-          <t>Hostname</t>
-        </is>
-      </c>
-      <c r="B5" s="7" t="n"/>
-      <c r="C5" s="7" t="n"/>
-      <c r="D5" s="7" t="n"/>
-      <c r="E5" s="7" t="n"/>
-      <c r="F5" s="7" t="n"/>
-      <c r="G5" s="7" t="n"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="6" t="inlineStr">
-        <is>
-          <t>Vmname</t>
-        </is>
-      </c>
-      <c r="B6" s="7" t="n"/>
-      <c r="C6" s="7" t="n"/>
-      <c r="D6" s="7" t="n"/>
-      <c r="E6" s="7" t="n"/>
-      <c r="F6" s="7" t="n"/>
-      <c r="G6" s="7" t="n"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="6" t="inlineStr">
-        <is>
-          <t>Target Server Type</t>
-        </is>
-      </c>
-      <c r="B7" s="7" t="n"/>
-      <c r="C7" s="7" t="n"/>
-      <c r="D7" s="7" t="n"/>
-      <c r="E7" s="7" t="n"/>
-      <c r="F7" s="7" t="n"/>
-      <c r="G7" s="7" t="n"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="6" t="inlineStr">
-        <is>
-          <t>Target Server IP or FQDN</t>
-        </is>
-      </c>
-      <c r="B8" s="7" t="n"/>
-      <c r="C8" s="7" t="n"/>
-      <c r="D8" s="7" t="n"/>
-      <c r="E8" s="7" t="n"/>
-      <c r="F8" s="7" t="n"/>
-      <c r="G8" s="7" t="n"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="3" t="inlineStr">
-        <is>
-          <t>Management network</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="6" t="inlineStr">
-        <is>
-          <t>Management IP Address</t>
-        </is>
-      </c>
-      <c r="B10" s="7" t="n"/>
-      <c r="C10" s="7" t="n"/>
-      <c r="D10" s="7" t="n"/>
-      <c r="E10" s="7" t="n"/>
-      <c r="F10" s="7" t="n"/>
-      <c r="G10" s="7" t="n"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="6" t="inlineStr">
-        <is>
-          <t>Management Network Gateway</t>
-        </is>
-      </c>
-      <c r="B11" s="7" t="n"/>
-      <c r="C11" s="7" t="n"/>
-      <c r="D11" s="7" t="n"/>
-      <c r="E11" s="7" t="n"/>
-      <c r="F11" s="7" t="n"/>
-      <c r="G11" s="7" t="n"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="6" t="inlineStr">
-        <is>
-          <t>Management Network Prefix Length</t>
-        </is>
-      </c>
-      <c r="B12" s="7" t="n"/>
-      <c r="C12" s="7" t="n"/>
-      <c r="D12" s="7" t="n"/>
-      <c r="E12" s="7" t="n"/>
-      <c r="F12" s="7" t="n"/>
-      <c r="G12" s="7" t="n"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="3" t="inlineStr">
-        <is>
-          <t>VM details</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="6" t="inlineStr">
-        <is>
-          <t>Image path of the Proxy VM</t>
-        </is>
-      </c>
-      <c r="B14" s="7" t="n"/>
-      <c r="C14" s="7" t="n"/>
-      <c r="D14" s="7" t="n"/>
-      <c r="E14" s="7" t="n"/>
-      <c r="F14" s="7" t="n"/>
-      <c r="G14" s="7" t="n"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="6" t="inlineStr">
-        <is>
-          <t>Image file name of the Proxy VM</t>
-        </is>
-      </c>
-      <c r="B15" s="7" t="n"/>
-      <c r="C15" s="7" t="n"/>
-      <c r="D15" s="7" t="n"/>
-      <c r="E15" s="7" t="n"/>
-      <c r="F15" s="7" t="n"/>
-      <c r="G15" s="7" t="n"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="6" t="inlineStr">
-        <is>
-          <t>VM VCPUs</t>
-        </is>
-      </c>
-      <c r="B16" s="7" t="n"/>
-      <c r="C16" s="7" t="n"/>
-      <c r="D16" s="7" t="n"/>
-      <c r="E16" s="7" t="n"/>
-      <c r="F16" s="7" t="n"/>
-      <c r="G16" s="7" t="n"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="6" t="inlineStr">
-        <is>
-          <t>VM RAM</t>
-        </is>
-      </c>
-      <c r="B17" s="7" t="n"/>
-      <c r="C17" s="7" t="n"/>
-      <c r="D17" s="7" t="n"/>
-      <c r="E17" s="7" t="n"/>
-      <c r="F17" s="7" t="n"/>
-      <c r="G17" s="7" t="n"/>
-    </row>
-    <row r="18">
-      <c r="A18" s="3" t="inlineStr">
-        <is>
-          <t>VSD fqdn</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="6" t="inlineStr">
-        <is>
-          <t>FQDN of VSD1</t>
-        </is>
-      </c>
-      <c r="B19" s="7" t="n"/>
-      <c r="C19" s="7" t="n"/>
-      <c r="D19" s="7" t="n"/>
-      <c r="E19" s="7" t="n"/>
-      <c r="F19" s="7" t="n"/>
-      <c r="G19" s="7" t="n"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="6" t="inlineStr">
-        <is>
-          <t>FQDN of VSD2</t>
-        </is>
-      </c>
-      <c r="B20" s="7" t="n"/>
-      <c r="C20" s="7" t="n"/>
-      <c r="D20" s="7" t="n"/>
-      <c r="E20" s="7" t="n"/>
-      <c r="F20" s="7" t="n"/>
-      <c r="G20" s="7" t="n"/>
-    </row>
-    <row r="21">
-      <c r="A21" s="6" t="inlineStr">
-        <is>
-          <t>FQDN of VSD3</t>
-        </is>
-      </c>
-      <c r="B21" s="7" t="n"/>
-      <c r="C21" s="7" t="n"/>
-      <c r="D21" s="7" t="n"/>
-      <c r="E21" s="7" t="n"/>
-      <c r="F21" s="7" t="n"/>
-      <c r="G21" s="7" t="n"/>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="A9:G9"/>
-    <mergeCell ref="A13:G13"/>
-    <mergeCell ref="A18:G18"/>
-  </mergeCells>
-  <dataValidations count="18">
-    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="B7" type="list">
-      <formula1>"kvm,vcenter"</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="C7" type="list">
-      <formula1>"kvm,vcenter"</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="D7" type="list">
-      <formula1>"kvm,vcenter"</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="E7" type="list">
-      <formula1>"kvm,vcenter"</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="F7" type="list">
-      <formula1>"kvm,vcenter"</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="G7" type="list">
-      <formula1>"kvm,vcenter"</formula1>
-    </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B16" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="C16" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="D16" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="E16" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="F16" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="G16" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B17" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="C17" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="D17" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="E17" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="F17" type="whole"/>
-    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="G17" type="whole"/>
   </dataValidations>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <legacyDrawing r:id="anysvml"/>
@@ -8336,6 +8195,297 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:G21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col customWidth="1" max="1" min="1" width="70"/>
+    <col customWidth="1" max="2" min="2" width="25"/>
+    <col customWidth="1" max="3" min="3" width="25"/>
+    <col customWidth="1" max="4" min="4" width="25"/>
+    <col customWidth="1" max="5" min="5" width="25"/>
+    <col customWidth="1" max="6" min="6" width="25"/>
+    <col customWidth="1" max="7" min="7" width="25"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Proxy VM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>Specify configuration for Proxy to Architect</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="inlineStr">
+        <is>
+          <t>Host and target server info</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="6" t="inlineStr">
+        <is>
+          <t>Hostname</t>
+        </is>
+      </c>
+      <c r="B5" s="7" t="n"/>
+      <c r="C5" s="7" t="n"/>
+      <c r="D5" s="7" t="n"/>
+      <c r="E5" s="7" t="n"/>
+      <c r="F5" s="7" t="n"/>
+      <c r="G5" s="7" t="n"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="6" t="inlineStr">
+        <is>
+          <t>Vmname</t>
+        </is>
+      </c>
+      <c r="B6" s="7" t="n"/>
+      <c r="C6" s="7" t="n"/>
+      <c r="D6" s="7" t="n"/>
+      <c r="E6" s="7" t="n"/>
+      <c r="F6" s="7" t="n"/>
+      <c r="G6" s="7" t="n"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="6" t="inlineStr">
+        <is>
+          <t>Target Server Type</t>
+        </is>
+      </c>
+      <c r="B7" s="7" t="n"/>
+      <c r="C7" s="7" t="n"/>
+      <c r="D7" s="7" t="n"/>
+      <c r="E7" s="7" t="n"/>
+      <c r="F7" s="7" t="n"/>
+      <c r="G7" s="7" t="n"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="6" t="inlineStr">
+        <is>
+          <t>Target Server IP or FQDN</t>
+        </is>
+      </c>
+      <c r="B8" s="7" t="n"/>
+      <c r="C8" s="7" t="n"/>
+      <c r="D8" s="7" t="n"/>
+      <c r="E8" s="7" t="n"/>
+      <c r="F8" s="7" t="n"/>
+      <c r="G8" s="7" t="n"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="3" t="inlineStr">
+        <is>
+          <t>Management network</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="6" t="inlineStr">
+        <is>
+          <t>Management IP Address</t>
+        </is>
+      </c>
+      <c r="B10" s="7" t="n"/>
+      <c r="C10" s="7" t="n"/>
+      <c r="D10" s="7" t="n"/>
+      <c r="E10" s="7" t="n"/>
+      <c r="F10" s="7" t="n"/>
+      <c r="G10" s="7" t="n"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="6" t="inlineStr">
+        <is>
+          <t>Management Network Gateway</t>
+        </is>
+      </c>
+      <c r="B11" s="7" t="n"/>
+      <c r="C11" s="7" t="n"/>
+      <c r="D11" s="7" t="n"/>
+      <c r="E11" s="7" t="n"/>
+      <c r="F11" s="7" t="n"/>
+      <c r="G11" s="7" t="n"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="6" t="inlineStr">
+        <is>
+          <t>Management Network Prefix Length</t>
+        </is>
+      </c>
+      <c r="B12" s="7" t="n"/>
+      <c r="C12" s="7" t="n"/>
+      <c r="D12" s="7" t="n"/>
+      <c r="E12" s="7" t="n"/>
+      <c r="F12" s="7" t="n"/>
+      <c r="G12" s="7" t="n"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="3" t="inlineStr">
+        <is>
+          <t>VM details</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="6" t="inlineStr">
+        <is>
+          <t>Image path of the Proxy VM</t>
+        </is>
+      </c>
+      <c r="B14" s="7" t="n"/>
+      <c r="C14" s="7" t="n"/>
+      <c r="D14" s="7" t="n"/>
+      <c r="E14" s="7" t="n"/>
+      <c r="F14" s="7" t="n"/>
+      <c r="G14" s="7" t="n"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="6" t="inlineStr">
+        <is>
+          <t>Image file name of the Proxy VM</t>
+        </is>
+      </c>
+      <c r="B15" s="7" t="n"/>
+      <c r="C15" s="7" t="n"/>
+      <c r="D15" s="7" t="n"/>
+      <c r="E15" s="7" t="n"/>
+      <c r="F15" s="7" t="n"/>
+      <c r="G15" s="7" t="n"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="6" t="inlineStr">
+        <is>
+          <t>VM VCPUs</t>
+        </is>
+      </c>
+      <c r="B16" s="7" t="n"/>
+      <c r="C16" s="7" t="n"/>
+      <c r="D16" s="7" t="n"/>
+      <c r="E16" s="7" t="n"/>
+      <c r="F16" s="7" t="n"/>
+      <c r="G16" s="7" t="n"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="6" t="inlineStr">
+        <is>
+          <t>VM RAM</t>
+        </is>
+      </c>
+      <c r="B17" s="7" t="n"/>
+      <c r="C17" s="7" t="n"/>
+      <c r="D17" s="7" t="n"/>
+      <c r="E17" s="7" t="n"/>
+      <c r="F17" s="7" t="n"/>
+      <c r="G17" s="7" t="n"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="3" t="inlineStr">
+        <is>
+          <t>VSD fqdn</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="6" t="inlineStr">
+        <is>
+          <t>FQDN of VSD1</t>
+        </is>
+      </c>
+      <c r="B19" s="7" t="n"/>
+      <c r="C19" s="7" t="n"/>
+      <c r="D19" s="7" t="n"/>
+      <c r="E19" s="7" t="n"/>
+      <c r="F19" s="7" t="n"/>
+      <c r="G19" s="7" t="n"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="6" t="inlineStr">
+        <is>
+          <t>FQDN of VSD2</t>
+        </is>
+      </c>
+      <c r="B20" s="7" t="n"/>
+      <c r="C20" s="7" t="n"/>
+      <c r="D20" s="7" t="n"/>
+      <c r="E20" s="7" t="n"/>
+      <c r="F20" s="7" t="n"/>
+      <c r="G20" s="7" t="n"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="6" t="inlineStr">
+        <is>
+          <t>FQDN of VSD3</t>
+        </is>
+      </c>
+      <c r="B21" s="7" t="n"/>
+      <c r="C21" s="7" t="n"/>
+      <c r="D21" s="7" t="n"/>
+      <c r="E21" s="7" t="n"/>
+      <c r="F21" s="7" t="n"/>
+      <c r="G21" s="7" t="n"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="A9:G9"/>
+    <mergeCell ref="A13:G13"/>
+    <mergeCell ref="A18:G18"/>
+  </mergeCells>
+  <dataValidations count="18">
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="B7" type="list">
+      <formula1>"kvm,vcenter"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="C7" type="list">
+      <formula1>"kvm,vcenter"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="D7" type="list">
+      <formula1>"kvm,vcenter"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="E7" type="list">
+      <formula1>"kvm,vcenter"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="F7" type="list">
+      <formula1>"kvm,vcenter"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="G7" type="list">
+      <formula1>"kvm,vcenter"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B16" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="C16" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="D16" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="E16" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="F16" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="G16" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="B17" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="C17" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="D17" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="E17" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="F17" type="whole"/>
+    <dataValidation allowBlank="1" error="Your entry is not an integer, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please provide integer" promptTitle="Integer Selection" showErrorMessage="1" showInputMessage="1" sqref="G17" type="whole"/>
+  </dataValidations>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <legacyDrawing r:id="anysvml"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8402,7 +8552,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -8686,7 +8836,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -8984,7 +9134,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -9678,7 +9828,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -9902,7 +10052,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -10226,13 +10376,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10417,7 +10567,7 @@
     <row r="17">
       <c r="A17" s="8" t="inlineStr">
         <is>
-          <t>Run incompass operation command</t>
+          <t>Http proxy</t>
         </is>
       </c>
       <c r="B17" s="9" t="n"/>
@@ -10426,6 +10576,45 @@
       <c r="E17" s="9" t="n"/>
       <c r="F17" s="9" t="n"/>
       <c r="G17" s="9" t="n"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="8" t="inlineStr">
+        <is>
+          <t>Http proxy host</t>
+        </is>
+      </c>
+      <c r="B18" s="9" t="n"/>
+      <c r="C18" s="9" t="n"/>
+      <c r="D18" s="9" t="n"/>
+      <c r="E18" s="9" t="n"/>
+      <c r="F18" s="9" t="n"/>
+      <c r="G18" s="9" t="n"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="8" t="inlineStr">
+        <is>
+          <t>Http proxy port</t>
+        </is>
+      </c>
+      <c r="B19" s="9" t="n"/>
+      <c r="C19" s="9" t="n"/>
+      <c r="D19" s="9" t="n"/>
+      <c r="E19" s="9" t="n"/>
+      <c r="F19" s="9" t="n"/>
+      <c r="G19" s="9" t="n"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="8" t="inlineStr">
+        <is>
+          <t>Run incompass operation command</t>
+        </is>
+      </c>
+      <c r="B20" s="9" t="n"/>
+      <c r="C20" s="9" t="n"/>
+      <c r="D20" s="9" t="n"/>
+      <c r="E20" s="9" t="n"/>
+      <c r="F20" s="9" t="n"/>
+      <c r="G20" s="9" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -10458,22 +10647,22 @@
     <dataValidation allowBlank="1" error="Your entry is not in the list, Change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select from the list" promptTitle="List Selection" showErrorMessage="1" showInputMessage="1" sqref="G12" type="list">
       <formula1>"kvm"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="B17" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="B20" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="C17" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="C20" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="D17" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="D20" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="E17" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="E20" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="F17" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="F20" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="G17" type="list">
+    <dataValidation allowBlank="1" error="Your entry is not true or false, change anyway?" errorStyle="warning" errorTitle="Invalid Entry" prompt="Please select true or false" promptTitle="True or False Selection" showErrorMessage="1" showInputMessage="1" sqref="G20" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
   </dataValidations>
@@ -11555,7 +11744,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C75"/>
+  <dimension ref="A1:C76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12207,6 +12396,15 @@
       </c>
       <c r="B75" s="9" t="n"/>
       <c r="C75" s="9" t="n"/>
+    </row>
+    <row r="76">
+      <c r="A76" s="8" t="inlineStr">
+        <is>
+          <t>Custom VSC Config Filename</t>
+        </is>
+      </c>
+      <c r="B76" s="9" t="n"/>
+      <c r="C76" s="9" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -13122,7 +13320,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G69"/>
+  <dimension ref="A1:G70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13707,7 +13905,7 @@
     <row r="51">
       <c r="A51" s="3" t="inlineStr">
         <is>
-          <t>SMTP</t>
+          <t>SMTP and NFS</t>
         </is>
       </c>
     </row>
@@ -13738,29 +13936,29 @@
       <c r="G53" s="7" t="n"/>
     </row>
     <row r="54">
-      <c r="A54" s="3" t="inlineStr">
+      <c r="A54" s="6" t="inlineStr">
+        <is>
+          <t>NFS System Username</t>
+        </is>
+      </c>
+      <c r="B54" s="7" t="n"/>
+      <c r="C54" s="7" t="n"/>
+      <c r="D54" s="7" t="n"/>
+      <c r="E54" s="7" t="n"/>
+      <c r="F54" s="7" t="n"/>
+      <c r="G54" s="7" t="n"/>
+    </row>
+    <row r="55">
+      <c r="A55" s="3" t="inlineStr">
         <is>
           <t>NETCONF Manager</t>
         </is>
       </c>
-    </row>
-    <row r="55">
-      <c r="A55" s="6" t="inlineStr">
-        <is>
-          <t>NETCONF Manager VM username</t>
-        </is>
-      </c>
-      <c r="B55" s="7" t="n"/>
-      <c r="C55" s="7" t="n"/>
-      <c r="D55" s="7" t="n"/>
-      <c r="E55" s="7" t="n"/>
-      <c r="F55" s="7" t="n"/>
-      <c r="G55" s="7" t="n"/>
     </row>
     <row r="56">
       <c r="A56" s="6" t="inlineStr">
         <is>
-          <t>NETCONF Manager VM password for running sudo commands</t>
+          <t>NETCONF Manager VM username</t>
         </is>
       </c>
       <c r="B56" s="7" t="n"/>
@@ -13773,7 +13971,7 @@
     <row r="57">
       <c r="A57" s="6" t="inlineStr">
         <is>
-          <t>NETCONF Manager username</t>
+          <t>NETCONF Manager VM password for running sudo commands</t>
         </is>
       </c>
       <c r="B57" s="7" t="n"/>
@@ -13786,7 +13984,7 @@
     <row r="58">
       <c r="A58" s="6" t="inlineStr">
         <is>
-          <t>NETCONF Manager password</t>
+          <t>NETCONF Manager username</t>
         </is>
       </c>
       <c r="B58" s="7" t="n"/>
@@ -13797,29 +13995,29 @@
       <c r="G58" s="7" t="n"/>
     </row>
     <row r="59">
-      <c r="A59" s="3" t="inlineStr">
+      <c r="A59" s="6" t="inlineStr">
+        <is>
+          <t>NETCONF Manager password</t>
+        </is>
+      </c>
+      <c r="B59" s="7" t="n"/>
+      <c r="C59" s="7" t="n"/>
+      <c r="D59" s="7" t="n"/>
+      <c r="E59" s="7" t="n"/>
+      <c r="F59" s="7" t="n"/>
+      <c r="G59" s="7" t="n"/>
+    </row>
+    <row r="60">
+      <c r="A60" s="3" t="inlineStr">
         <is>
           <t>Health Report Email Server</t>
         </is>
       </c>
-    </row>
-    <row r="60">
-      <c r="A60" s="6" t="inlineStr">
-        <is>
-          <t>Health Report SMTP Server Username</t>
-        </is>
-      </c>
-      <c r="B60" s="7" t="n"/>
-      <c r="C60" s="7" t="n"/>
-      <c r="D60" s="7" t="n"/>
-      <c r="E60" s="7" t="n"/>
-      <c r="F60" s="7" t="n"/>
-      <c r="G60" s="7" t="n"/>
     </row>
     <row r="61">
       <c r="A61" s="6" t="inlineStr">
         <is>
-          <t>Health Report SMTP Server Password</t>
+          <t>Health Report SMTP Server Username</t>
         </is>
       </c>
       <c r="B61" s="7" t="n"/>
@@ -13830,29 +14028,29 @@
       <c r="G61" s="7" t="n"/>
     </row>
     <row r="62">
-      <c r="A62" s="3" t="inlineStr">
+      <c r="A62" s="6" t="inlineStr">
+        <is>
+          <t>Health Report SMTP Server Password</t>
+        </is>
+      </c>
+      <c r="B62" s="7" t="n"/>
+      <c r="C62" s="7" t="n"/>
+      <c r="D62" s="7" t="n"/>
+      <c r="E62" s="7" t="n"/>
+      <c r="F62" s="7" t="n"/>
+      <c r="G62" s="7" t="n"/>
+    </row>
+    <row r="63">
+      <c r="A63" s="3" t="inlineStr">
         <is>
           <t>Monit Alerts Email Server</t>
         </is>
       </c>
-    </row>
-    <row r="63">
-      <c r="A63" s="6" t="inlineStr">
-        <is>
-          <t>VSD Monit Mail Server Username</t>
-        </is>
-      </c>
-      <c r="B63" s="7" t="n"/>
-      <c r="C63" s="7" t="n"/>
-      <c r="D63" s="7" t="n"/>
-      <c r="E63" s="7" t="n"/>
-      <c r="F63" s="7" t="n"/>
-      <c r="G63" s="7" t="n"/>
     </row>
     <row r="64">
       <c r="A64" s="6" t="inlineStr">
         <is>
-          <t>VSD Monit Mail Server Password</t>
+          <t>VSD Monit Mail Server Username</t>
         </is>
       </c>
       <c r="B64" s="7" t="n"/>
@@ -13863,29 +14061,29 @@
       <c r="G64" s="7" t="n"/>
     </row>
     <row r="65">
-      <c r="A65" s="3" t="inlineStr">
+      <c r="A65" s="6" t="inlineStr">
+        <is>
+          <t>VSD Monit Mail Server Password</t>
+        </is>
+      </c>
+      <c r="B65" s="7" t="n"/>
+      <c r="C65" s="7" t="n"/>
+      <c r="D65" s="7" t="n"/>
+      <c r="E65" s="7" t="n"/>
+      <c r="F65" s="7" t="n"/>
+      <c r="G65" s="7" t="n"/>
+    </row>
+    <row r="66">
+      <c r="A66" s="3" t="inlineStr">
         <is>
           <t>NUH notification application</t>
         </is>
       </c>
-    </row>
-    <row r="66">
-      <c r="A66" s="6" t="inlineStr">
-        <is>
-          <t>NUH notification application 1 username</t>
-        </is>
-      </c>
-      <c r="B66" s="7" t="n"/>
-      <c r="C66" s="7" t="n"/>
-      <c r="D66" s="7" t="n"/>
-      <c r="E66" s="7" t="n"/>
-      <c r="F66" s="7" t="n"/>
-      <c r="G66" s="7" t="n"/>
     </row>
     <row r="67">
       <c r="A67" s="6" t="inlineStr">
         <is>
-          <t>NUH notification application 1 password</t>
+          <t>NUH notification application 1 username</t>
         </is>
       </c>
       <c r="B67" s="7" t="n"/>
@@ -13898,7 +14096,7 @@
     <row r="68">
       <c r="A68" s="6" t="inlineStr">
         <is>
-          <t>NUH notification application 2 username</t>
+          <t>NUH notification application 1 password</t>
         </is>
       </c>
       <c r="B68" s="7" t="n"/>
@@ -13911,7 +14109,7 @@
     <row r="69">
       <c r="A69" s="6" t="inlineStr">
         <is>
-          <t>NUH notification application 2 password</t>
+          <t>NUH notification application 2 username</t>
         </is>
       </c>
       <c r="B69" s="7" t="n"/>
@@ -13920,6 +14118,19 @@
       <c r="E69" s="7" t="n"/>
       <c r="F69" s="7" t="n"/>
       <c r="G69" s="7" t="n"/>
+    </row>
+    <row r="70">
+      <c r="A70" s="6" t="inlineStr">
+        <is>
+          <t>NUH notification application 2 password</t>
+        </is>
+      </c>
+      <c r="B70" s="7" t="n"/>
+      <c r="C70" s="7" t="n"/>
+      <c r="D70" s="7" t="n"/>
+      <c r="E70" s="7" t="n"/>
+      <c r="F70" s="7" t="n"/>
+      <c r="G70" s="7" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="15">
@@ -13934,10 +14145,10 @@
     <mergeCell ref="A42:G42"/>
     <mergeCell ref="A46:G46"/>
     <mergeCell ref="A51:G51"/>
-    <mergeCell ref="A54:G54"/>
-    <mergeCell ref="A59:G59"/>
-    <mergeCell ref="A62:G62"/>
-    <mergeCell ref="A65:G65"/>
+    <mergeCell ref="A55:G55"/>
+    <mergeCell ref="A60:G60"/>
+    <mergeCell ref="A63:G63"/>
+    <mergeCell ref="A66:G66"/>
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <legacyDrawing r:id="anysvml"/>

</xml_diff>